<commit_message>
📊 Horarios actualizados Línea 141 - 719
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 00:05:23</t>
+          <t>Última actualización: 01:12:01</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 2</t>
+          <t>Total filas: 3</t>
         </is>
       </c>
     </row>
@@ -487,7 +487,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>00:05:23</t>
+          <t>01:12:01</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -501,7 +501,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -512,7 +512,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>00:05:23</t>
+          <t>01:12:01</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -526,9 +526,34 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>113</v>
+        <v>46</v>
       </c>
       <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>01:12:01</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>02:58</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>106</v>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -545,7 +570,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -563,14 +588,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 00:05:23</t>
+          <t>Última actualización: 01:12:01</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 1</t>
+          <t>Total filas: 2</t>
         </is>
       </c>
     </row>
@@ -604,7 +629,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>00:05:23</t>
+          <t>01:12:01</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -618,9 +643,34 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>01:12:01</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>02:58</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>106</v>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -655,7 +705,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 00:05:23</t>
+          <t>Última actualización: 01:12:01</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 720
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:12:01</t>
+          <t>Última actualización: 01:56:31</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 3</t>
+          <t>Total filas: 5</t>
         </is>
       </c>
     </row>
@@ -512,7 +512,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>01:12:01</t>
+          <t>01:56:31</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -554,6 +554,56 @@
         <v>106</v>
       </c>
       <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>01:56:31</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>02:59</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>63</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>01:56:31</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>03:48</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>112</v>
+      </c>
+      <c r="E10" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -570,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -588,14 +638,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:12:01</t>
+          <t>Última actualización: 01:56:31</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 2</t>
+          <t>Total filas: 3</t>
         </is>
       </c>
     </row>
@@ -671,6 +721,31 @@
         <v>106</v>
       </c>
       <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>01:56:31</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>02:59</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>63</v>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -705,7 +780,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:12:01</t>
+          <t>Última actualización: 01:56:31</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 721
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:56:31</t>
+          <t>Última actualización: 02:24:16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 5</t>
+          <t>Total filas: 8</t>
         </is>
       </c>
     </row>
@@ -604,6 +604,81 @@
         <v>112</v>
       </c>
       <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>02:24:16</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>03:53</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>89</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>02:24:16</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>03:58</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>94</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>02:24:16</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>04:01</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>97</v>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -620,7 +695,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -638,14 +713,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:56:31</t>
+          <t>Última actualización: 02:24:16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 3</t>
+          <t>Total filas: 4</t>
         </is>
       </c>
     </row>
@@ -746,6 +821,31 @@
         <v>63</v>
       </c>
       <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>02:24:16</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>03:58</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>94</v>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -780,7 +880,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:56:31</t>
+          <t>Última actualización: 02:24:16</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 722
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:24:16</t>
+          <t>Última actualización: 02:49:45</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 8</t>
+          <t>Total filas: 10</t>
         </is>
       </c>
     </row>
@@ -537,12 +537,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>01:12:01</t>
+          <t>02:49:45</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>02:49</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -551,7 +551,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>106</v>
+        <v>0</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -562,12 +562,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>01:56:31</t>
+          <t>01:12:01</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>02:59</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -576,7 +576,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -592,16 +592,16 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>02:59</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -612,12 +612,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>02:24:16</t>
+          <t>02:49:45</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>03:53</t>
+          <t>03:48</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -626,7 +626,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -642,16 +642,16 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>03:58</t>
+          <t>03:53</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -667,18 +667,68 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>03:58</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>94</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>02:49:45</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>04:01</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>81_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D13" t="n">
-        <v>97</v>
-      </c>
-      <c r="E13" t="inlineStr">
+      <c r="D14" t="n">
+        <v>72</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>02:49:45</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>04:35</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>106</v>
+      </c>
+      <c r="E15" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -695,7 +745,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -713,14 +763,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:24:16</t>
+          <t>Última actualización: 02:49:45</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 4</t>
+          <t>Total filas: 6</t>
         </is>
       </c>
     </row>
@@ -779,12 +829,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>01:12:01</t>
+          <t>02:49:45</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>02:49</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -793,7 +843,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>106</v>
+        <v>0</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -804,12 +854,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>01:56:31</t>
+          <t>01:12:01</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>02:59</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -818,7 +868,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -829,23 +879,73 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>01:56:31</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>02:59</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>63</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>02:24:16</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>03:58</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>215_ALUAR</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
         <v>94</v>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>02:49:45</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>04:35</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>106</v>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -880,7 +980,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:24:16</t>
+          <t>Última actualización: 02:49:45</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 723
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:49:45</t>
+          <t>Última actualización: 03:00:18</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 10</t>
+          <t>Total filas: 12</t>
         </is>
       </c>
     </row>
@@ -612,7 +612,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>02:49:45</t>
+          <t>03:00:18</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -626,7 +626,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -687,7 +687,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>02:49:45</t>
+          <t>03:00:18</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -701,7 +701,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -729,6 +729,56 @@
         <v>106</v>
       </c>
       <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>03:00:18</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>04:44</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>104</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>03:00:18</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>04:53</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>113</v>
+      </c>
+      <c r="E17" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -745,7 +795,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -763,14 +813,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:49:45</t>
+          <t>Última actualización: 03:00:18</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 6</t>
+          <t>Total filas: 7</t>
         </is>
       </c>
     </row>
@@ -946,6 +996,31 @@
         <v>106</v>
       </c>
       <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>03:00:18</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>04:44</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>104</v>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -980,7 +1055,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:49:45</t>
+          <t>Última actualización: 03:00:18</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 724
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:00:18</t>
+          <t>Última actualización: 03:42:43</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 12</t>
+          <t>Total filas: 18</t>
         </is>
       </c>
     </row>
@@ -612,12 +612,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>03:00:18</t>
+          <t>03:42:43</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>03:45</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -626,7 +626,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -637,12 +637,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>02:24:16</t>
+          <t>03:00:18</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>03:53</t>
+          <t>03:48</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -651,7 +651,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -667,16 +667,16 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>03:58</t>
+          <t>03:53</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -687,21 +687,21 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>03:00:18</t>
+          <t>02:24:16</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>03:58</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>61</v>
+        <v>94</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -712,21 +712,21 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>02:49:45</t>
+          <t>03:42:43</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>04:35</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>106</v>
+        <v>19</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -737,12 +737,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>03:00:18</t>
+          <t>02:49:45</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>04:44</t>
+          <t>04:35</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -751,7 +751,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -767,18 +767,168 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>04:44</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>104</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>03:42:43</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>04:45</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>63</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>03:42:43</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>04:53</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D17" t="n">
+      <c r="D19" t="n">
+        <v>71</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>03:42:43</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>05:16</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>94</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>03:42:43</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>05:22</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>100</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>03:42:43</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>05:34</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>112</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>03:42:43</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
         <v>113</v>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -795,7 +945,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -813,14 +963,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:00:18</t>
+          <t>Última actualización: 03:42:43</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 7</t>
+          <t>Total filas: 9</t>
         </is>
       </c>
     </row>
@@ -1021,6 +1171,56 @@
         <v>104</v>
       </c>
       <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>03:42:43</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>04:45</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>63</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>03:42:43</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>05:34</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>112</v>
+      </c>
+      <c r="E14" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1055,7 +1255,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:00:18</t>
+          <t>Última actualización: 03:42:43</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 725
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:42:43</t>
+          <t>Última actualización: 04:17:03</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 18</t>
+          <t>Total filas: 25</t>
         </is>
       </c>
     </row>
@@ -737,12 +737,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>02:49:45</t>
+          <t>04:17:03</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>04:35</t>
+          <t>04:31</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -751,7 +751,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>106</v>
+        <v>14</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -762,12 +762,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>03:00:18</t>
+          <t>02:49:45</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>04:44</t>
+          <t>04:35</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -776,7 +776,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -787,21 +787,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>03:00:18</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>04:45</t>
+          <t>04:44</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>63</v>
+        <v>104</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -817,16 +817,16 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>04:45</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -837,21 +837,21 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>04:17:03</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>04:53</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>94</v>
+        <v>36</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -862,21 +862,21 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>04:17:03</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>100</v>
+        <v>59</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -887,21 +887,21 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>04:17:03</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>05:34</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>112</v>
+        <v>65</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -917,18 +917,193 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>05:34</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>112</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>03:42:43</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
           <t>05:35</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D23" t="n">
+      <c r="D24" t="n">
         <v>113</v>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>04:17:03</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>78</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>04:17:03</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>05:36</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>79</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>04:17:03</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>05:46</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>89</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>04:17:03</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>06:05</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>108</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>04:17:03</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>06:12</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>115</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>04:17:03</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>06:14</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>225_HARAS DEL SUR</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>117</v>
+      </c>
+      <c r="E30" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -945,7 +1120,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -963,14 +1138,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:42:43</t>
+          <t>Última actualización: 04:17:03</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 9</t>
+          <t>Total filas: 12</t>
         </is>
       </c>
     </row>
@@ -1129,12 +1304,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>02:49:45</t>
+          <t>04:17:03</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>04:35</t>
+          <t>04:31</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1143,7 +1318,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>106</v>
+        <v>14</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1154,12 +1329,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>03:00:18</t>
+          <t>02:49:45</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>04:44</t>
+          <t>04:35</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1168,7 +1343,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1179,21 +1354,21 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>03:00:18</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>04:45</t>
+          <t>04:44</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>63</v>
+        <v>104</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1209,18 +1384,93 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>04:45</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>63</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>03:42:43</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>05:34</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D14" t="n">
+      <c r="D15" t="n">
         <v>112</v>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>04:17:03</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>78</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>04:17:03</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>06:12</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>115</v>
+      </c>
+      <c r="E17" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1237,7 +1487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1255,14 +1505,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:42:43</t>
+          <t>Última actualización: 04:17:03</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 1</t>
+          <t>Total filas: 2</t>
         </is>
       </c>
     </row>
@@ -1313,6 +1563,31 @@
         <v>3</v>
       </c>
       <c r="E6" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>04:17:03</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>05:44</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>87</v>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 726
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:17:03</t>
+          <t>Última actualización: 04:44:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 25</t>
+          <t>Total filas: 32</t>
         </is>
       </c>
     </row>
@@ -812,7 +812,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>04:44:38</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -826,7 +826,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -837,7 +837,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>04:44:38</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -851,7 +851,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -862,7 +862,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>04:44:38</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -876,7 +876,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -887,7 +887,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>04:44:38</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -901,7 +901,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -912,7 +912,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>04:44:38</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -926,7 +926,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -937,7 +937,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>04:17:03</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -947,11 +947,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -962,7 +962,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>03:42:43</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -972,11 +972,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1012,7 +1012,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>04:44:38</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1037,21 +1037,21 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>04:44:38</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>06:05</t>
+          <t>05:54</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1062,21 +1062,21 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>04:44:38</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>06:12</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1092,18 +1092,193 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
+          <t>06:05</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>108</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>04:44:38</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>06:11</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>87</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>04:17:03</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>06:12</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>115</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>04:44:38</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
           <t>06:14</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t>225_HARAS DEL SUR</t>
         </is>
       </c>
-      <c r="D30" t="n">
-        <v>117</v>
-      </c>
-      <c r="E30" t="inlineStr">
+      <c r="D33" t="n">
+        <v>90</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>04:44:38</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>06:21</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>97</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>04:44:38</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>06:27</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>103</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>04:44:38</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>06:29</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>86_EST CHICA-ESC AGRARIA</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>105</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>04:44:38</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>06:31</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>107</v>
+      </c>
+      <c r="E37" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1120,7 +1295,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1138,14 +1313,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:17:03</t>
+          <t>Última actualización: 04:44:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 12</t>
+          <t>Total filas: 13</t>
         </is>
       </c>
     </row>
@@ -1379,7 +1554,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>04:44:38</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1393,7 +1568,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1404,7 +1579,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>04:44:38</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1418,7 +1593,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -1454,23 +1629,48 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>04:44:38</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>06:11</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>87</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
           <t>04:17:03</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B18" t="inlineStr">
         <is>
           <t>06:12</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D17" t="n">
+      <c r="D18" t="n">
         <v>115</v>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1487,7 +1687,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1505,14 +1705,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:17:03</t>
+          <t>Última actualización: 04:44:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 2</t>
+          <t>Total filas: 5</t>
         </is>
       </c>
     </row>
@@ -1571,25 +1771,100 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>04:44:38</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>05:43</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>59</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>04:17:03</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>05:44</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="D8" t="n">
         <v>87</v>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>04:44:38</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>06:08</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>84</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>04:44:38</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>06:32</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>108</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 727
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:44:38</t>
+          <t>Última actualización: 04:57:25</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 32</t>
+          <t>Total filas: 34</t>
         </is>
       </c>
     </row>
@@ -862,7 +862,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>04:44:38</t>
+          <t>04:57:25</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -876,7 +876,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -887,7 +887,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>04:44:38</t>
+          <t>04:57:25</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -901,7 +901,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -912,7 +912,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>04:44:38</t>
+          <t>04:57:25</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -926,7 +926,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1012,7 +1012,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>04:44:38</t>
+          <t>04:57:25</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1037,7 +1037,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>04:44:38</t>
+          <t>04:57:25</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1051,7 +1051,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1062,7 +1062,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>04:44:38</t>
+          <t>04:57:25</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1076,7 +1076,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1112,7 +1112,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>04:44:38</t>
+          <t>04:57:25</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1126,7 +1126,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1162,7 +1162,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>04:44:38</t>
+          <t>04:57:25</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1176,7 +1176,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1187,7 +1187,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>04:44:38</t>
+          <t>04:57:25</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1201,7 +1201,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1212,7 +1212,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>04:44:38</t>
+          <t>04:57:25</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1226,7 +1226,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>04:44:38</t>
+          <t>04:57:25</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1251,7 +1251,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1262,7 +1262,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>04:44:38</t>
+          <t>04:57:25</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1276,9 +1276,59 @@
         </is>
       </c>
       <c r="D37" t="n">
+        <v>94</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>04:57:25</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>06:44</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
         <v>107</v>
       </c>
-      <c r="E37" t="inlineStr">
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>04:57:25</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>06:46</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>109</v>
+      </c>
+      <c r="E39" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1295,7 +1345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1313,14 +1363,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:44:38</t>
+          <t>Última actualización: 04:57:25</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 13</t>
+          <t>Total filas: 14</t>
         </is>
       </c>
     </row>
@@ -1579,7 +1629,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04:44:38</t>
+          <t>04:57:25</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1593,7 +1643,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -1629,7 +1679,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>04:44:38</t>
+          <t>04:57:25</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1643,7 +1693,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1671,6 +1721,31 @@
         <v>115</v>
       </c>
       <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>04:57:25</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>06:46</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>109</v>
+      </c>
+      <c r="E19" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1687,7 +1762,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1705,14 +1780,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:44:38</t>
+          <t>Última actualización: 04:57:25</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 5</t>
+          <t>Total filas: 7</t>
         </is>
       </c>
     </row>
@@ -1796,7 +1871,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>04:57:25</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1810,7 +1885,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>87</v>
+        <v>47</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1846,23 +1921,73 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>04:57:25</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>06:09</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>72</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>04:44:38</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>06:32</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="D11" t="n">
         <v>108</v>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>04:57:25</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>06:33</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>96</v>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 728
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:57:25</t>
+          <t>Última actualización: 05:27:50</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 34</t>
+          <t>Total filas: 42</t>
         </is>
       </c>
     </row>
@@ -912,7 +912,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>04:57:25</t>
+          <t>05:27:50</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -926,7 +926,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -937,7 +937,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>03:42:43</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -947,11 +947,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -962,7 +962,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>04:17:03</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -972,11 +972,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1012,7 +1012,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>04:57:25</t>
+          <t>05:27:50</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1037,7 +1037,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>04:57:25</t>
+          <t>05:27:50</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1051,7 +1051,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1062,7 +1062,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>04:57:25</t>
+          <t>05:27:50</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1076,7 +1076,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1112,7 +1112,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>04:57:25</t>
+          <t>05:27:50</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1126,7 +1126,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1162,7 +1162,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>04:57:25</t>
+          <t>05:27:50</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1176,7 +1176,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1187,7 +1187,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>04:57:25</t>
+          <t>05:27:50</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1201,7 +1201,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1212,7 +1212,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>04:57:25</t>
+          <t>05:27:50</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1226,7 +1226,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>04:57:25</t>
+          <t>05:27:50</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1251,7 +1251,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1262,7 +1262,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>04:57:25</t>
+          <t>05:27:50</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1276,7 +1276,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1287,7 +1287,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>04:57:25</t>
+          <t>05:27:50</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1301,7 +1301,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1312,7 +1312,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>04:57:25</t>
+          <t>05:27:50</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1326,9 +1326,209 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="E39" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>05:27:50</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>06:59</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>92</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>05:27:50</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>07:04</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>97</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>05:27:50</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>07:05</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>98</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>05:27:50</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>07:06</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>99</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>05:27:50</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>07:11</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>104</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>05:27:50</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>07:15</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>108</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>05:27:50</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>07:21</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>114</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>05:27:50</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>07:23</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>116</v>
+      </c>
+      <c r="E47" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1345,7 +1545,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1363,14 +1563,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:57:25</t>
+          <t>Última actualización: 05:27:50</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 14</t>
+          <t>Total filas: 15</t>
         </is>
       </c>
     </row>
@@ -1629,7 +1829,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04:57:25</t>
+          <t>05:27:50</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1643,7 +1843,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -1679,7 +1879,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>04:57:25</t>
+          <t>05:27:50</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1693,7 +1893,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1729,7 +1929,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>04:57:25</t>
+          <t>05:27:50</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1743,9 +1943,34 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>05:27:50</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>07:11</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>104</v>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1762,7 +1987,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1780,14 +2005,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:57:25</t>
+          <t>Última actualización: 05:27:50</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 7</t>
+          <t>Total filas: 8</t>
         </is>
       </c>
     </row>
@@ -1846,7 +2071,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>04:44:38</t>
+          <t>05:27:50</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1860,7 +2085,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -1896,7 +2121,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>04:44:38</t>
+          <t>05:27:50</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1910,7 +2135,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -1946,7 +2171,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>04:44:38</t>
+          <t>05:27:50</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1960,7 +2185,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>108</v>
+        <v>65</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1990,6 +2215,31 @@
       <c r="E12" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>05:27:50</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>06:59</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>92</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 729
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:27:50</t>
+          <t>Última actualización: 05:55:46</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 42</t>
+          <t>Total filas: 50</t>
         </is>
       </c>
     </row>
@@ -937,7 +937,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>04:17:03</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -947,11 +947,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -962,7 +962,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>03:42:43</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -972,11 +972,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1062,21 +1062,21 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>05:27:50</t>
+          <t>05:55:46</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>06:04</t>
+          <t>05:55</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1087,12 +1087,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>05:27:50</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>06:05</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1101,7 +1101,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>108</v>
+        <v>37</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1112,21 +1112,21 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>05:27:50</t>
+          <t>04:17:03</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>06:05</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1137,12 +1137,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>05:55:46</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>06:12</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1151,7 +1151,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>115</v>
+        <v>16</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1162,21 +1162,21 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>05:27:50</t>
+          <t>04:17:03</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>06:14</t>
+          <t>06:12</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>47</v>
+        <v>115</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1187,21 +1187,21 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>05:27:50</t>
+          <t>05:55:46</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>06:21</t>
+          <t>06:14</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1212,21 +1212,21 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>05:27:50</t>
+          <t>05:55:46</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>06:27</t>
+          <t>06:21</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1237,21 +1237,21 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>05:27:50</t>
+          <t>05:55:46</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>06:29</t>
+          <t>06:27</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1262,21 +1262,21 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>05:27:50</t>
+          <t>05:55:46</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>06:29</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1287,21 +1287,21 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>05:27:50</t>
+          <t>05:55:46</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>06:44</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1312,21 +1312,21 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>05:27:50</t>
+          <t>05:55:46</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>06:46</t>
+          <t>06:44</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1337,21 +1337,21 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>05:27:50</t>
+          <t>05:55:46</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>06:59</t>
+          <t>06:46</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1362,21 +1362,21 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>05:27:50</t>
+          <t>05:55:46</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>07:04</t>
+          <t>06:59</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1387,21 +1387,21 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>05:27:50</t>
+          <t>05:55:46</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>07:05</t>
+          <t>07:04</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1412,21 +1412,21 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>05:27:50</t>
+          <t>05:55:46</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>07:06</t>
+          <t>07:05</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1442,16 +1442,16 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>07:11</t>
+          <t>07:06</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1462,21 +1462,21 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>05:27:50</t>
+          <t>05:55:46</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1487,21 +1487,21 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>05:27:50</t>
+          <t>05:55:46</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>07:11</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1512,23 +1512,223 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>05:27:50</t>
+          <t>05:55:46</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
+          <t>07:15</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>80</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>05:55:46</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>07:21</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>86</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>05:55:46</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
           <t>07:23</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="C49" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D47" t="n">
+      <c r="D49" t="n">
+        <v>88</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>05:55:46</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>07:31</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>96</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>05:55:46</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>07:31</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>96</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>05:55:46</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>07:32</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>97</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>05:55:46</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>07:36</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>101</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>05:55:46</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>07:47</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>112</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>05:55:46</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
         <v>116</v>
       </c>
-      <c r="E47" t="inlineStr">
+      <c r="E55" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1545,7 +1745,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1563,14 +1763,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:27:50</t>
+          <t>Última actualización: 05:55:46</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 15</t>
+          <t>Total filas: 16</t>
         </is>
       </c>
     </row>
@@ -1879,7 +2079,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:27:50</t>
+          <t>05:55:46</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1893,7 +2093,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1929,7 +2129,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>05:27:50</t>
+          <t>05:55:46</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1943,7 +2143,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1954,7 +2154,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>05:27:50</t>
+          <t>05:55:46</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1968,9 +2168,34 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>05:55:46</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>116</v>
+      </c>
+      <c r="E21" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1987,7 +2212,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2005,14 +2230,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:27:50</t>
+          <t>Última actualización: 05:55:46</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 8</t>
+          <t>Total filas: 9</t>
         </is>
       </c>
     </row>
@@ -2121,7 +2346,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>05:27:50</t>
+          <t>05:55:46</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2135,7 +2360,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -2171,7 +2396,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>05:27:50</t>
+          <t>05:55:46</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -2185,7 +2410,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -2221,7 +2446,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>05:27:50</t>
+          <t>05:55:46</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -2235,9 +2460,34 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="E13" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>05:55:46</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>07:35</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>100</v>
+      </c>
+      <c r="E14" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 730
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:55:46</t>
+          <t>Última actualización: 06:25:30</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 50</t>
+          <t>Total filas: 56</t>
         </is>
       </c>
     </row>
@@ -937,7 +937,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>03:42:43</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -947,11 +947,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -962,7 +962,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>04:17:03</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -972,11 +972,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>05:55:46</t>
+          <t>06:25:30</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1251,7 +1251,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1262,7 +1262,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>05:55:46</t>
+          <t>06:25:30</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1276,7 +1276,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1287,7 +1287,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>05:55:46</t>
+          <t>06:25:30</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1301,7 +1301,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1312,7 +1312,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>05:55:46</t>
+          <t>06:25:30</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1326,7 +1326,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1337,7 +1337,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>05:55:46</t>
+          <t>06:25:30</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1351,7 +1351,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1362,7 +1362,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>05:55:46</t>
+          <t>06:25:30</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1376,7 +1376,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1387,21 +1387,21 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>05:55:46</t>
+          <t>06:25:30</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>07:04</t>
+          <t>07:01</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1412,21 +1412,21 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>05:55:46</t>
+          <t>06:25:30</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>07:05</t>
+          <t>07:04</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1437,21 +1437,21 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>05:27:50</t>
+          <t>06:25:30</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>07:06</t>
+          <t>07:05</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1462,12 +1462,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>05:55:46</t>
+          <t>05:27:50</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>07:07</t>
+          <t>07:06</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1476,7 +1476,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1487,21 +1487,21 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>05:55:46</t>
+          <t>06:25:30</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>07:11</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1512,21 +1512,21 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>05:55:46</t>
+          <t>06:25:30</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>07:11</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1537,21 +1537,21 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>05:55:46</t>
+          <t>06:25:30</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1562,21 +1562,21 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>05:55:46</t>
+          <t>06:25:30</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>07:23</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1587,21 +1587,21 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>05:55:46</t>
+          <t>06:25:30</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>07:31</t>
+          <t>07:23</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1637,21 +1637,21 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>05:55:46</t>
+          <t>06:25:30</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>07:32</t>
+          <t>07:31</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1662,21 +1662,21 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>05:55:46</t>
+          <t>06:25:30</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>07:36</t>
+          <t>07:32</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>101</v>
+        <v>67</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1687,21 +1687,21 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>05:55:46</t>
+          <t>06:25:30</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>07:47</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1712,23 +1712,173 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>05:55:46</t>
+          <t>06:25:30</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
+          <t>07:39</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>74</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>06:25:30</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>07:47</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>82</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>06:25:30</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
           <t>07:51</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
+      <c r="C57" t="inlineStr">
         <is>
           <t>215D_EL PATO</t>
         </is>
       </c>
-      <c r="D55" t="n">
+      <c r="D57" t="n">
+        <v>86</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>06:25:30</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>08:12</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>107</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>06:25:30</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>08:21</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
         <v>116</v>
       </c>
-      <c r="E55" t="inlineStr">
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>06:25:30</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>08:22</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>117</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>06:25:30</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>118</v>
+      </c>
+      <c r="E61" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1745,7 +1895,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1763,14 +1913,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:55:46</t>
+          <t>Última actualización: 06:25:30</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 16</t>
+          <t>Total filas: 17</t>
         </is>
       </c>
     </row>
@@ -2129,7 +2279,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>05:55:46</t>
+          <t>06:25:30</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2143,7 +2293,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -2154,7 +2304,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>05:55:46</t>
+          <t>06:25:30</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2168,7 +2318,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -2179,7 +2329,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>05:55:46</t>
+          <t>06:25:30</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2193,9 +2343,34 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>06:25:30</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>118</v>
+      </c>
+      <c r="E22" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2212,7 +2387,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2230,14 +2405,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:55:46</t>
+          <t>Última actualización: 06:25:30</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 9</t>
+          <t>Total filas: 12</t>
         </is>
       </c>
     </row>
@@ -2421,7 +2596,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>04:57:25</t>
+          <t>06:25:30</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -2435,7 +2610,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>96</v>
+        <v>8</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -2471,25 +2646,100 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>06:25:30</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>35</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>05:55:46</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>07:35</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D14" t="n">
+      <c r="D15" t="n">
         <v>100</v>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>06:25:30</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>07:40</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>75</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>06:25:30</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>08:07</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>102</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 731
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:25:30</t>
+          <t>Última actualización: 06:52:31</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 56</t>
+          <t>Total filas: 61</t>
         </is>
       </c>
     </row>
@@ -937,7 +937,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>04:17:03</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -947,11 +947,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -962,7 +962,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>03:42:43</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -972,11 +972,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1362,7 +1362,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>06:25:30</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1376,7 +1376,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1387,7 +1387,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>06:25:30</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1401,7 +1401,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1437,7 +1437,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>06:25:30</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1447,11 +1447,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1462,21 +1462,21 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>05:27:50</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>07:06</t>
+          <t>07:05</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>99</v>
+        <v>13</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1487,12 +1487,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>06:25:30</t>
+          <t>05:27:50</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>07:07</t>
+          <t>07:06</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1501,7 +1501,7 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1512,21 +1512,21 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>06:25:30</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>07:11</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1537,21 +1537,21 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>06:25:30</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>07:11</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1562,21 +1562,21 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>06:25:30</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1587,21 +1587,21 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>06:25:30</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>07:23</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1612,21 +1612,21 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>05:55:46</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>07:31</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1637,21 +1637,21 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>06:25:30</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>07:31</t>
+          <t>07:23</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1662,21 +1662,21 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>06:25:30</t>
+          <t>05:55:46</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>07:32</t>
+          <t>07:31</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1687,21 +1687,21 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>06:25:30</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>07:36</t>
+          <t>07:31</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1712,21 +1712,21 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>06:25:30</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>07:39</t>
+          <t>07:32</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1737,21 +1737,21 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>06:25:30</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>07:47</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1762,21 +1762,21 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>06:25:30</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>07:51</t>
+          <t>07:39</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>86</v>
+        <v>47</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1787,21 +1787,21 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>06:25:30</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>08:12</t>
+          <t>07:47</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>107</v>
+        <v>55</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1812,21 +1812,21 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>06:25:30</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>08:21</t>
+          <t>07:51</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>116</v>
+        <v>59</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1837,21 +1837,21 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>06:25:30</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>08:22</t>
+          <t>08:12</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>117</v>
+        <v>80</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1862,23 +1862,148 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>06:25:30</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
+          <t>08:21</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>89</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>06:52:31</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>08:22</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>90</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>06:52:31</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
           <t>08:23</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
+      <c r="C63" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D61" t="n">
-        <v>118</v>
-      </c>
-      <c r="E61" t="inlineStr">
+      <c r="D63" t="n">
+        <v>91</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>06:52:31</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>08:27</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>95</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>06:52:31</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>08:35</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>103</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>06:52:31</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>08:42</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>110</v>
+      </c>
+      <c r="E66" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1913,7 +2038,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:25:30</t>
+          <t>Última actualización: 06:52:31</t>
         </is>
       </c>
     </row>
@@ -2304,7 +2429,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>06:25:30</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2318,7 +2443,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -2329,7 +2454,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>06:25:30</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2343,7 +2468,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -2354,7 +2479,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>06:25:30</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2368,7 +2493,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -2387,7 +2512,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2405,14 +2530,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:25:30</t>
+          <t>Última actualización: 06:52:31</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 12</t>
+          <t>Total filas: 14</t>
         </is>
       </c>
     </row>
@@ -2646,7 +2771,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>06:25:30</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -2660,7 +2785,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -2721,25 +2846,75 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>06:25:30</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>07:41</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>49</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>06:52:31</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>08:07</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D17" t="n">
-        <v>102</v>
-      </c>
-      <c r="E17" t="inlineStr">
+      <c r="D18" t="n">
+        <v>75</v>
+      </c>
+      <c r="E18" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>06:52:31</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>08:30</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>98</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 732
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:52:31</t>
+          <t>Última actualización: 07:17:57</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 61</t>
+          <t>Total filas: 79</t>
         </is>
       </c>
     </row>
@@ -1612,12 +1612,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>06:52:31</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>07:20</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1626,7 +1626,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1642,16 +1642,16 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>07:23</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1662,21 +1662,21 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>05:55:46</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>07:31</t>
+          <t>07:22</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>96</v>
+        <v>5</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1692,16 +1692,16 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>07:31</t>
+          <t>07:23</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1712,12 +1712,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>06:52:31</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>07:32</t>
+          <t>07:31</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1726,7 +1726,7 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1737,21 +1737,21 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>06:52:31</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>07:36</t>
+          <t>07:31</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1762,21 +1762,21 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>06:52:31</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>07:39</t>
+          <t>07:31</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1792,16 +1792,16 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>07:47</t>
+          <t>07:32</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1812,21 +1812,21 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>06:52:31</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>07:51</t>
+          <t>07:35</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1837,21 +1837,21 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>06:52:31</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>08:12</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1862,21 +1862,21 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>06:52:31</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>08:21</t>
+          <t>07:38</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1892,16 +1892,16 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>08:22</t>
+          <t>07:39</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1912,21 +1912,21 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>06:52:31</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>08:23</t>
+          <t>07:46</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>91</v>
+        <v>29</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -1937,21 +1937,21 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>06:52:31</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>08:27</t>
+          <t>07:47</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>95</v>
+        <v>30</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1962,21 +1962,21 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>06:52:31</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>08:35</t>
+          <t>07:51</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>103</v>
+        <v>34</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1987,23 +1987,473 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
+          <t>07:17:57</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>07:59</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>42</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>07:17:57</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>08:03</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>46</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>07:17:57</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>08:11</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>54</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
           <t>06:52:31</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr">
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>08:12</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>80</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>07:17:57</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>08:20</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>63</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>06:52:31</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>08:21</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>89</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>07:17:57</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>08:22</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>65</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>07:17:57</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>08:22</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>65</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>06:52:31</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>91</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>07:17:57</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>08:26</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>69</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>06:52:31</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>08:27</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>95</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>06:52:31</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>08:35</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>103</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>07:17:57</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>08:41</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>84</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>06:52:31</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
         <is>
           <t>08:42</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr">
+      <c r="C79" t="inlineStr">
         <is>
           <t>81_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D66" t="n">
+      <c r="D79" t="n">
         <v>110</v>
       </c>
-      <c r="E66" t="inlineStr">
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>07:17:57</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>08:43</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>86</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>07:17:57</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>08:53</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>96</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>07:17:57</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>09:01</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>104</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>07:17:57</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>09:10</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>113</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>07:17:57</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>09:16</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>119</v>
+      </c>
+      <c r="E84" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2020,7 +2470,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2038,14 +2488,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:52:31</t>
+          <t>Última actualización: 07:17:57</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 17</t>
+          <t>Total filas: 19</t>
         </is>
       </c>
     </row>
@@ -2454,7 +2904,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>06:52:31</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2468,7 +2918,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -2479,23 +2929,73 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>07:17:57</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>08:22</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>65</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>06:52:31</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B23" t="inlineStr">
         <is>
           <t>08:23</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D22" t="n">
+      <c r="D23" t="n">
         <v>91</v>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>07:17:57</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>09:01</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>104</v>
+      </c>
+      <c r="E24" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2512,7 +3012,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2530,14 +3030,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:52:31</t>
+          <t>Última actualización: 07:17:57</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 14</t>
+          <t>Total filas: 18</t>
         </is>
       </c>
     </row>
@@ -2871,25 +3371,25 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>06:52:31</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>08:07</t>
+          <t>07:48</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
@@ -2901,20 +3401,120 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>08:07</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>75</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>07:17:57</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>08:09</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>52</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>06:52:31</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>08:30</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D19" t="n">
+      <c r="D21" t="n">
         <v>98</v>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>07:17:57</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>08:34</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>77</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>07:17:57</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>09:08</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>111</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 733
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:17:57</t>
+          <t>Última actualización: 07:50:23</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 79</t>
+          <t>Total filas: 95</t>
         </is>
       </c>
     </row>
@@ -1722,7 +1722,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1747,7 +1747,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1772,7 +1772,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -1962,7 +1962,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1976,7 +1976,7 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1987,7 +1987,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -2001,7 +2001,7 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2037,21 +2037,21 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>08:11</t>
+          <t>08:07</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2062,21 +2062,21 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>06:52:31</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>08:12</t>
+          <t>08:10</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2092,16 +2092,16 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>08:20</t>
+          <t>08:11</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2112,21 +2112,21 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>06:52:31</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>08:21</t>
+          <t>08:12</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>89</v>
+        <v>22</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2137,21 +2137,21 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>08:22</t>
+          <t>08:13</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2167,16 +2167,16 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>08:22</t>
+          <t>08:20</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2187,21 +2187,21 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>06:52:31</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>08:23</t>
+          <t>08:21</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>91</v>
+        <v>31</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2212,21 +2212,21 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>08:26</t>
+          <t>08:22</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2237,21 +2237,21 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>06:52:31</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>08:27</t>
+          <t>08:22</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2262,21 +2262,21 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>06:52:31</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>08:35</t>
+          <t>08:23</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2292,16 +2292,16 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>08:41</t>
+          <t>08:26</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2312,21 +2312,21 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>06:52:31</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>08:42</t>
+          <t>08:27</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>110</v>
+        <v>37</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2337,21 +2337,21 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>08:43</t>
+          <t>08:34</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2362,21 +2362,21 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>08:35</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2392,16 +2392,16 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>09:01</t>
+          <t>08:41</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2412,21 +2412,21 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>09:10</t>
+          <t>08:42</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>113</v>
+        <v>52</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2437,23 +2437,423 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
+          <t>07:50:23</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>08:43</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>53</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
           <t>07:17:57</t>
         </is>
       </c>
-      <c r="B84" t="inlineStr">
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>08:53</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>96</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>07:50:23</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>08:53</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>63</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>07:50:23</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>08:54</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>64</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>07:50:23</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>09:01</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>71</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>07:50:23</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>09:03</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>73</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>07:50:23</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>09:10</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>80</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>07:17:57</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
         <is>
           <t>09:16</t>
         </is>
       </c>
-      <c r="C84" t="inlineStr">
+      <c r="C91" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="D84" t="n">
+      <c r="D91" t="n">
         <v>119</v>
       </c>
-      <c r="E84" t="inlineStr">
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>07:50:23</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>09:17</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>87</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>07:50:23</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>09:21</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>91</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>07:50:23</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>09:23</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>93</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>07:50:23</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>09:23</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>93</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>07:50:23</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>09:31</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>101</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>07:50:23</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>09:32</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>102</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>07:50:23</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>09:33</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>103</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>07:50:23</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>112</v>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>07:50:23</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>113</v>
+      </c>
+      <c r="E100" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2470,7 +2870,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2488,14 +2888,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:17:57</t>
+          <t>Última actualización: 07:50:23</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 19</t>
+          <t>Total filas: 20</t>
         </is>
       </c>
     </row>
@@ -2904,7 +3304,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2918,7 +3318,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -2954,7 +3354,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:52:31</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2968,7 +3368,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>91</v>
+        <v>33</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -2979,7 +3379,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2993,9 +3393,34 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>07:50:23</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>112</v>
+      </c>
+      <c r="E25" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3012,7 +3437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3030,14 +3455,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:17:57</t>
+          <t>Última actualización: 07:50:23</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 18</t>
+          <t>Total filas: 22</t>
         </is>
       </c>
     </row>
@@ -3396,37 +3821,37 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>06:52:31</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>08:07</t>
+          <t>07:53</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>08:09</t>
+          <t>08:07</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -3435,7 +3860,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -3446,73 +3871,173 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>06:52:31</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>08:30</t>
+          <t>08:09</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>08:34</t>
+          <t>08:14</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>77</v>
+        <v>24</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>06:52:31</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>08:30</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>98</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
           <t>07:17:57</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>08:34</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>77</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>07:50:23</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>08:35</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>45</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>07:17:57</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
         <is>
           <t>09:08</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>215D_LA PLATA</t>
         </is>
       </c>
-      <c r="D23" t="n">
+      <c r="D26" t="n">
         <v>111</v>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>07:50:23</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>09:09</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>79</v>
+      </c>
+      <c r="E27" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 734
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E100"/>
+  <dimension ref="A1:E108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:50:23</t>
+          <t>Última actualización: 08:16:28</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 95</t>
+          <t>Total filas: 103</t>
         </is>
       </c>
     </row>
@@ -2187,7 +2187,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2201,7 +2201,7 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2212,7 +2212,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2222,11 +2222,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2237,7 +2237,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2247,11 +2247,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2262,7 +2262,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2276,7 +2276,7 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2312,7 +2312,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2326,7 +2326,7 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2337,7 +2337,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2351,7 +2351,7 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2412,7 +2412,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2426,7 +2426,7 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2437,7 +2437,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2451,7 +2451,7 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2462,7 +2462,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2472,11 +2472,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2487,7 +2487,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2497,11 +2497,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2512,7 +2512,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2526,7 +2526,7 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2537,21 +2537,21 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>09:01</t>
+          <t>08:55</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2562,21 +2562,21 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>09:03</t>
+          <t>09:01</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2587,21 +2587,21 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>09:10</t>
+          <t>09:03</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2612,21 +2612,21 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>09:16</t>
+          <t>09:08</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>119</v>
+        <v>52</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -2637,21 +2637,21 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:10</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -2662,21 +2662,21 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>09:13</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2687,21 +2687,21 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>09:16</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -2717,16 +2717,16 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2737,21 +2737,21 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>09:31</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2762,21 +2762,21 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>09:32</t>
+          <t>09:22</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -2787,21 +2787,21 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>09:33</t>
+          <t>09:22</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2812,21 +2812,21 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>09:42</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>112</v>
+        <v>67</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2842,18 +2842,218 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
+          <t>09:23</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>93</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>08:16:28</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>09:29</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>73</v>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>07:50:23</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>09:31</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>101</v>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>08:16:28</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>09:32</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>76</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>08:16:28</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>09:33</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>77</v>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>08:16:28</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>86</v>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>08:16:28</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
           <t>09:43</t>
         </is>
       </c>
-      <c r="C100" t="inlineStr">
+      <c r="C106" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D100" t="n">
-        <v>113</v>
-      </c>
-      <c r="E100" t="inlineStr">
+      <c r="D106" t="n">
+        <v>87</v>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>08:16:28</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>10:10</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>114</v>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>08:16:28</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>10:12</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>116</v>
+      </c>
+      <c r="E108" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2888,7 +3088,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:50:23</t>
+          <t>Última actualización: 08:16:28</t>
         </is>
       </c>
     </row>
@@ -3354,7 +3554,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -3368,7 +3568,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -3379,7 +3579,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -3393,7 +3593,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -3404,7 +3604,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -3418,7 +3618,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -3437,7 +3637,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3455,14 +3655,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:50:23</t>
+          <t>Última actualización: 08:16:28</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 22</t>
+          <t>Total filas: 24</t>
         </is>
       </c>
     </row>
@@ -3921,37 +4121,37 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:52:31</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>08:30</t>
+          <t>08:22</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>98</v>
+        <v>6</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>06:52:31</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>08:34</t>
+          <t>08:30</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -3960,7 +4160,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -3971,12 +4171,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>08:35</t>
+          <t>08:34</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -3985,7 +4185,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -3996,50 +4196,100 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>09:08</t>
+          <t>08:35</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>215D_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>111</v>
+        <v>19</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>09:08</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>111</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>08:16:28</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
           <t>09:09</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C28" t="inlineStr">
         <is>
           <t>215D_LA PLATA</t>
         </is>
       </c>
-      <c r="D27" t="n">
-        <v>79</v>
-      </c>
-      <c r="E27" t="inlineStr">
+      <c r="D28" t="n">
+        <v>53</v>
+      </c>
+      <c r="E28" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>08:16:28</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>10:03</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>107</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 735
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E108"/>
+  <dimension ref="A1:E115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:16:28</t>
+          <t>Última actualización: 08:39:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 103</t>
+          <t>Total filas: 110</t>
         </is>
       </c>
     </row>
@@ -937,7 +937,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>03:42:43</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -947,11 +947,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -962,7 +962,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>04:17:03</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -972,11 +972,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1722,7 +1722,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1747,7 +1747,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1772,7 +1772,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -2412,7 +2412,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2426,7 +2426,7 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2437,7 +2437,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2451,7 +2451,7 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2462,7 +2462,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2472,11 +2472,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2487,7 +2487,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2497,11 +2497,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2512,7 +2512,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2526,7 +2526,7 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2537,7 +2537,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2551,7 +2551,7 @@
         </is>
       </c>
       <c r="D88" t="n">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2562,7 +2562,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2576,7 +2576,7 @@
         </is>
       </c>
       <c r="D89" t="n">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2587,7 +2587,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2601,7 +2601,7 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2612,12 +2612,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>09:08</t>
+          <t>09:04</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -2626,7 +2626,7 @@
         </is>
       </c>
       <c r="D91" t="n">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -2642,16 +2642,16 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>09:10</t>
+          <t>09:08</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -2662,21 +2662,21 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>09:13</t>
+          <t>09:10</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2692,16 +2692,16 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>09:16</t>
+          <t>09:13</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -2712,12 +2712,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:16</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2726,7 +2726,7 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2737,21 +2737,21 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2762,21 +2762,21 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>09:22</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -2787,7 +2787,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -2797,11 +2797,11 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2812,21 +2812,21 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>09:22</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2837,7 +2837,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2847,11 +2847,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>93</v>
+        <v>44</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2862,21 +2862,21 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>09:29</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2887,12 +2887,12 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>09:31</t>
+          <t>09:29</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -2901,7 +2901,7 @@
         </is>
       </c>
       <c r="D102" t="n">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2912,21 +2912,21 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>09:32</t>
+          <t>09:31</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2937,21 +2937,21 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>09:33</t>
+          <t>09:32</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -2962,21 +2962,21 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>09:42</t>
+          <t>09:33</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2987,21 +2987,21 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>09:34</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3012,21 +3012,21 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>09:39</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>114</v>
+        <v>60</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3037,23 +3037,198 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
+          <t>08:39:38</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>62</v>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>08:39:38</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>63</v>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
           <t>08:16:28</t>
         </is>
       </c>
-      <c r="B108" t="inlineStr">
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>86</v>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>08:39:38</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>64</v>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>08:39:38</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>10:10</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>91</v>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>08:39:38</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
         <is>
           <t>10:12</t>
         </is>
       </c>
-      <c r="C108" t="inlineStr">
+      <c r="C113" t="inlineStr">
         <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D108" t="n">
-        <v>116</v>
-      </c>
-      <c r="E108" t="inlineStr">
+      <c r="D113" t="n">
+        <v>93</v>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>08:39:38</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>10:21</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>102</v>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>08:39:38</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>10:26</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>107</v>
+      </c>
+      <c r="E115" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3070,7 +3245,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3088,14 +3263,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:16:28</t>
+          <t>Última actualización: 08:39:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 20</t>
+          <t>Total filas: 22</t>
         </is>
       </c>
     </row>
@@ -3579,7 +3754,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -3593,7 +3768,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -3604,23 +3779,73 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>08:39:38</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>62</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
           <t>08:16:28</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B26" t="inlineStr">
         <is>
           <t>09:42</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D25" t="n">
+      <c r="D26" t="n">
         <v>86</v>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>08:39:38</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>10:26</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>107</v>
+      </c>
+      <c r="E27" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3637,7 +3862,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3655,14 +3880,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:16:28</t>
+          <t>Última actualización: 08:39:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 24</t>
+          <t>Total filas: 25</t>
         </is>
       </c>
     </row>
@@ -4221,7 +4446,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -4235,7 +4460,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>111</v>
+        <v>29</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -4271,23 +4496,48 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>08:39:38</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>10:02</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>83</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
           <t>08:16:28</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B30" t="inlineStr">
         <is>
           <t>10:03</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
-      <c r="D29" t="n">
+      <c r="D30" t="n">
         <v>107</v>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 736
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E115"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:39:38</t>
+          <t>Última actualización: 08:52:26</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 110</t>
+          <t>Total filas: 116</t>
         </is>
       </c>
     </row>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1472,7 +1472,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1747,7 +1747,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1772,7 +1772,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -2212,7 +2212,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2222,11 +2222,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2237,7 +2237,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2247,11 +2247,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2462,7 +2462,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2472,11 +2472,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2487,7 +2487,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2497,11 +2497,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2512,7 +2512,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2526,7 +2526,7 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2537,21 +2537,21 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>08:55</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2562,21 +2562,21 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>09:01</t>
+          <t>08:55</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2587,21 +2587,21 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>09:03</t>
+          <t>09:01</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2612,21 +2612,21 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>09:04</t>
+          <t>09:03</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -2637,12 +2637,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>09:08</t>
+          <t>09:04</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2651,7 +2651,7 @@
         </is>
       </c>
       <c r="D92" t="n">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -2662,21 +2662,21 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>09:10</t>
+          <t>09:08</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2687,21 +2687,21 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>09:13</t>
+          <t>09:10</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -2712,21 +2712,21 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>09:16</t>
+          <t>09:13</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2737,12 +2737,12 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:16</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2751,7 +2751,7 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2762,21 +2762,21 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -2787,21 +2787,21 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>09:22</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2812,21 +2812,21 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>09:22</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2837,21 +2837,21 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>09:22</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2862,12 +2862,12 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>09:22</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -2876,7 +2876,7 @@
         </is>
       </c>
       <c r="D101" t="n">
-        <v>93</v>
+        <v>43</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2887,21 +2887,21 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>09:29</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2912,21 +2912,21 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>09:31</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>101</v>
+        <v>31</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2937,21 +2937,21 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:16:28</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>09:32</t>
+          <t>09:29</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -2962,21 +2962,21 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>09:33</t>
+          <t>09:31</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>54</v>
+        <v>101</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2987,21 +2987,21 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>09:34</t>
+          <t>09:32</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3012,21 +3012,21 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>09:39</t>
+          <t>09:33</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3037,21 +3037,21 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:34</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3067,16 +3067,16 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>09:42</t>
+          <t>09:39</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3087,12 +3087,12 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>09:42</t>
+          <t>09:41</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3101,7 +3101,7 @@
         </is>
       </c>
       <c r="D110" t="n">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3117,16 +3117,16 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>09:42</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3137,21 +3137,21 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>09:42</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>91</v>
+        <v>50</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,21 +3162,21 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>10:12</t>
+          <t>09:43</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>93</v>
+        <v>51</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3187,21 +3187,21 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>10:21</t>
+          <t>09:52</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>102</v>
+        <v>60</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3212,23 +3212,173 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
+          <t>08:52:26</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>09:53</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>61</v>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>08:52:26</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>10:10</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>78</v>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
           <t>08:39:38</t>
         </is>
       </c>
-      <c r="B115" t="inlineStr">
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>10:12</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>93</v>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>08:52:26</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>10:21</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>89</v>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>08:52:26</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
         <is>
           <t>10:26</t>
         </is>
       </c>
-      <c r="C115" t="inlineStr">
+      <c r="C119" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D115" t="n">
-        <v>107</v>
-      </c>
-      <c r="E115" t="inlineStr">
+      <c r="D119" t="n">
+        <v>94</v>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>08:52:26</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>10:42</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>110</v>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>08:52:26</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>10:43</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>111</v>
+      </c>
+      <c r="E121" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3263,7 +3413,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:39:38</t>
+          <t>Última actualización: 08:52:26</t>
         </is>
       </c>
     </row>
@@ -3754,7 +3904,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -3768,7 +3918,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -3804,7 +3954,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -3818,7 +3968,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -3829,7 +3979,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -3843,7 +3993,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -3880,7 +4030,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:39:38</t>
+          <t>Última actualización: 08:52:26</t>
         </is>
       </c>
     </row>
@@ -4471,7 +4621,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -4485,7 +4635,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -4521,7 +4671,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>08:16:28</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -4535,7 +4685,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>107</v>
+        <v>71</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 737
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:52:26</t>
+          <t>Última actualización: 09:28:24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 116</t>
+          <t>Total filas: 130</t>
         </is>
       </c>
     </row>
@@ -937,7 +937,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>04:17:03</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -947,11 +947,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -962,7 +962,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>03:42:43</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -972,11 +972,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1722,7 +1722,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1772,7 +1772,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -2462,7 +2462,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2472,11 +2472,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2487,7 +2487,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2497,11 +2497,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2522,7 +2522,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2547,7 +2547,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -2887,7 +2887,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2897,11 +2897,11 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2912,7 +2912,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2922,11 +2922,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -3012,7 +3012,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -3026,7 +3026,7 @@
         </is>
       </c>
       <c r="D107" t="n">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3062,12 +3062,12 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>09:39</t>
+          <t>09:35</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3076,7 +3076,7 @@
         </is>
       </c>
       <c r="D109" t="n">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3092,16 +3092,16 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:39</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3117,16 +3117,16 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>09:42</t>
+          <t>09:41</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3137,7 +3137,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3147,11 +3147,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,21 +3162,21 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>09:42</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3187,21 +3187,21 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>09:52</t>
+          <t>09:43</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3212,21 +3212,21 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>09:53</t>
+          <t>09:46</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3237,21 +3237,21 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>09:47</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -3262,12 +3262,12 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>10:12</t>
+          <t>09:52</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -3276,7 +3276,7 @@
         </is>
       </c>
       <c r="D117" t="n">
-        <v>93</v>
+        <v>24</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3287,21 +3287,21 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>10:21</t>
+          <t>09:53</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>89</v>
+        <v>25</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3312,21 +3312,21 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>10:26</t>
+          <t>10:02</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3337,21 +3337,21 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>10:42</t>
+          <t>10:03</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>110</v>
+        <v>35</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3362,23 +3362,373 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
+          <t>10:10</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>42</v>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>09:28:24</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>10:12</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D122" t="n">
+        <v>44</v>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>09:28:24</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>10:13</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D123" t="n">
+        <v>45</v>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>09:28:24</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>10:21</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D124" t="n">
+        <v>53</v>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>09:28:24</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>10:23</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D125" t="n">
+        <v>55</v>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>09:28:24</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>10:26</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D126" t="n">
+        <v>58</v>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>09:28:24</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>10:34</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D127" t="n">
+        <v>66</v>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>09:28:24</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>10:42</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>74</v>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>09:28:24</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
           <t>10:43</t>
         </is>
       </c>
-      <c r="C121" t="inlineStr">
+      <c r="C129" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D121" t="n">
+      <c r="D129" t="n">
+        <v>75</v>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>09:28:24</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>10:54</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>86</v>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>09:28:24</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>11:02</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D131" t="n">
+        <v>94</v>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>09:28:24</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>11:06</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D132" t="n">
+        <v>98</v>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>09:28:24</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>11:19</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>86_EST CHICA-ESC AGRARIA</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
         <v>111</v>
       </c>
-      <c r="E121" t="inlineStr">
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>09:28:24</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>11:21</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>113</v>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>09:28:24</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>11:27</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>119</v>
+      </c>
+      <c r="E135" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3395,7 +3745,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3413,14 +3763,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:52:26</t>
+          <t>Última actualización: 09:28:24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 22</t>
+          <t>Total filas: 23</t>
         </is>
       </c>
     </row>
@@ -3954,7 +4304,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -3968,7 +4318,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -3979,7 +4329,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -3993,9 +4343,34 @@
         </is>
       </c>
       <c r="D27" t="n">
+        <v>58</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>09:28:24</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>11:02</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
         <v>94</v>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4012,7 +4387,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4030,14 +4405,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:52:26</t>
+          <t>Última actualización: 09:28:24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 25</t>
+          <t>Total filas: 27</t>
         </is>
       </c>
     </row>
@@ -4671,7 +5046,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -4685,11 +5060,61 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>09:28:24</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>10:54</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>86</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>09:28:24</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>11:14</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>106</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 738
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E135"/>
+  <dimension ref="A1:E159"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 09:28:24</t>
+          <t>Última actualización: 10:25:56</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 130</t>
+          <t>Total filas: 154</t>
         </is>
       </c>
     </row>
@@ -1722,7 +1722,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1747,7 +1747,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -2522,7 +2522,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2547,7 +2547,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -2837,7 +2837,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2847,11 +2847,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2862,7 +2862,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2872,11 +2872,11 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -3137,7 +3137,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3147,11 +3147,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,7 +3162,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3172,11 +3172,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3487,7 +3487,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -3501,7 +3501,7 @@
         </is>
       </c>
       <c r="D126" t="n">
-        <v>58</v>
+        <v>1</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3512,21 +3512,21 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>10:34</t>
+          <t>10:28</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>66</v>
+        <v>3</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3537,21 +3537,21 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>10:42</t>
+          <t>10:34</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>74</v>
+        <v>9</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3562,21 +3562,21 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>10:43</t>
+          <t>10:34</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>75</v>
+        <v>9</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3587,21 +3587,21 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>10:54</t>
+          <t>10:41</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3617,16 +3617,16 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>11:02</t>
+          <t>10:42</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3637,21 +3637,21 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>11:06</t>
+          <t>10:43</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>98</v>
+        <v>18</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3662,21 +3662,21 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>11:19</t>
+          <t>10:46</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>111</v>
+        <v>21</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3687,21 +3687,21 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>11:21</t>
+          <t>10:52</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>113</v>
+        <v>27</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3712,23 +3712,623 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>10:52</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>27</v>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
           <t>09:28:24</t>
         </is>
       </c>
-      <c r="B135" t="inlineStr">
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>10:54</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D136" t="n">
+        <v>86</v>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>10:56</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>31</v>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D138" t="n">
+        <v>36</v>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>09:28:24</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>11:02</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D139" t="n">
+        <v>94</v>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>11:03</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D140" t="n">
+        <v>38</v>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>11:04</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D141" t="n">
+        <v>39</v>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>11:06</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D142" t="n">
+        <v>41</v>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>11:19</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>86_EST CHICA-ESC AGRARIA</t>
+        </is>
+      </c>
+      <c r="D143" t="n">
+        <v>54</v>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>11:20</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D144" t="n">
+        <v>55</v>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>09:28:24</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>11:21</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D145" t="n">
+        <v>113</v>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>11:26</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D146" t="n">
+        <v>61</v>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>09:28:24</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
         <is>
           <t>11:27</t>
         </is>
       </c>
-      <c r="C135" t="inlineStr">
+      <c r="C147" t="inlineStr">
         <is>
           <t>225_C ROCA-H SUR</t>
         </is>
       </c>
-      <c r="D135" t="n">
+      <c r="D147" t="n">
         <v>119</v>
       </c>
-      <c r="E135" t="inlineStr">
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>11:32</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D148" t="n">
+        <v>67</v>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>11:35</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D149" t="n">
+        <v>70</v>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>11:41</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D150" t="n">
+        <v>76</v>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>11:43</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D151" t="n">
+        <v>78</v>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>11:49</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D152" t="n">
+        <v>84</v>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>11:51</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D153" t="n">
+        <v>86</v>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>11:58</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D154" t="n">
+        <v>93</v>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>12:02</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D155" t="n">
+        <v>97</v>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D156" t="n">
+        <v>101</v>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D157" t="n">
+        <v>115</v>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D158" t="n">
+        <v>115</v>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D159" t="n">
+        <v>115</v>
+      </c>
+      <c r="E159" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3745,7 +4345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3763,14 +4363,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 09:28:24</t>
+          <t>Última actualización: 10:25:56</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 23</t>
+          <t>Total filas: 26</t>
         </is>
       </c>
     </row>
@@ -4329,7 +4929,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -4343,7 +4943,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>58</v>
+        <v>1</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -4354,23 +4954,98 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>36</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
           <t>09:28:24</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B29" t="inlineStr">
         <is>
           <t>11:02</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D28" t="n">
+      <c r="D29" t="n">
         <v>94</v>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>11:51</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>86</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>115</v>
+      </c>
+      <c r="E31" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4387,7 +5062,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4405,14 +5080,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 09:28:24</t>
+          <t>Última actualización: 10:25:56</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 27</t>
+          <t>Total filas: 30</t>
         </is>
       </c>
     </row>
@@ -5071,12 +5746,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>10:54</t>
+          <t>10:53</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -5085,7 +5760,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>86</v>
+        <v>28</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -5101,20 +5776,95 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
+          <t>10:54</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>86</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>11:13</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>48</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>09:28:24</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
           <t>11:14</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D32" t="n">
+      <c r="D34" t="n">
         <v>106</v>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>12:03</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>98</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 739
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E159"/>
+  <dimension ref="A1:E176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:25:56</t>
+          <t>Última actualización: 11:00:36</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 154</t>
+          <t>Total filas: 171</t>
         </is>
       </c>
     </row>
@@ -937,7 +937,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>03:42:43</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -947,11 +947,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -962,7 +962,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>04:17:03</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -972,11 +972,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1722,7 +1722,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1772,7 +1772,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -2462,7 +2462,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2472,11 +2472,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2487,7 +2487,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2497,11 +2497,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2522,7 +2522,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2547,7 +2547,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -2797,7 +2797,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D98" t="n">
@@ -2822,7 +2822,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -2837,7 +2837,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2847,11 +2847,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2862,7 +2862,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2872,11 +2872,11 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2887,7 +2887,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2897,11 +2897,11 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2912,7 +2912,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2922,11 +2922,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -3137,7 +3137,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3147,11 +3147,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,7 +3162,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3172,11 +3172,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3547,7 +3547,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D128" t="n">
@@ -3572,7 +3572,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D129" t="n">
@@ -3787,7 +3787,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3797,11 +3797,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3812,12 +3812,12 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>11:02</t>
+          <t>11:01</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -3826,7 +3826,7 @@
         </is>
       </c>
       <c r="D139" t="n">
-        <v>94</v>
+        <v>1</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -3837,21 +3837,21 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>11:03</t>
+          <t>11:02</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3862,21 +3862,21 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>11:04</t>
+          <t>11:02</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -3892,16 +3892,16 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>11:06</t>
+          <t>11:03</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3912,21 +3912,21 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>11:19</t>
+          <t>11:04</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3937,21 +3937,21 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>11:20</t>
+          <t>11:06</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -3962,21 +3962,21 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>11:21</t>
+          <t>11:11</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D145" t="n">
-        <v>113</v>
+        <v>11</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -3987,21 +3987,21 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>11:26</t>
+          <t>11:12</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4012,21 +4012,21 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>11:27</t>
+          <t>11:16</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>119</v>
+        <v>16</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4037,21 +4037,21 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>11:32</t>
+          <t>11:19</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4067,16 +4067,16 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>11:35</t>
+          <t>11:20</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -4087,21 +4087,21 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>11:41</t>
+          <t>11:21</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D150" t="n">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -4112,21 +4112,21 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>11:43</t>
+          <t>11:22</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>78</v>
+        <v>22</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4142,16 +4142,16 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>11:49</t>
+          <t>11:26</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4162,21 +4162,21 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>11:51</t>
+          <t>11:27</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4187,21 +4187,21 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>11:32</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4212,21 +4212,21 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>12:02</t>
+          <t>11:34</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D155" t="n">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -4237,21 +4237,21 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>11:35</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>101</v>
+        <v>35</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -4267,16 +4267,16 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>12:20</t>
+          <t>11:41</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D157" t="n">
-        <v>115</v>
+        <v>76</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -4287,21 +4287,21 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>12:20</t>
+          <t>11:42</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>115</v>
+        <v>42</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -4312,23 +4312,448 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
+          <t>11:00:36</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>11:43</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D159" t="n">
+        <v>43</v>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
           <t>10:25:56</t>
         </is>
       </c>
-      <c r="B159" t="inlineStr">
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>11:49</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D160" t="n">
+        <v>84</v>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>11:00:36</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>11:51</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D161" t="n">
+        <v>51</v>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>11:00:36</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>11:52</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D162" t="n">
+        <v>52</v>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>11:58</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D163" t="n">
+        <v>93</v>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>11:00:36</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>11:59</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D164" t="n">
+        <v>59</v>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>11:00:36</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>12:02</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D165" t="n">
+        <v>62</v>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>11:00:36</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D166" t="n">
+        <v>66</v>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>11:00:36</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D167" t="n">
+        <v>66</v>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>11:00:36</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>12:13</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D168" t="n">
+        <v>73</v>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>11:00:36</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
         <is>
           <t>12:20</t>
         </is>
       </c>
-      <c r="C159" t="inlineStr">
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D169" t="n">
+        <v>80</v>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
         <is>
           <t>26_HERNANDEZ</t>
         </is>
       </c>
-      <c r="D159" t="n">
+      <c r="D170" t="n">
         <v>115</v>
       </c>
-      <c r="E159" t="inlineStr">
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D171" t="n">
+        <v>115</v>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>11:00:36</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D172" t="n">
+        <v>81</v>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>11:00:36</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D173" t="n">
+        <v>81</v>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>11:00:36</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D174" t="n">
+        <v>96</v>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>11:00:36</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>12:38</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="D175" t="n">
+        <v>98</v>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>11:00:36</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D176" t="n">
+        <v>108</v>
+      </c>
+      <c r="E176" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4363,7 +4788,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:25:56</t>
+          <t>Última actualización: 11:00:36</t>
         </is>
       </c>
     </row>
@@ -4954,7 +5379,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -4968,7 +5393,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -5004,7 +5429,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -5018,7 +5443,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -5029,7 +5454,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -5043,7 +5468,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -5062,7 +5487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5080,14 +5505,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:25:56</t>
+          <t>Última actualización: 11:00:36</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 30</t>
+          <t>Total filas: 32</t>
         </is>
       </c>
     </row>
@@ -5796,7 +6221,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -5810,7 +6235,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -5865,6 +6290,56 @@
       <c r="E35" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>11:00:36</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>12:04</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>64</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>11:00:36</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>12:53</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>113</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 740
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E176"/>
+  <dimension ref="A1:E193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:00:36</t>
+          <t>Última actualización: 11:45:10</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 171</t>
+          <t>Total filas: 188</t>
         </is>
       </c>
     </row>
@@ -937,7 +937,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>04:17:03</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -947,11 +947,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -962,7 +962,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>03:42:43</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -972,11 +972,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1472,7 +1472,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1722,7 +1722,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1747,7 +1747,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -2522,7 +2522,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2547,7 +2547,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -2837,7 +2837,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2847,11 +2847,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2862,7 +2862,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2872,11 +2872,11 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2887,7 +2887,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2897,11 +2897,11 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2912,7 +2912,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2922,11 +2922,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -3547,7 +3547,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D128" t="n">
@@ -3572,7 +3572,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D129" t="n">
@@ -3697,7 +3697,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -3722,7 +3722,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D135" t="n">
@@ -3797,7 +3797,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D138" t="n">
@@ -3822,7 +3822,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -4337,21 +4337,21 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:45:10</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>11:49</t>
+          <t>11:46</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>84</v>
+        <v>1</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4362,21 +4362,21 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>11:51</t>
+          <t>11:49</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4387,21 +4387,21 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>11:45:10</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>11:52</t>
+          <t>11:51</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4412,21 +4412,21 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:45:10</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>11:52</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D163" t="n">
-        <v>93</v>
+        <v>7</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -4437,21 +4437,21 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>11:45:10</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>11:59</t>
+          <t>11:57</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4462,21 +4462,21 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>12:02</t>
+          <t>11:58</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4487,21 +4487,21 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>11:45:10</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>11:59</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D166" t="n">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -4512,21 +4512,21 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>11:45:10</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>12:02</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4537,21 +4537,21 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>11:45:10</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>12:13</t>
+          <t>12:05</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4567,16 +4567,16 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>12:20</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4587,21 +4587,21 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>12:20</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>115</v>
+        <v>66</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4612,21 +4612,21 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:45:10</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>12:20</t>
+          <t>12:07</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>115</v>
+        <v>22</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4637,21 +4637,21 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>11:45:10</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:13</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4662,21 +4662,21 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>11:45:10</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:14</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>81</v>
+        <v>29</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4687,21 +4687,21 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:20</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4717,16 +4717,16 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>12:38</t>
+          <t>12:20</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4737,23 +4737,448 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D176" t="n">
+        <v>115</v>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>11:45:10</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D177" t="n">
+        <v>36</v>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>11:45:10</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D178" t="n">
+        <v>36</v>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>11:45:10</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D179" t="n">
+        <v>36</v>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>11:45:10</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>12:35</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D180" t="n">
+        <v>50</v>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>11:45:10</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>12:35</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D181" t="n">
+        <v>50</v>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
           <t>11:00:36</t>
         </is>
       </c>
-      <c r="B176" t="inlineStr">
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D182" t="n">
+        <v>96</v>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>11:45:10</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>12:37</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D183" t="n">
+        <v>52</v>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>11:45:10</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>12:38</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="D184" t="n">
+        <v>53</v>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>11:45:10</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>12:41</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D185" t="n">
+        <v>56</v>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>11:00:36</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
         <is>
           <t>12:48</t>
         </is>
       </c>
-      <c r="C176" t="inlineStr">
+      <c r="C186" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D176" t="n">
+      <c r="D186" t="n">
         <v>108</v>
       </c>
-      <c r="E176" t="inlineStr">
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>11:45:10</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>12:49</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D187" t="n">
+        <v>64</v>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>11:45:10</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>12:50</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D188" t="n">
+        <v>65</v>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>11:45:10</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>13:07</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D189" t="n">
+        <v>82</v>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>11:45:10</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>13:14</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D190" t="n">
+        <v>89</v>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>11:45:10</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>13:20</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D191" t="n">
+        <v>95</v>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>11:45:10</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D192" t="n">
+        <v>96</v>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>11:45:10</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>13:27</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D193" t="n">
+        <v>102</v>
+      </c>
+      <c r="E193" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4770,7 +5195,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4788,14 +5213,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:00:36</t>
+          <t>Última actualización: 11:45:10</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 26</t>
+          <t>Total filas: 28</t>
         </is>
       </c>
     </row>
@@ -5429,7 +5854,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>11:45:10</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -5443,7 +5868,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -5471,6 +5896,56 @@
         <v>80</v>
       </c>
       <c r="E31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>11:45:10</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>36</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>11:45:10</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>13:14</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>89</v>
+      </c>
+      <c r="E33" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5487,7 +5962,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5505,14 +5980,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:00:36</t>
+          <t>Última actualización: 11:45:10</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 32</t>
+          <t>Total filas: 34</t>
         </is>
       </c>
     </row>
@@ -6296,7 +6771,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>11:45:10</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -6310,7 +6785,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -6340,6 +6815,56 @@
       <c r="E37" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>11:45:10</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>12:54</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>69</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>11:45:10</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>13:31</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>106</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 741
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E193"/>
+  <dimension ref="A1:E204"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:45:10</t>
+          <t>Última actualización: 12:04:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 188</t>
+          <t>Total filas: 199</t>
         </is>
       </c>
     </row>
@@ -937,7 +937,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>03:42:43</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -947,11 +947,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -962,7 +962,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>04:17:03</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -972,11 +972,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1472,7 +1472,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -2212,7 +2212,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2222,11 +2222,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2237,7 +2237,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2247,11 +2247,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2797,7 +2797,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D98" t="n">
@@ -2822,7 +2822,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -3137,7 +3137,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3147,11 +3147,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,7 +3162,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3172,11 +3172,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3797,7 +3797,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D138" t="n">
@@ -3822,7 +3822,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -3837,7 +3837,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3847,11 +3847,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>94</v>
+        <v>2</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3862,7 +3862,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3872,11 +3872,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4537,21 +4537,21 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>12:05</t>
+          <t>12:04</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4562,21 +4562,21 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>12:05</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>66</v>
+        <v>1</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4587,21 +4587,21 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>11:45:10</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>12:05</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4612,21 +4612,21 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>12:07</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4637,21 +4637,21 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>12:13</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4662,21 +4662,21 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>12:14</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4687,21 +4687,21 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>12:20</t>
+          <t>12:07</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>115</v>
+        <v>3</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4712,21 +4712,21 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>12:20</t>
+          <t>12:13</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4737,21 +4737,21 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>12:20</t>
+          <t>12:14</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>115</v>
+        <v>10</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4762,21 +4762,21 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:20</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>36</v>
+        <v>115</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4787,21 +4787,21 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:20</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>36</v>
+        <v>115</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4812,12 +4812,12 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:20</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -4826,7 +4826,7 @@
         </is>
       </c>
       <c r="D179" t="n">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4837,21 +4837,21 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>12:35</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D180" t="n">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -4862,21 +4862,21 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>12:35</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D181" t="n">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4887,21 +4887,21 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -4912,21 +4912,21 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>12:37</t>
+          <t>12:35</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D183" t="n">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -4937,21 +4937,21 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>12:38</t>
+          <t>12:35</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4962,21 +4962,21 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>12:41</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -4987,21 +4987,21 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:37</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>108</v>
+        <v>33</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5012,21 +5012,21 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>12:49</t>
+          <t>12:38</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5037,21 +5037,21 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>12:50</t>
+          <t>12:41</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5062,21 +5062,21 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>13:07</t>
+          <t>12:47</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D189" t="n">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -5087,21 +5087,21 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>13:14</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D190" t="n">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -5112,21 +5112,21 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>13:20</t>
+          <t>12:49</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>95</v>
+        <v>45</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -5137,21 +5137,21 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>13:21</t>
+          <t>12:50</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>96</v>
+        <v>46</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -5162,23 +5162,298 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
+          <t>12:04:07</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>12:55</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D193" t="n">
+        <v>51</v>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>12:04:07</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>13:07</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D194" t="n">
+        <v>63</v>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>12:04:07</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>13:14</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D195" t="n">
+        <v>70</v>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>12:04:07</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>13:20</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D196" t="n">
+        <v>76</v>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>12:04:07</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D197" t="n">
+        <v>77</v>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
           <t>11:45:10</t>
         </is>
       </c>
-      <c r="B193" t="inlineStr">
+      <c r="B198" t="inlineStr">
         <is>
           <t>13:27</t>
         </is>
       </c>
-      <c r="C193" t="inlineStr">
+      <c r="C198" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D193" t="n">
+      <c r="D198" t="n">
         <v>102</v>
       </c>
-      <c r="E193" t="inlineStr">
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>12:04:07</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>13:35</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D199" t="n">
+        <v>91</v>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>12:04:07</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>13:36</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D200" t="n">
+        <v>92</v>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>12:04:07</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>13:46</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D201" t="n">
+        <v>102</v>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>12:04:07</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>13:51</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D202" t="n">
+        <v>107</v>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>12:04:07</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D203" t="n">
+        <v>112</v>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>12:04:07</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>13:57</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D204" t="n">
+        <v>113</v>
+      </c>
+      <c r="E204" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5195,7 +5470,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5213,14 +5488,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:45:10</t>
+          <t>Última actualización: 12:04:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 28</t>
+          <t>Total filas: 29</t>
         </is>
       </c>
     </row>
@@ -5904,7 +6179,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -5918,7 +6193,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -5929,7 +6204,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -5943,9 +6218,34 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="E33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>12:04:07</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>13:51</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>107</v>
+      </c>
+      <c r="E34" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5980,7 +6280,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:45:10</t>
+          <t>Última actualización: 12:04:07</t>
         </is>
       </c>
     </row>
@@ -6771,7 +7071,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -6785,7 +7085,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -6821,7 +7121,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -6835,7 +7135,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -6846,7 +7146,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -6860,7 +7160,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 742
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E204"/>
+  <dimension ref="A1:E224"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:04:07</t>
+          <t>Última actualización: 12:44:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 199</t>
+          <t>Total filas: 219</t>
         </is>
       </c>
     </row>
@@ -1722,7 +1722,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1772,7 +1772,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -2212,7 +2212,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2222,11 +2222,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2237,7 +2237,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2247,11 +2247,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2522,7 +2522,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2547,7 +2547,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -2837,7 +2837,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2847,11 +2847,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2862,7 +2862,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2872,11 +2872,11 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2887,7 +2887,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2897,11 +2897,11 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2912,7 +2912,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2922,11 +2922,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -3697,7 +3697,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -3722,7 +3722,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D135" t="n">
@@ -3797,7 +3797,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D138" t="n">
@@ -3822,7 +3822,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -4612,7 +4612,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -4622,11 +4622,11 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4662,7 +4662,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -4672,11 +4672,11 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4762,7 +4762,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4772,11 +4772,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4812,7 +4812,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -4822,11 +4822,11 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4847,7 +4847,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -4897,7 +4897,7 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D182" t="n">
@@ -5062,12 +5062,12 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>12:47</t>
+          <t>12:45</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
@@ -5076,7 +5076,7 @@
         </is>
       </c>
       <c r="D189" t="n">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -5087,21 +5087,21 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:46</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D190" t="n">
-        <v>108</v>
+        <v>2</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -5117,16 +5117,16 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>12:49</t>
+          <t>12:47</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -5137,21 +5137,21 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>12:50</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -5167,16 +5167,16 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>12:55</t>
+          <t>12:49</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5192,16 +5192,16 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>13:07</t>
+          <t>12:50</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5212,21 +5212,21 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>13:14</t>
+          <t>12:55</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D195" t="n">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -5237,21 +5237,21 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>13:20</t>
+          <t>13:02</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D196" t="n">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -5262,21 +5262,21 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>13:21</t>
+          <t>13:02</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D197" t="n">
-        <v>77</v>
+        <v>18</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -5287,21 +5287,21 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>13:27</t>
+          <t>13:04</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D198" t="n">
-        <v>102</v>
+        <v>20</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -5312,21 +5312,21 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>13:35</t>
+          <t>13:06</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>91</v>
+        <v>22</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5342,16 +5342,16 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>13:36</t>
+          <t>13:07</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -5362,21 +5362,21 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>13:46</t>
+          <t>13:08</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -5387,21 +5387,21 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>13:51</t>
+          <t>13:13</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D202" t="n">
-        <v>107</v>
+        <v>29</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -5417,16 +5417,16 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>13:56</t>
+          <t>13:14</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D203" t="n">
-        <v>112</v>
+        <v>70</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -5437,23 +5437,523 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
+          <t>12:44:48</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>13:14</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D204" t="n">
+        <v>30</v>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
           <t>12:04:07</t>
         </is>
       </c>
-      <c r="B204" t="inlineStr">
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>13:20</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D205" t="n">
+        <v>76</v>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>12:44:48</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D206" t="n">
+        <v>37</v>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>12:44:48</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D207" t="n">
+        <v>37</v>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>12:44:48</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>13:26</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D208" t="n">
+        <v>42</v>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>11:45:10</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>13:27</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D209" t="n">
+        <v>102</v>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>12:44:48</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>13:32</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D210" t="n">
+        <v>48</v>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>12:44:48</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>13:34</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D211" t="n">
+        <v>50</v>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>12:04:07</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>13:35</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D212" t="n">
+        <v>91</v>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>12:44:48</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>13:36</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D213" t="n">
+        <v>52</v>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>12:44:48</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>13:46</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D214" t="n">
+        <v>62</v>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>12:44:48</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>13:50</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D215" t="n">
+        <v>66</v>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>12:04:07</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>13:51</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D216" t="n">
+        <v>107</v>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>12:44:48</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>13:55</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D217" t="n">
+        <v>71</v>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>12:04:07</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D218" t="n">
+        <v>112</v>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>12:44:48</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D219" t="n">
+        <v>72</v>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>12:04:07</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
         <is>
           <t>13:57</t>
         </is>
       </c>
-      <c r="C204" t="inlineStr">
+      <c r="C220" t="inlineStr">
         <is>
           <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
-      <c r="D204" t="n">
+      <c r="D220" t="n">
         <v>113</v>
       </c>
-      <c r="E204" t="inlineStr">
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>12:44:48</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>14:04</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D221" t="n">
+        <v>80</v>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>12:44:48</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>14:16</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D222" t="n">
+        <v>92</v>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>12:44:48</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>14:19</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D223" t="n">
+        <v>95</v>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>12:44:48</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>14:21</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D224" t="n">
+        <v>97</v>
+      </c>
+      <c r="E224" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5470,7 +5970,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5488,14 +5988,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:04:07</t>
+          <t>Última actualización: 12:44:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 29</t>
+          <t>Total filas: 32</t>
         </is>
       </c>
     </row>
@@ -6204,12 +6704,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>13:14</t>
+          <t>13:13</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -6218,7 +6718,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -6234,18 +6734,93 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
+          <t>13:14</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>70</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>12:44:48</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>13:50</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>66</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>12:04:07</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
           <t>13:51</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D34" t="n">
+      <c r="D36" t="n">
         <v>107</v>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>12:44:48</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>14:19</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>95</v>
+      </c>
+      <c r="E37" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6262,7 +6837,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6280,14 +6855,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:04:07</t>
+          <t>Última actualización: 12:44:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 34</t>
+          <t>Total filas: 36</t>
         </is>
       </c>
     </row>
@@ -7096,7 +7671,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -7110,7 +7685,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>113</v>
+        <v>9</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -7146,23 +7721,73 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
+          <t>12:44:48</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>13:30</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>46</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
           <t>12:04:07</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B40" t="inlineStr">
         <is>
           <t>13:31</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="C40" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
-      <c r="D39" t="n">
+      <c r="D40" t="n">
         <v>87</v>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>12:44:48</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>14:09</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>85</v>
+      </c>
+      <c r="E41" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 743
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -39,7 +39,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -47,22 +47,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -428,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E224"/>
+  <dimension ref="A1:E234"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,39 +437,39 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:44:48</t>
+          <t>Última actualización: 13:03:49</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 219</t>
+          <t>Total filas: 229</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>Hora_Scrap</t>
         </is>
       </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>Hora_Llegada</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>Linea</t>
         </is>
       </c>
-      <c r="D5" s="2" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Minutos</t>
         </is>
       </c>
-      <c r="E5" s="2" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Parada</t>
         </is>
@@ -937,7 +928,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>04:17:03</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -947,11 +938,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -962,7 +953,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>03:42:43</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -972,11 +963,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1447,7 +1438,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1472,7 +1463,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1722,7 +1713,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1747,7 +1738,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -2797,7 +2788,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D98" t="n">
@@ -2822,7 +2813,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -2887,7 +2878,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2897,11 +2888,11 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2912,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2922,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -3137,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3147,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3172,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3547,7 +3538,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D128" t="n">
@@ -3572,7 +3563,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D129" t="n">
@@ -3797,7 +3788,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D138" t="n">
@@ -3822,7 +3813,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -4637,7 +4628,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -4647,11 +4638,11 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4662,7 +4653,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -4672,11 +4663,11 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4762,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4772,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4787,7 +4778,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4797,11 +4788,11 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4922,7 +4913,7 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D183" t="n">
@@ -4947,7 +4938,7 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D184" t="n">
@@ -5287,21 +5278,21 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>13:04</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D198" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -5312,21 +5303,21 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>13:06</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5337,21 +5328,21 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>13:07</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -5362,21 +5353,21 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>13:08</t>
+          <t>13:04</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -5392,16 +5383,16 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>13:13</t>
+          <t>13:04</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D202" t="n">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -5412,21 +5403,21 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>13:14</t>
+          <t>13:06</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D203" t="n">
-        <v>70</v>
+        <v>3</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -5437,21 +5428,21 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>13:14</t>
+          <t>13:07</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D204" t="n">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -5462,12 +5453,12 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>13:20</t>
+          <t>13:08</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
@@ -5476,7 +5467,7 @@
         </is>
       </c>
       <c r="D205" t="n">
-        <v>76</v>
+        <v>5</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -5487,21 +5478,21 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>13:21</t>
+          <t>13:13</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D206" t="n">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -5512,21 +5503,21 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>13:21</t>
+          <t>13:14</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5537,21 +5528,21 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>13:26</t>
+          <t>13:14</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5562,21 +5553,21 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>13:27</t>
+          <t>13:20</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>102</v>
+        <v>17</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5592,7 +5583,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>13:32</t>
+          <t>13:21</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
@@ -5601,7 +5592,7 @@
         </is>
       </c>
       <c r="D210" t="n">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5612,21 +5603,21 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>13:34</t>
+          <t>13:21</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -5637,21 +5628,21 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>13:35</t>
+          <t>13:26</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D212" t="n">
-        <v>91</v>
+        <v>42</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -5662,12 +5653,12 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>13:36</t>
+          <t>13:26</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
@@ -5676,7 +5667,7 @@
         </is>
       </c>
       <c r="D213" t="n">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5687,21 +5678,21 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>11:45:10</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>13:46</t>
+          <t>13:27</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5712,21 +5703,21 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>13:50</t>
+          <t>13:32</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D215" t="n">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -5737,21 +5728,21 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>13:51</t>
+          <t>13:34</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D216" t="n">
-        <v>107</v>
+        <v>31</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -5762,21 +5753,21 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>13:55</t>
+          <t>13:35</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D217" t="n">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -5787,21 +5778,21 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>13:56</t>
+          <t>13:36</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>112</v>
+        <v>52</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -5812,21 +5803,21 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>13:56</t>
+          <t>13:46</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D219" t="n">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -5837,21 +5828,21 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>13:57</t>
+          <t>13:50</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D220" t="n">
-        <v>113</v>
+        <v>47</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -5862,21 +5853,21 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>14:04</t>
+          <t>13:50</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D221" t="n">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -5887,21 +5878,21 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>14:16</t>
+          <t>13:51</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D222" t="n">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -5912,21 +5903,21 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>14:19</t>
+          <t>13:55</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5937,23 +5928,273 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D224" t="n">
+        <v>112</v>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>13:03:48</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D225" t="n">
+        <v>53</v>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>12:04:07</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>13:57</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D226" t="n">
+        <v>113</v>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>13:03:48</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>14:04</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D227" t="n">
+        <v>61</v>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>13:03:48</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>14:16</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D228" t="n">
+        <v>73</v>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>13:03:48</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>14:19</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D229" t="n">
+        <v>76</v>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>13:03:48</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
           <t>14:21</t>
         </is>
       </c>
-      <c r="C224" t="inlineStr">
+      <c r="C230" t="inlineStr">
         <is>
           <t>26_HERNANDEZ</t>
         </is>
       </c>
-      <c r="D224" t="n">
-        <v>97</v>
-      </c>
-      <c r="E224" t="inlineStr">
+      <c r="D230" t="n">
+        <v>78</v>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>13:03:48</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>14:44</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D231" t="n">
+        <v>101</v>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>13:03:48</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>14:56</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D232" t="n">
+        <v>113</v>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>13:03:48</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D233" t="n">
+        <v>115</v>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>13:03:48</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D234" t="n">
+        <v>117</v>
+      </c>
+      <c r="E234" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5970,7 +6211,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5988,39 +6229,39 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:44:48</t>
+          <t>Última actualización: 13:03:49</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 32</t>
+          <t>Total filas: 33</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>Hora_Scrap</t>
         </is>
       </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>Hora_Llegada</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>Linea</t>
         </is>
       </c>
-      <c r="D5" s="2" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Minutos</t>
         </is>
       </c>
-      <c r="E5" s="2" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Parada</t>
         </is>
@@ -6704,7 +6945,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -6718,7 +6959,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -6754,7 +6995,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -6768,7 +7009,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -6804,7 +7045,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -6818,9 +7059,34 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="E37" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>13:03:48</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>115</v>
+      </c>
+      <c r="E38" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6837,7 +7103,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6855,39 +7121,39 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:44:48</t>
+          <t>Última actualización: 13:03:49</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 36</t>
+          <t>Total filas: 37</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>Hora_Scrap</t>
         </is>
       </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>Hora_Llegada</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>Linea</t>
         </is>
       </c>
-      <c r="D5" s="2" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Minutos</t>
         </is>
       </c>
-      <c r="E5" s="2" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Parada</t>
         </is>
@@ -7721,7 +7987,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -7735,7 +8001,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -7771,7 +8037,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -7785,11 +8051,36 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>13:03:48</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>14:52</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>109</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 744
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E234"/>
+  <dimension ref="A1:E252"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:03:49</t>
+          <t>Última actualización: 14:13:45</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 229</t>
+          <t>Total filas: 247</t>
         </is>
       </c>
     </row>
@@ -928,7 +928,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>03:42:43</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -938,11 +938,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -953,7 +953,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>04:17:03</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -963,11 +963,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2513,7 +2513,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2538,7 +2538,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -2788,7 +2788,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D98" t="n">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2853,7 +2853,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2863,11 +2863,11 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3788,7 +3788,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D138" t="n">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -4553,7 +4553,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>11:45:10</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -4563,11 +4563,11 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4578,7 +4578,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -4588,11 +4588,11 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4603,7 +4603,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -4613,11 +4613,11 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4628,7 +4628,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -4638,11 +4638,11 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4663,7 +4663,7 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D173" t="n">
@@ -4763,7 +4763,7 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D177" t="n">
@@ -4778,7 +4778,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4788,11 +4788,11 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4803,7 +4803,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -4813,11 +4813,11 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4838,7 +4838,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -4888,7 +4888,7 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D182" t="n">
@@ -5238,7 +5238,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D196" t="n">
@@ -5263,7 +5263,7 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D197" t="n">
@@ -5503,7 +5503,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -5513,11 +5513,11 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5578,7 +5578,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -5588,11 +5588,11 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5603,7 +5603,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -5613,11 +5613,11 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5938,11 +5938,11 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>112</v>
+        <v>53</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5953,7 +5953,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -5963,11 +5963,11 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -6028,21 +6028,21 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>14:16</t>
+          <t>14:13</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6053,21 +6053,21 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>14:19</t>
+          <t>14:16</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6078,21 +6078,21 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>14:21</t>
+          <t>14:16</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>78</v>
+        <v>3</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6103,21 +6103,21 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>14:44</t>
+          <t>14:19</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6128,21 +6128,21 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>14:56</t>
+          <t>14:21</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6153,21 +6153,21 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>14:58</t>
+          <t>14:34</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D233" t="n">
-        <v>115</v>
+        <v>21</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -6178,23 +6178,473 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
+          <t>14:44</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D234" t="n">
+        <v>31</v>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>14:46</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D235" t="n">
+        <v>33</v>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>14:51</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D236" t="n">
+        <v>38</v>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>14:56</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D237" t="n">
+        <v>43</v>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D238" t="n">
+        <v>45</v>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
           <t>15:00</t>
         </is>
       </c>
-      <c r="C234" t="inlineStr">
+      <c r="C239" t="inlineStr">
         <is>
           <t>81_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D234" t="n">
-        <v>117</v>
-      </c>
-      <c r="E234" t="inlineStr">
+      <c r="D239" t="n">
+        <v>47</v>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>15:05</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D240" t="n">
+        <v>52</v>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>15:06</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D241" t="n">
+        <v>53</v>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>15:10</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D242" t="n">
+        <v>57</v>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>15:13</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D243" t="n">
+        <v>60</v>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>15:20</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D244" t="n">
+        <v>67</v>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>15:21</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D245" t="n">
+        <v>68</v>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>15:32</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D246" t="n">
+        <v>79</v>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>15:36</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D247" t="n">
+        <v>83</v>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>15:37</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D248" t="n">
+        <v>84</v>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>15:38</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D249" t="n">
+        <v>85</v>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>15:46</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D250" t="n">
+        <v>93</v>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D251" t="n">
+        <v>100</v>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>15:56</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D252" t="n">
+        <v>103</v>
+      </c>
+      <c r="E252" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6211,7 +6661,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6229,14 +6679,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:03:49</t>
+          <t>Última actualización: 14:13:45</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 33</t>
+          <t>Total filas: 34</t>
         </is>
       </c>
     </row>
@@ -7045,7 +7495,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -7059,7 +7509,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -7070,7 +7520,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -7084,9 +7534,34 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="E38" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>15:38</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>85</v>
+      </c>
+      <c r="E39" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7103,7 +7578,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7121,14 +7596,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:03:49</t>
+          <t>Última actualización: 14:13:45</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 37</t>
+          <t>Total filas: 38</t>
         </is>
       </c>
     </row>
@@ -8062,7 +8537,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -8076,11 +8551,36 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>109</v>
+        <v>39</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>15:34</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>81</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 745
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E252"/>
+  <dimension ref="A1:E273"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:13:45</t>
+          <t>Última actualización: 15:06:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 247</t>
+          <t>Total filas: 268</t>
         </is>
       </c>
     </row>
@@ -928,7 +928,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>04:17:03</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -938,11 +938,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -953,7 +953,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>03:42:43</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -963,11 +963,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2513,7 +2513,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2538,7 +2538,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -2788,7 +2788,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D98" t="n">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2853,7 +2853,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2863,11 +2863,11 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3538,7 +3538,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D128" t="n">
@@ -3563,7 +3563,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D129" t="n">
@@ -3828,7 +3828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3838,11 +3838,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,7 +3853,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3863,11 +3863,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>94</v>
+        <v>2</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4603,7 +4603,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -4613,11 +4613,11 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4653,7 +4653,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -4663,11 +4663,11 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4763,7 +4763,7 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D177" t="n">
@@ -4778,7 +4778,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4788,11 +4788,11 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4803,7 +4803,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -4813,11 +4813,11 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4838,7 +4838,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -4888,7 +4888,7 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D182" t="n">
@@ -4913,7 +4913,7 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D183" t="n">
@@ -4938,7 +4938,7 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D184" t="n">
@@ -5238,7 +5238,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D196" t="n">
@@ -5263,7 +5263,7 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D197" t="n">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -5353,7 +5353,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -5363,11 +5363,11 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -5378,7 +5378,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
@@ -5388,11 +5388,11 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D202" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -5578,7 +5578,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -5588,11 +5588,11 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5603,7 +5603,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -5613,11 +5613,11 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -6378,21 +6378,21 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>15:10</t>
+          <t>15:06</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6403,21 +6403,21 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>15:13</t>
+          <t>15:10</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6433,16 +6433,16 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>15:20</t>
+          <t>15:13</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6453,21 +6453,21 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>15:21</t>
+          <t>15:14</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -6478,21 +6478,21 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>15:32</t>
+          <t>15:17</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D246" t="n">
-        <v>79</v>
+        <v>11</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -6503,21 +6503,21 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>15:36</t>
+          <t>15:20</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D247" t="n">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -6528,21 +6528,21 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>15:37</t>
+          <t>15:21</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D248" t="n">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -6553,21 +6553,21 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>15:38</t>
+          <t>15:27</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D249" t="n">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -6578,21 +6578,21 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>15:46</t>
+          <t>15:32</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -6603,21 +6603,21 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:35</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D251" t="n">
-        <v>100</v>
+        <v>29</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -6633,18 +6633,543 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
+          <t>15:36</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D252" t="n">
+        <v>83</v>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>15:37</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D253" t="n">
+        <v>31</v>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>15:38</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D254" t="n">
+        <v>85</v>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>15:39</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D255" t="n">
+        <v>33</v>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>15:45</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D256" t="n">
+        <v>39</v>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>15:46</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D257" t="n">
+        <v>40</v>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>15:46</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D258" t="n">
+        <v>93</v>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>15:47</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D259" t="n">
+        <v>41</v>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D260" t="n">
+        <v>100</v>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>15:54</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D261" t="n">
+        <v>48</v>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
           <t>15:56</t>
         </is>
       </c>
-      <c r="C252" t="inlineStr">
+      <c r="C262" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="D252" t="n">
+      <c r="D262" t="n">
         <v>103</v>
       </c>
-      <c r="E252" t="inlineStr">
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>15:57</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D263" t="n">
+        <v>51</v>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>16:01</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D264" t="n">
+        <v>55</v>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>16:09</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D265" t="n">
+        <v>63</v>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>16:15</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D266" t="n">
+        <v>69</v>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D267" t="n">
+        <v>74</v>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>16:21</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D268" t="n">
+        <v>75</v>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D269" t="n">
+        <v>84</v>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>16:43</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D270" t="n">
+        <v>97</v>
+      </c>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>16:43</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D271" t="n">
+        <v>97</v>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>16:56</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="D272" t="n">
+        <v>110</v>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D273" t="n">
+        <v>119</v>
+      </c>
+      <c r="E273" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6661,7 +7186,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6679,14 +7204,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:13:45</t>
+          <t>Última actualización: 15:06:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 34</t>
+          <t>Total filas: 37</t>
         </is>
       </c>
     </row>
@@ -7562,6 +8087,81 @@
         <v>85</v>
       </c>
       <c r="E39" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>15:39</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>33</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>74</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>119</v>
+      </c>
+      <c r="E42" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7578,7 +8178,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7596,14 +8196,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:13:45</t>
+          <t>Última actualización: 15:06:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 38</t>
+          <t>Total filas: 40</t>
         </is>
       </c>
     </row>
@@ -8562,7 +9162,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -8576,9 +9176,59 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E43" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>16:14</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>68</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>16:53</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>107</v>
+      </c>
+      <c r="E45" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 746
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E273"/>
+  <dimension ref="A1:E295"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:06:15</t>
+          <t>Última actualización: 15:57:46</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 268</t>
+          <t>Total filas: 290</t>
         </is>
       </c>
     </row>
@@ -928,7 +928,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>03:42:43</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -938,11 +938,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -953,7 +953,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>04:17:03</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -963,11 +963,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1738,7 +1738,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2513,7 +2513,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2538,7 +2538,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -2788,7 +2788,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D98" t="n">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2853,7 +2853,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2863,11 +2863,11 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2878,7 +2878,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2888,11 +2888,11 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3688,7 +3688,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -3713,7 +3713,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D135" t="n">
@@ -3828,7 +3828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3838,11 +3838,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>94</v>
+        <v>2</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,7 +3853,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3863,11 +3863,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4553,7 +4553,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -4563,11 +4563,11 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4578,7 +4578,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>11:45:10</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -4588,11 +4588,11 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4628,7 +4628,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -4638,11 +4638,11 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4653,7 +4653,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -4663,11 +4663,11 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4778,7 +4778,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4788,11 +4788,11 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4803,7 +4803,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -4813,11 +4813,11 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4838,7 +4838,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -4888,7 +4888,7 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D182" t="n">
@@ -5238,7 +5238,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D196" t="n">
@@ -5263,7 +5263,7 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D197" t="n">
@@ -6063,7 +6063,7 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D229" t="n">
@@ -6088,7 +6088,7 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D230" t="n">
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,7 +6378,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6388,11 +6388,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6753,7 +6753,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -6763,11 +6763,11 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6778,7 +6778,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -6788,11 +6788,11 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -6903,7 +6903,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>15:57:46</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
@@ -6913,11 +6913,11 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D263" t="n">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -6928,21 +6928,21 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>15:57:46</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>16:01</t>
+          <t>15:57</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -6953,21 +6953,21 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>15:57:46</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>16:09</t>
+          <t>15:59</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -6983,16 +6983,16 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>16:01</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D266" t="n">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -7003,21 +7003,21 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>15:57:46</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>16:02</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D267" t="n">
-        <v>74</v>
+        <v>5</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -7028,21 +7028,21 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>15:57:46</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>16:21</t>
+          <t>16:08</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D268" t="n">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -7058,16 +7058,16 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>16:09</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D269" t="n">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -7078,21 +7078,21 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>15:57:46</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>16:43</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>97</v>
+        <v>18</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -7103,21 +7103,21 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>15:57:46</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>16:43</t>
+          <t>16:18</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -7128,21 +7128,21 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>15:57:46</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>16:19</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -7158,18 +7158,568 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D273" t="n">
+        <v>74</v>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>16:21</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D274" t="n">
+        <v>24</v>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>16:22</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D275" t="n">
+        <v>25</v>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D276" t="n">
+        <v>33</v>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>16:34</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D277" t="n">
+        <v>37</v>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>16:36</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D278" t="n">
+        <v>39</v>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>16:42</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D279" t="n">
+        <v>45</v>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>16:43</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D280" t="n">
+        <v>97</v>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>16:43</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D281" t="n">
+        <v>46</v>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>16:48</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D282" t="n">
+        <v>51</v>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>16:56</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="D283" t="n">
+        <v>59</v>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>16:57</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D284" t="n">
+        <v>60</v>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>17:04</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D285" t="n">
+        <v>67</v>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>17:04</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D286" t="n">
+        <v>67</v>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
           <t>17:05</t>
         </is>
       </c>
-      <c r="C273" t="inlineStr">
+      <c r="C287" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D273" t="n">
+      <c r="D287" t="n">
         <v>119</v>
       </c>
-      <c r="E273" t="inlineStr">
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>17:07</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D288" t="n">
+        <v>70</v>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>17:21</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D289" t="n">
+        <v>84</v>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>17:24</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D290" t="n">
+        <v>87</v>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>17:34</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D291" t="n">
+        <v>97</v>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>17:40</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D292" t="n">
+        <v>103</v>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>17:42</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D293" t="n">
+        <v>105</v>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D294" t="n">
+        <v>113</v>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>17:52</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D295" t="n">
+        <v>115</v>
+      </c>
+      <c r="E295" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7181,998 +7731,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E42"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>LÍNEA 141 - LP1912-215 - 21/01/2026</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Última actualización: 15:06:15</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Total filas: 37</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Hora_Scrap</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Hora_Llegada</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Linea</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Minutos</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Parada</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>01:12:01</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>01:12</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>215_ALUAR</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>02:49:45</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>02:49</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>215_ALUAR</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>01:12:01</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>02:58</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>215_ALUAR</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>106</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>01:56:31</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>02:59</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>215_ALUAR</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>63</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>02:24:16</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>03:58</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>215_ALUAR</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>94</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>04:17:03</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>04:31</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>215_ALUAR</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>14</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>02:49:45</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>04:35</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>215_ALUAR</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>106</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>03:00:18</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>04:44</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>215_ALUAR</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>104</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>04:44:38</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>04:45</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>1</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>05:27:50</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>05:34</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>7</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>04:17:03</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>05:35</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>78</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>05:55:46</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>06:11</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>16</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>04:17:03</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>06:12</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>115</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>06:25:30</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>06:46</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>21</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>06:52:31</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>07:11</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>19</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>07:50:23</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>07:51</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>215D_EL PATO</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>1</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>07:17:57</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>08:22</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>65</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>08:16:28</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>08:23</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>7</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>08:52:26</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>09:01</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>9</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>08:39:38</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>09:41</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>62</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>09:28:24</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>09:42</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>14</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>10:25:56</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>10:26</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
-        <v>1</v>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>11:00:36</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>11:01</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>1</v>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>09:28:24</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>11:02</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>94</v>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>11:45:10</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>11:51</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D30" t="n">
-        <v>6</v>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>11:00:36</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>12:20</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
-        <v>80</v>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>12:04:07</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>12:21</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D32" t="n">
-        <v>17</v>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>13:03:48</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>13:13</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>215D_EL PATO</t>
-        </is>
-      </c>
-      <c r="D33" t="n">
-        <v>10</v>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>12:04:07</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>13:14</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>215D_EL PATO</t>
-        </is>
-      </c>
-      <c r="D34" t="n">
-        <v>70</v>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>13:03:48</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>13:50</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
-        <v>47</v>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>12:04:07</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>13:51</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D36" t="n">
-        <v>107</v>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>14:13:45</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>14:19</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
-        <v>6</v>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>14:13:45</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>14:58</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D38" t="n">
-        <v>45</v>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>14:13:45</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>15:38</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D39" t="n">
-        <v>85</v>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>15:06:15</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>15:39</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D40" t="n">
-        <v>33</v>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>15:06:15</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>16:20</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="D41" t="n">
-        <v>74</v>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>15:06:15</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>17:05</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D42" t="n">
-        <v>119</v>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -8189,14 +7747,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - 6203-6173 - 21/01/2026</t>
+          <t>LÍNEA 141 - LP1912-215 - 21/01/2026</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:06:15</t>
+          <t>Última actualización: 15:57:46</t>
         </is>
       </c>
     </row>
@@ -8237,6 +7795,1073 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>01:12:01</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>01:12</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>02:49:45</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>02:49</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>01:12:01</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>02:58</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>106</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>01:56:31</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>02:59</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>63</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>02:24:16</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>03:58</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>94</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>04:17:03</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>04:31</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>14</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>02:49:45</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>04:35</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>106</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>03:00:18</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>04:44</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>104</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>04:44:38</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>04:45</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>05:27:50</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>05:34</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>7</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>04:17:03</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>78</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>05:55:46</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>06:11</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>16</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>04:17:03</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>06:12</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>115</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>06:25:30</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>06:46</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>21</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>06:52:31</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>07:11</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>19</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>07:50:23</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>07:17:57</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>08:22</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>65</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>08:16:28</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>7</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>08:52:26</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>09:01</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>9</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>08:39:38</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>62</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>09:28:24</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>14</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>10:25:56</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>10:26</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>11:00:36</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>09:28:24</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>11:02</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>94</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>11:45:10</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>11:51</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>6</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>11:00:36</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>80</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>12:04:07</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>17</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>13:03:48</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>13:13</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>10</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>12:04:07</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>13:14</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>70</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>13:03:48</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>13:50</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>47</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>12:04:07</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>13:51</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>107</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>14:19</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>6</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>45</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>14:13:45</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>15:38</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>85</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>15:39</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>33</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>16:19</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>22</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>74</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>17:04</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>67</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>119</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>17:40</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>103</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LÍNEA 141 - 6203-6173 - 21/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Última actualización: 15:57:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Total filas: 43</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Linea</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Parada</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>00:05:23</t>
         </is>
       </c>
@@ -9187,12 +9812,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>15:57:46</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>16:14</t>
+          <t>16:13</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -9201,7 +9826,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -9217,18 +9842,93 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
+          <t>16:14</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>68</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>16:52</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>55</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>15:06:15</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
           <t>16:53</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="C47" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
-      <c r="D45" t="n">
+      <c r="D47" t="n">
         <v>107</v>
       </c>
-      <c r="E45" t="inlineStr">
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>17:23</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>86</v>
+      </c>
+      <c r="E48" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 747
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E295"/>
+  <dimension ref="A1:E306"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:57:46</t>
+          <t>Última actualización: 16:24:39</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 290</t>
+          <t>Total filas: 301</t>
         </is>
       </c>
     </row>
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2513,7 +2513,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2538,7 +2538,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -2788,7 +2788,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D98" t="n">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -2878,7 +2878,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2888,11 +2888,11 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3688,7 +3688,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -3713,7 +3713,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D135" t="n">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D138" t="n">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -3828,7 +3828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3838,11 +3838,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,7 +3853,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3863,11 +3863,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>94</v>
+        <v>2</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4553,7 +4553,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>11:45:10</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -4563,11 +4563,11 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4578,7 +4578,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -4588,11 +4588,11 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4613,7 +4613,7 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D171" t="n">
@@ -4663,7 +4663,7 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D173" t="n">
@@ -4763,7 +4763,7 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D177" t="n">
@@ -4778,7 +4778,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4788,11 +4788,11 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4803,7 +4803,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -4813,11 +4813,11 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4838,7 +4838,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -4863,7 +4863,7 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D181" t="n">
@@ -4888,7 +4888,7 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D182" t="n">
@@ -4913,7 +4913,7 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D183" t="n">
@@ -4938,7 +4938,7 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D184" t="n">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -5353,7 +5353,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -5363,11 +5363,11 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -5378,7 +5378,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
@@ -5388,11 +5388,11 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D202" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -5503,7 +5503,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -5513,11 +5513,11 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -6753,7 +6753,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -6763,11 +6763,11 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6778,7 +6778,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -6788,11 +6788,11 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -6913,7 +6913,7 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D263" t="n">
@@ -6938,7 +6938,7 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D264" t="n">
@@ -7253,7 +7253,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
@@ -7263,11 +7263,11 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7278,21 +7278,21 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>16:36</t>
+          <t>16:34</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7303,21 +7303,21 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>16:42</t>
+          <t>16:36</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D279" t="n">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -7328,12 +7328,12 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>16:43</t>
+          <t>16:42</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -7342,7 +7342,7 @@
         </is>
       </c>
       <c r="D280" t="n">
-        <v>97</v>
+        <v>18</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -7353,7 +7353,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -7367,7 +7367,7 @@
         </is>
       </c>
       <c r="D281" t="n">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7378,21 +7378,21 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>16:48</t>
+          <t>16:43</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>51</v>
+        <v>97</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -7403,21 +7403,21 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>16:48</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7428,21 +7428,21 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>16:57</t>
+          <t>16:50</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7453,21 +7453,21 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -7478,21 +7478,21 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7503,21 +7503,21 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>17:05</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>119</v>
+        <v>40</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7528,12 +7528,12 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -7542,7 +7542,7 @@
         </is>
       </c>
       <c r="D288" t="n">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -7553,21 +7553,21 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7578,21 +7578,21 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:05</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7608,16 +7608,16 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D291" t="n">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -7628,21 +7628,21 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>103</v>
+        <v>46</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,21 +7653,21 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>17:42</t>
+          <t>17:20</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>105</v>
+        <v>56</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7678,21 +7678,21 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>113</v>
+        <v>57</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7703,23 +7703,298 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
+          <t>16:24:39</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>17:24</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D295" t="n">
+        <v>60</v>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>16:24:39</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>17:28</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D296" t="n">
+        <v>64</v>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>16:24:39</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>17:31</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D297" t="n">
+        <v>67</v>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>16:24:39</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>17:32</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D298" t="n">
+        <v>68</v>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
           <t>15:57:46</t>
         </is>
       </c>
-      <c r="B295" t="inlineStr">
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>17:34</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D299" t="n">
+        <v>97</v>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>16:24:39</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D300" t="n">
+        <v>74</v>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>16:24:39</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>17:40</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D301" t="n">
+        <v>76</v>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>17:42</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D302" t="n">
+        <v>105</v>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>16:24:39</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D303" t="n">
+        <v>86</v>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>16:24:39</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
         <is>
           <t>17:52</t>
         </is>
       </c>
-      <c r="C295" t="inlineStr">
+      <c r="C304" t="inlineStr">
         <is>
           <t>81_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D295" t="n">
-        <v>115</v>
-      </c>
-      <c r="E295" t="inlineStr">
+      <c r="D304" t="n">
+        <v>88</v>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>16:24:39</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D305" t="n">
+        <v>100</v>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>16:24:39</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D306" t="n">
+        <v>117</v>
+      </c>
+      <c r="E306" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7754,7 +8029,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:57:46</t>
+          <t>Última actualización: 16:24:39</t>
         </is>
       </c>
     </row>
@@ -8720,7 +8995,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -8734,7 +9009,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -8770,7 +9045,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -8784,7 +9059,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -8803,7 +9078,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8821,14 +9096,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:57:46</t>
+          <t>Última actualización: 16:24:39</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 43</t>
+          <t>Total filas: 45</t>
         </is>
       </c>
     </row>
@@ -9862,7 +10137,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -9876,7 +10151,7 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -9931,6 +10206,56 @@
       <c r="E48" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>16:24:39</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>17:25</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>61</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>16:24:39</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>18:03</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>99</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 748
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E306"/>
+  <dimension ref="A1:E314"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:24:39</t>
+          <t>Última actualización: 16:47:36</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 301</t>
+          <t>Total filas: 309</t>
         </is>
       </c>
     </row>
@@ -928,7 +928,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>04:17:03</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -938,11 +938,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -953,7 +953,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>03:42:43</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -963,11 +963,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1738,7 +1738,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2513,7 +2513,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2538,7 +2538,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -2788,7 +2788,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D98" t="n">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2853,7 +2853,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2863,11 +2863,11 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4603,7 +4603,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -4613,11 +4613,11 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4628,7 +4628,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -4638,11 +4638,11 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4763,7 +4763,7 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D177" t="n">
@@ -4778,7 +4778,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4788,11 +4788,11 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4803,7 +4803,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -4813,11 +4813,11 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4838,7 +4838,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -4863,7 +4863,7 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D181" t="n">
@@ -4888,7 +4888,7 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D182" t="n">
@@ -4913,7 +4913,7 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D183" t="n">
@@ -4938,7 +4938,7 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D184" t="n">
@@ -5238,7 +5238,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D196" t="n">
@@ -5263,7 +5263,7 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D197" t="n">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -5353,7 +5353,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -5363,11 +5363,11 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -5378,7 +5378,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
@@ -5388,11 +5388,11 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D202" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -5503,7 +5503,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -5513,11 +5513,11 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5578,7 +5578,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -5588,11 +5588,11 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5603,7 +5603,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -5613,11 +5613,11 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -7353,7 +7353,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -7363,11 +7363,11 @@
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7378,7 +7378,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
@@ -7388,11 +7388,11 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -7403,7 +7403,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -7413,11 +7413,11 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7433,16 +7433,16 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>16:50</t>
+          <t>16:48</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7458,16 +7458,16 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>16:50</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -7478,21 +7478,21 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>16:57</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7503,21 +7503,21 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7528,7 +7528,7 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
@@ -7542,7 +7542,7 @@
         </is>
       </c>
       <c r="D288" t="n">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -7553,7 +7553,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -7567,7 +7567,7 @@
         </is>
       </c>
       <c r="D289" t="n">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7578,21 +7578,21 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>17:05</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>119</v>
+        <v>17</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7603,21 +7603,21 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>17:05</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D291" t="n">
-        <v>70</v>
+        <v>119</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -7628,21 +7628,21 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>15:57:46</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>17:10</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,21 +7653,21 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>17:20</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7678,21 +7678,21 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:16</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7703,21 +7703,21 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:20</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7728,21 +7728,21 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -7753,21 +7753,21 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>17:31</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -7778,21 +7778,21 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D298" t="n">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -7803,21 +7803,21 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:31</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D299" t="n">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -7833,16 +7833,16 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D300" t="n">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -7853,21 +7853,21 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>15:57:46</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7878,21 +7878,21 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>17:42</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>105</v>
+        <v>47</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7903,21 +7903,21 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D303" t="n">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -7928,21 +7928,21 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D304" t="n">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -7953,21 +7953,21 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D305" t="n">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -7978,23 +7978,223 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
+          <t>17:40</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D306" t="n">
+        <v>53</v>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>17:42</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D307" t="n">
+        <v>105</v>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>16:47:35</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D308" t="n">
+        <v>58</v>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>16:47:35</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D309" t="n">
+        <v>63</v>
+      </c>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>16:47:35</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>17:52</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D310" t="n">
+        <v>65</v>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>16:47:35</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D311" t="n">
+        <v>77</v>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>16:47:35</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
           <t>18:21</t>
         </is>
       </c>
-      <c r="C306" t="inlineStr">
+      <c r="C312" t="inlineStr">
         <is>
           <t>26_HERNANDEZ</t>
         </is>
       </c>
-      <c r="D306" t="n">
-        <v>117</v>
-      </c>
-      <c r="E306" t="inlineStr">
+      <c r="D312" t="n">
+        <v>94</v>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>16:47:35</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>18:28</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D313" t="n">
+        <v>101</v>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>16:47:35</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>18:32</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D314" t="n">
+        <v>105</v>
+      </c>
+      <c r="E314" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8011,7 +8211,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8029,14 +8229,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:24:39</t>
+          <t>Última actualización: 16:47:36</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 40</t>
+          <t>Total filas: 41</t>
         </is>
       </c>
     </row>
@@ -8995,7 +9195,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -9009,7 +9209,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -9045,7 +9245,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -9059,9 +9259,34 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="E45" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>16:47:35</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>18:28</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>101</v>
+      </c>
+      <c r="E46" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9078,7 +9303,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9096,14 +9321,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:24:39</t>
+          <t>Última actualización: 16:47:36</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 45</t>
+          <t>Total filas: 47</t>
         </is>
       </c>
     </row>
@@ -10137,12 +10362,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>16:52</t>
+          <t>16:49</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -10151,7 +10376,7 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -10162,12 +10387,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>16:52</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -10176,7 +10401,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>107</v>
+        <v>28</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -10187,21 +10412,21 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>17:23</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -10212,12 +10437,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>15:57:46</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>17:25</t>
+          <t>17:23</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -10226,7 +10451,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -10237,23 +10462,73 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
+          <t>16:47:35</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>17:24</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>37</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
           <t>16:24:39</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>17:25</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>61</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>16:47:35</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
         <is>
           <t>18:03</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="C52" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D50" t="n">
-        <v>99</v>
-      </c>
-      <c r="E50" t="inlineStr">
+      <c r="D52" t="n">
+        <v>76</v>
+      </c>
+      <c r="E52" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 749
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E314"/>
+  <dimension ref="A1:E334"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:47:36</t>
+          <t>Última actualización: 17:03:02</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 309</t>
+          <t>Total filas: 329</t>
         </is>
       </c>
     </row>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1738,7 +1738,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2513,7 +2513,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2538,7 +2538,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2853,7 +2853,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2863,11 +2863,11 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -3538,7 +3538,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D128" t="n">
@@ -3563,7 +3563,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D129" t="n">
@@ -3688,7 +3688,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -3713,7 +3713,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D135" t="n">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D138" t="n">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -3828,7 +3828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3838,11 +3838,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>94</v>
+        <v>2</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,7 +3853,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3863,11 +3863,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4603,7 +4603,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -4613,11 +4613,11 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4628,7 +4628,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -4638,11 +4638,11 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4838,7 +4838,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -4863,7 +4863,7 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D181" t="n">
@@ -4888,7 +4888,7 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D182" t="n">
@@ -5238,7 +5238,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D196" t="n">
@@ -5263,7 +5263,7 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D197" t="n">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -5353,7 +5353,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -5363,11 +5363,11 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -5378,7 +5378,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
@@ -5388,11 +5388,11 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D202" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -5503,7 +5503,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -5513,11 +5513,11 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5938,11 +5938,11 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5953,7 +5953,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -5963,11 +5963,11 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>112</v>
+        <v>53</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,7 +6378,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6388,11 +6388,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6913,7 +6913,7 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D263" t="n">
@@ -6938,7 +6938,7 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D264" t="n">
@@ -7263,7 +7263,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D277" t="n">
@@ -7288,7 +7288,7 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D278" t="n">
@@ -7538,7 +7538,7 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D288" t="n">
@@ -7563,7 +7563,7 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D289" t="n">
@@ -7603,7 +7603,7 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
@@ -7613,11 +7613,11 @@
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D291" t="n">
-        <v>119</v>
+        <v>2</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -7628,21 +7628,21 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>17:05</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7653,21 +7653,21 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>17:10</t>
+          <t>17:05</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7678,21 +7678,21 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>15:57:46</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>17:16</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7703,21 +7703,21 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>17:20</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7733,16 +7733,16 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:16</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -7753,21 +7753,21 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:17</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -7783,16 +7783,16 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>17:20</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D298" t="n">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -7803,21 +7803,21 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>17:31</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D299" t="n">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -7828,21 +7828,21 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D300" t="n">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -7853,21 +7853,21 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>97</v>
+        <v>37</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7878,21 +7878,21 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:25</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7908,16 +7908,16 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D303" t="n">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -7928,21 +7928,21 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D304" t="n">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -7958,16 +7958,16 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:31</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D305" t="n">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -7978,21 +7978,21 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -8003,21 +8003,21 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>17:42</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>105</v>
+        <v>29</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8028,21 +8028,21 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>15:57:46</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>58</v>
+        <v>97</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8053,21 +8053,21 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8083,16 +8083,16 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8103,21 +8103,21 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>17:35</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D311" t="n">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -8133,16 +8133,16 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D312" t="n">
-        <v>94</v>
+        <v>49</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -8153,21 +8153,21 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>18:28</t>
+          <t>17:37</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D313" t="n">
-        <v>101</v>
+        <v>34</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -8183,18 +8183,518 @@
       </c>
       <c r="B314" t="inlineStr">
         <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D314" t="n">
+        <v>51</v>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>17:03:02</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>17:39</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D315" t="n">
+        <v>36</v>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>16:47:35</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>17:40</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D316" t="n">
+        <v>53</v>
+      </c>
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>16:47:35</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>17:40</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D317" t="n">
+        <v>53</v>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>17:03:02</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>17:41</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D318" t="n">
+        <v>38</v>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>17:03:02</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>17:41</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D319" t="n">
+        <v>38</v>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>15:57:46</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>17:42</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D320" t="n">
+        <v>105</v>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>16:47:35</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D321" t="n">
+        <v>58</v>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>17:03:02</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>17:46</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D322" t="n">
+        <v>43</v>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>16:47:35</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D323" t="n">
+        <v>63</v>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>17:03:02</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>17:51</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D324" t="n">
+        <v>48</v>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>16:47:35</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>17:52</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D325" t="n">
+        <v>65</v>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>17:03:02</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>17:53</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D326" t="n">
+        <v>50</v>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>16:47:35</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D327" t="n">
+        <v>77</v>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>17:03:02</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>18:05</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D328" t="n">
+        <v>62</v>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>17:03:02</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>18:09</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D329" t="n">
+        <v>66</v>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>17:03:02</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D330" t="n">
+        <v>78</v>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>17:03:02</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>18:28</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D331" t="n">
+        <v>85</v>
+      </c>
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>17:03:02</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
           <t>18:32</t>
         </is>
       </c>
-      <c r="C314" t="inlineStr">
+      <c r="C332" t="inlineStr">
         <is>
           <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D314" t="n">
+      <c r="D332" t="n">
+        <v>89</v>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>17:03:02</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>18:48</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D333" t="n">
         <v>105</v>
       </c>
-      <c r="E314" t="inlineStr">
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>17:03:02</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>18:59</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D334" t="n">
+        <v>116</v>
+      </c>
+      <c r="E334" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8211,7 +8711,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8229,14 +8729,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:47:36</t>
+          <t>Última actualización: 17:03:02</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 41</t>
+          <t>Total filas: 43</t>
         </is>
       </c>
     </row>
@@ -9220,7 +9720,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -9234,7 +9734,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>119</v>
+        <v>2</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -9270,23 +9770,73 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
+          <t>17:41</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>38</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>17:03:02</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
           <t>18:28</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="C47" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D46" t="n">
-        <v>101</v>
-      </c>
-      <c r="E46" t="inlineStr">
+      <c r="D47" t="n">
+        <v>85</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>17:03:02</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>18:59</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>116</v>
+      </c>
+      <c r="E48" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9303,7 +9853,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9321,14 +9871,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:47:36</t>
+          <t>Última actualización: 17:03:02</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 47</t>
+          <t>Total filas: 49</t>
         </is>
       </c>
     </row>
@@ -10462,7 +11012,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -10476,7 +11026,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -10531,6 +11081,56 @@
       <c r="E52" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>17:03:02</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>61</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>17:03:02</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>18:52</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>109</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 750
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E334"/>
+  <dimension ref="A1:E351"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:03:02</t>
+          <t>Última actualización: 17:44:09</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 329</t>
+          <t>Total filas: 346</t>
         </is>
       </c>
     </row>
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1738,7 +1738,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2878,7 +2878,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2888,11 +2888,11 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3538,7 +3538,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D128" t="n">
@@ -3563,7 +3563,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D129" t="n">
@@ -3688,7 +3688,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -3713,7 +3713,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D135" t="n">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D138" t="n">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -4553,7 +4553,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -4563,11 +4563,11 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4578,7 +4578,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>11:45:10</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -4588,11 +4588,11 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4763,7 +4763,7 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D177" t="n">
@@ -4788,7 +4788,7 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D178" t="n">
@@ -5238,7 +5238,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D196" t="n">
@@ -5263,7 +5263,7 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D197" t="n">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -5353,7 +5353,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -5363,11 +5363,11 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -5378,7 +5378,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
@@ -5388,11 +5388,11 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D202" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -5503,7 +5503,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -5513,11 +5513,11 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5628,7 +5628,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
@@ -5638,11 +5638,11 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D212" t="n">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -5653,7 +5653,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5663,11 +5663,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -5863,7 +5863,7 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D221" t="n">
@@ -6063,7 +6063,7 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D229" t="n">
@@ -6088,7 +6088,7 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D230" t="n">
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,7 +6378,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6388,11 +6388,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6753,7 +6753,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -6763,11 +6763,11 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6778,7 +6778,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -6788,11 +6788,11 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -6913,7 +6913,7 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D263" t="n">
@@ -6938,7 +6938,7 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D264" t="n">
@@ -7353,7 +7353,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -7363,11 +7363,11 @@
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7378,7 +7378,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
@@ -7388,11 +7388,11 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -7403,7 +7403,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -7413,11 +7413,11 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7428,7 +7428,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
@@ -7438,11 +7438,11 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7563,7 +7563,7 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D289" t="n">
@@ -7588,7 +7588,7 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D290" t="n">
@@ -7613,7 +7613,7 @@
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D291" t="n">
@@ -7638,7 +7638,7 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D292" t="n">
@@ -7663,7 +7663,7 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D293" t="n">
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8063,11 +8063,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8078,7 +8078,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8088,11 +8088,11 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8238,7 +8238,7 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D316" t="n">
@@ -8263,7 +8263,7 @@
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D317" t="n">
@@ -8378,7 +8378,7 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
@@ -8388,11 +8388,11 @@
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D322" t="n">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -8403,21 +8403,21 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:46</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8428,12 +8428,12 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -8442,7 +8442,7 @@
         </is>
       </c>
       <c r="D324" t="n">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8453,21 +8453,21 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>17:51</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D325" t="n">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8478,12 +8478,12 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>17:53</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -8492,7 +8492,7 @@
         </is>
       </c>
       <c r="D326" t="n">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8503,21 +8503,21 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>17:53</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -8528,21 +8528,21 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>18:05</t>
+          <t>17:53</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8553,21 +8553,21 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>18:09</t>
+          <t>18:01</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8578,21 +8578,21 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D330" t="n">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -8603,21 +8603,21 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>18:28</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8633,16 +8633,16 @@
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>18:32</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -8658,16 +8658,16 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>18:09</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D333" t="n">
-        <v>105</v>
+        <v>66</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -8678,23 +8678,448 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
         <is>
+          <t>18:11</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D334" t="n">
+        <v>27</v>
+      </c>
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>17:44:08</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>18:16</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D335" t="n">
+        <v>32</v>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>17:44:08</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D336" t="n">
+        <v>37</v>
+      </c>
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>17:44:08</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>18:25</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D337" t="n">
+        <v>41</v>
+      </c>
+      <c r="E337" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>17:44:08</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>18:28</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D338" t="n">
+        <v>44</v>
+      </c>
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>17:44:08</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>18:32</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D339" t="n">
+        <v>48</v>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>17:44:08</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>18:35</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D340" t="n">
+        <v>51</v>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>17:44:08</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>18:41</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D341" t="n">
+        <v>57</v>
+      </c>
+      <c r="E341" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>17:44:08</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>18:48</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D342" t="n">
+        <v>64</v>
+      </c>
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>17:44:08</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>18:52</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D343" t="n">
+        <v>68</v>
+      </c>
+      <c r="E343" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>17:44:08</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
           <t>18:59</t>
         </is>
       </c>
-      <c r="C334" t="inlineStr">
+      <c r="C344" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D334" t="n">
+      <c r="D344" t="n">
+        <v>75</v>
+      </c>
+      <c r="E344" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>17:44:08</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>19:05</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D345" t="n">
+        <v>81</v>
+      </c>
+      <c r="E345" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>17:44:08</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>19:11</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D346" t="n">
+        <v>87</v>
+      </c>
+      <c r="E346" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>17:44:08</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>19:16</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D347" t="n">
+        <v>92</v>
+      </c>
+      <c r="E347" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>17:44:08</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D348" t="n">
+        <v>93</v>
+      </c>
+      <c r="E348" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>17:44:08</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D349" t="n">
+        <v>97</v>
+      </c>
+      <c r="E349" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>17:44:08</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D350" t="n">
+        <v>106</v>
+      </c>
+      <c r="E350" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>17:44:08</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D351" t="n">
         <v>116</v>
       </c>
-      <c r="E334" t="inlineStr">
+      <c r="E351" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8711,7 +9136,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8729,14 +9154,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:03:02</t>
+          <t>Última actualización: 17:44:09</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 43</t>
+          <t>Total filas: 44</t>
         </is>
       </c>
     </row>
@@ -9795,7 +10220,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -9809,7 +10234,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -9820,7 +10245,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -9834,9 +10259,34 @@
         </is>
       </c>
       <c r="D48" t="n">
+        <v>75</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>17:44:08</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
         <v>116</v>
       </c>
-      <c r="E48" t="inlineStr">
+      <c r="E49" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9853,7 +10303,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9871,14 +10321,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:03:02</t>
+          <t>Última actualización: 17:44:09</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 49</t>
+          <t>Total filas: 50</t>
         </is>
       </c>
     </row>
@@ -11087,7 +11537,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -11101,7 +11551,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -11112,7 +11562,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -11126,9 +11576,34 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="E54" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>17:44:08</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>80</v>
+      </c>
+      <c r="E55" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 751
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E351"/>
+  <dimension ref="A1:E366"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:44:09</t>
+          <t>Última actualización: 18:04:26</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 346</t>
+          <t>Total filas: 361</t>
         </is>
       </c>
     </row>
@@ -928,7 +928,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>03:42:43</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -938,11 +938,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -953,7 +953,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>04:17:03</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -963,11 +963,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1738,7 +1738,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2513,7 +2513,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2538,7 +2538,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3538,7 +3538,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D128" t="n">
@@ -3563,7 +3563,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D129" t="n">
@@ -3688,7 +3688,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -3713,7 +3713,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D135" t="n">
@@ -3828,7 +3828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3838,11 +3838,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,7 +3853,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3863,11 +3863,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>94</v>
+        <v>2</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4553,7 +4553,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>11:45:10</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -4563,11 +4563,11 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4578,7 +4578,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -4588,11 +4588,11 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4613,7 +4613,7 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D171" t="n">
@@ -4628,7 +4628,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -4638,11 +4638,11 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4653,7 +4653,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -4663,11 +4663,11 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4803,7 +4803,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -4813,11 +4813,11 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4838,7 +4838,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -4888,7 +4888,7 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D182" t="n">
@@ -4913,7 +4913,7 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D183" t="n">
@@ -4938,7 +4938,7 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D184" t="n">
@@ -5238,7 +5238,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D196" t="n">
@@ -5263,7 +5263,7 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D197" t="n">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -5353,7 +5353,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -5363,11 +5363,11 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -5378,7 +5378,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
@@ -5388,11 +5388,11 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D202" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -5503,7 +5503,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -5513,11 +5513,11 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5628,7 +5628,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
@@ -5638,11 +5638,11 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D212" t="n">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -5653,7 +5653,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5663,11 +5663,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -5863,7 +5863,7 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D221" t="n">
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5938,11 +5938,11 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>112</v>
+        <v>53</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5953,7 +5953,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -5963,11 +5963,11 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -6063,7 +6063,7 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D229" t="n">
@@ -6088,7 +6088,7 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D230" t="n">
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,7 +6378,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6388,11 +6388,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -7263,7 +7263,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D277" t="n">
@@ -7288,7 +7288,7 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D278" t="n">
@@ -7353,7 +7353,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -7363,11 +7363,11 @@
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7378,7 +7378,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
@@ -7388,11 +7388,11 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -7538,7 +7538,7 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D288" t="n">
@@ -7563,7 +7563,7 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D289" t="n">
@@ -7588,7 +7588,7 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D290" t="n">
@@ -7613,7 +7613,7 @@
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D291" t="n">
@@ -7663,7 +7663,7 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D293" t="n">
@@ -7813,7 +7813,7 @@
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D299" t="n">
@@ -7838,7 +7838,7 @@
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D300" t="n">
@@ -7978,7 +7978,7 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
@@ -7988,11 +7988,11 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -8003,7 +8003,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -8013,11 +8013,11 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8028,7 +8028,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -8038,11 +8038,11 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>97</v>
+        <v>31</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>15:57:46</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8063,11 +8063,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>47</v>
+        <v>97</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8078,7 +8078,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8088,11 +8088,11 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8288,7 +8288,7 @@
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D318" t="n">
@@ -8313,7 +8313,7 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D319" t="n">
@@ -8503,7 +8503,7 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
@@ -8513,11 +8513,11 @@
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -8528,7 +8528,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -8538,11 +8538,11 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8578,7 +8578,7 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
@@ -8592,7 +8592,7 @@
         </is>
       </c>
       <c r="D330" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -8653,21 +8653,21 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>18:09</t>
+          <t>18:06</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D333" t="n">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -8678,21 +8678,21 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>18:11</t>
+          <t>18:07</t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D334" t="n">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -8703,21 +8703,21 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>18:16</t>
+          <t>18:09</t>
         </is>
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D335" t="n">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
@@ -8733,16 +8733,16 @@
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>18:11</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D336" t="n">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -8753,21 +8753,21 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>18:25</t>
+          <t>18:16</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D337" t="n">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -8778,21 +8778,21 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>18:28</t>
+          <t>18:16</t>
         </is>
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D338" t="n">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -8803,21 +8803,21 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>18:32</t>
+          <t>18:20</t>
         </is>
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D339" t="n">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
@@ -8828,21 +8828,21 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>18:35</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D340" t="n">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -8853,12 +8853,12 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>18:41</t>
+          <t>18:24</t>
         </is>
       </c>
       <c r="C341" t="inlineStr">
@@ -8867,7 +8867,7 @@
         </is>
       </c>
       <c r="D341" t="n">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -8883,16 +8883,16 @@
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>18:25</t>
         </is>
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D342" t="n">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -8903,21 +8903,21 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>18:28</t>
         </is>
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D343" t="n">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -8928,21 +8928,21 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:30</t>
         </is>
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D344" t="n">
-        <v>75</v>
+        <v>26</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
@@ -8953,21 +8953,21 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>18:32</t>
         </is>
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D345" t="n">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -8978,21 +8978,21 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>19:11</t>
+          <t>18:34</t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D346" t="n">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -9008,16 +9008,16 @@
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D347" t="n">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -9033,16 +9033,16 @@
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>18:41</t>
         </is>
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D348" t="n">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -9053,21 +9053,21 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D349" t="n">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -9078,21 +9078,21 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D350" t="n">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>
@@ -9103,23 +9103,398 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
+          <t>18:04:26</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>18:56</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D351" t="n">
+        <v>52</v>
+      </c>
+      <c r="E351" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>18:04:26</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>18:58</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D352" t="n">
+        <v>54</v>
+      </c>
+      <c r="E352" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
           <t>17:44:08</t>
         </is>
       </c>
-      <c r="B351" t="inlineStr">
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>18:59</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D353" t="n">
+        <v>75</v>
+      </c>
+      <c r="E353" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>18:04:26</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D354" t="n">
+        <v>60</v>
+      </c>
+      <c r="E354" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>17:44:08</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>19:05</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D355" t="n">
+        <v>81</v>
+      </c>
+      <c r="E355" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>18:04:26</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>19:10</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D356" t="n">
+        <v>66</v>
+      </c>
+      <c r="E356" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>17:44:08</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>19:11</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D357" t="n">
+        <v>87</v>
+      </c>
+      <c r="E357" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>17:44:08</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>19:16</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D358" t="n">
+        <v>92</v>
+      </c>
+      <c r="E358" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>18:04:26</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D359" t="n">
+        <v>73</v>
+      </c>
+      <c r="E359" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>18:04:26</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D360" t="n">
+        <v>77</v>
+      </c>
+      <c r="E360" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>18:04:26</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D361" t="n">
+        <v>86</v>
+      </c>
+      <c r="E361" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>18:04:26</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
         <is>
           <t>19:40</t>
         </is>
       </c>
-      <c r="C351" t="inlineStr">
+      <c r="C362" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D351" t="n">
-        <v>116</v>
-      </c>
-      <c r="E351" t="inlineStr">
+      <c r="D362" t="n">
+        <v>96</v>
+      </c>
+      <c r="E362" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>18:04:26</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D363" t="n">
+        <v>106</v>
+      </c>
+      <c r="E363" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>18:04:26</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D364" t="n">
+        <v>106</v>
+      </c>
+      <c r="E364" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>18:04:26</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D365" t="n">
+        <v>107</v>
+      </c>
+      <c r="E365" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>18:04:26</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>19:59</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D366" t="n">
+        <v>115</v>
+      </c>
+      <c r="E366" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9136,7 +9511,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9154,14 +9529,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:44:09</t>
+          <t>Última actualización: 18:04:26</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 44</t>
+          <t>Total filas: 45</t>
         </is>
       </c>
     </row>
@@ -10220,7 +10595,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -10234,7 +10609,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -10245,12 +10620,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -10259,7 +10634,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -10275,18 +10650,43 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
+          <t>18:59</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>75</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>18:04:26</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
           <t>19:40</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="C50" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D49" t="n">
-        <v>116</v>
-      </c>
-      <c r="E49" t="inlineStr">
+      <c r="D50" t="n">
+        <v>96</v>
+      </c>
+      <c r="E50" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10303,7 +10703,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10321,14 +10721,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:44:09</t>
+          <t>Última actualización: 18:04:26</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 50</t>
+          <t>Total filas: 51</t>
         </is>
       </c>
     </row>
@@ -11537,7 +11937,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -11551,7 +11951,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -11562,7 +11962,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -11576,7 +11976,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -11587,7 +11987,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -11601,11 +12001,36 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>18:04:26</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>19:54</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>110</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 752
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E366"/>
+  <dimension ref="A1:E389"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:04:26</t>
+          <t>Última actualización: 18:38:58</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 361</t>
+          <t>Total filas: 384</t>
         </is>
       </c>
     </row>
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1738,7 +1738,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -2513,7 +2513,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2538,7 +2538,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -2878,7 +2878,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2888,11 +2888,11 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -3538,7 +3538,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D128" t="n">
@@ -3563,7 +3563,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D129" t="n">
@@ -4613,7 +4613,7 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D171" t="n">
@@ -4638,7 +4638,7 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D172" t="n">
@@ -4788,7 +4788,7 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D178" t="n">
@@ -4813,7 +4813,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D179" t="n">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -5503,7 +5503,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -5513,11 +5513,11 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5578,7 +5578,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -5588,11 +5588,11 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5603,7 +5603,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -5613,11 +5613,11 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -5628,7 +5628,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
@@ -5638,11 +5638,11 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D212" t="n">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -5653,7 +5653,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5663,11 +5663,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,7 +6378,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6388,11 +6388,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6753,7 +6753,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -6763,11 +6763,11 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6778,7 +6778,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -6788,11 +6788,11 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -6913,7 +6913,7 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D263" t="n">
@@ -6938,7 +6938,7 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D264" t="n">
@@ -7263,7 +7263,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D277" t="n">
@@ -7288,7 +7288,7 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D278" t="n">
@@ -7353,7 +7353,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -7363,11 +7363,11 @@
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7378,7 +7378,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
@@ -7388,11 +7388,11 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -7403,7 +7403,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -7413,11 +7413,11 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7428,7 +7428,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
@@ -7438,11 +7438,11 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -8288,7 +8288,7 @@
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D318" t="n">
@@ -8313,7 +8313,7 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D319" t="n">
@@ -8503,7 +8503,7 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
@@ -8513,11 +8513,11 @@
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -8528,7 +8528,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -8538,11 +8538,11 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8603,7 +8603,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
@@ -8613,11 +8613,11 @@
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8628,7 +8628,7 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
@@ -8638,11 +8638,11 @@
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -9028,21 +9028,21 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:38:58</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>18:41</t>
+          <t>18:38</t>
         </is>
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D348" t="n">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -9053,21 +9053,21 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>18:38:58</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>18:38</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D349" t="n">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -9078,21 +9078,21 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>18:41</t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D350" t="n">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>
@@ -9103,21 +9103,21 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>18:38:58</t>
         </is>
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>18:47</t>
         </is>
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D351" t="n">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="E351" t="inlineStr">
         <is>
@@ -9133,16 +9133,16 @@
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D352" t="n">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E352" t="inlineStr">
         <is>
@@ -9153,21 +9153,21 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:38:58</t>
         </is>
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:51</t>
         </is>
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D353" t="n">
-        <v>75</v>
+        <v>13</v>
       </c>
       <c r="E353" t="inlineStr">
         <is>
@@ -9183,16 +9183,16 @@
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D354" t="n">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="E354" t="inlineStr">
         <is>
@@ -9203,21 +9203,21 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:38:58</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>18:55</t>
         </is>
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D355" t="n">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -9233,16 +9233,16 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D356" t="n">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="E356" t="inlineStr">
         <is>
@@ -9253,21 +9253,21 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:38:58</t>
         </is>
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>19:11</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D357" t="n">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="E357" t="inlineStr">
         <is>
@@ -9283,16 +9283,16 @@
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C358" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D358" t="n">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="E358" t="inlineStr">
         <is>
@@ -9303,21 +9303,21 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>18:38:58</t>
         </is>
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D359" t="n">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
@@ -9328,21 +9328,21 @@
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>18:38:58</t>
         </is>
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D360" t="n">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="E360" t="inlineStr">
         <is>
@@ -9353,21 +9353,21 @@
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D361" t="n">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E361" t="inlineStr">
         <is>
@@ -9378,21 +9378,21 @@
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>18:38:58</t>
         </is>
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C362" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D362" t="n">
-        <v>96</v>
+        <v>32</v>
       </c>
       <c r="E362" t="inlineStr">
         <is>
@@ -9403,21 +9403,21 @@
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:11</t>
         </is>
       </c>
       <c r="C363" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D363" t="n">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="E363" t="inlineStr">
         <is>
@@ -9428,21 +9428,21 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>18:38:58</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:11</t>
         </is>
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D364" t="n">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
@@ -9453,21 +9453,21 @@
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>18:38:58</t>
         </is>
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:15</t>
         </is>
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D365" t="n">
-        <v>107</v>
+        <v>37</v>
       </c>
       <c r="E365" t="inlineStr">
         <is>
@@ -9478,23 +9478,598 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
+          <t>17:44:08</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>19:16</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D366" t="n">
+        <v>92</v>
+      </c>
+      <c r="E366" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>18:38:58</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>19:16</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D367" t="n">
+        <v>38</v>
+      </c>
+      <c r="E367" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
           <t>18:04:26</t>
         </is>
       </c>
-      <c r="B366" t="inlineStr">
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D368" t="n">
+        <v>73</v>
+      </c>
+      <c r="E368" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>18:38:58</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>19:20</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D369" t="n">
+        <v>42</v>
+      </c>
+      <c r="E369" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>18:38:58</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>19:20</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D370" t="n">
+        <v>42</v>
+      </c>
+      <c r="E370" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>18:38:58</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>19:20</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D371" t="n">
+        <v>42</v>
+      </c>
+      <c r="E371" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>18:04:26</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D372" t="n">
+        <v>77</v>
+      </c>
+      <c r="E372" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>18:38:58</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>19:29</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D373" t="n">
+        <v>51</v>
+      </c>
+      <c r="E373" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>18:38:58</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D374" t="n">
+        <v>52</v>
+      </c>
+      <c r="E374" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>18:04:26</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D375" t="n">
+        <v>86</v>
+      </c>
+      <c r="E375" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>18:38:58</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>19:39</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D376" t="n">
+        <v>61</v>
+      </c>
+      <c r="E376" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>18:04:26</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D377" t="n">
+        <v>96</v>
+      </c>
+      <c r="E377" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>18:38:58</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>19:49</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D378" t="n">
+        <v>71</v>
+      </c>
+      <c r="E378" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>18:38:58</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D379" t="n">
+        <v>72</v>
+      </c>
+      <c r="E379" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>18:38:58</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D380" t="n">
+        <v>72</v>
+      </c>
+      <c r="E380" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>18:04:26</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D381" t="n">
+        <v>106</v>
+      </c>
+      <c r="E381" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>18:04:26</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D382" t="n">
+        <v>107</v>
+      </c>
+      <c r="E382" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>18:38:58</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>19:58</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D383" t="n">
+        <v>80</v>
+      </c>
+      <c r="E383" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>18:04:26</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
         <is>
           <t>19:59</t>
         </is>
       </c>
-      <c r="C366" t="inlineStr">
+      <c r="C384" t="inlineStr">
         <is>
           <t>17_ROMERO</t>
         </is>
       </c>
-      <c r="D366" t="n">
+      <c r="D384" t="n">
         <v>115</v>
       </c>
-      <c r="E366" t="inlineStr">
+      <c r="E384" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>18:38:58</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D385" t="n">
+        <v>92</v>
+      </c>
+      <c r="E385" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>18:38:58</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>20:20</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D386" t="n">
+        <v>102</v>
+      </c>
+      <c r="E386" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>18:38:58</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D387" t="n">
+        <v>103</v>
+      </c>
+      <c r="E387" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>18:38:58</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D388" t="n">
+        <v>105</v>
+      </c>
+      <c r="E388" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>18:38:58</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D389" t="n">
+        <v>112</v>
+      </c>
+      <c r="E389" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9511,7 +10086,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9529,14 +10104,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:04:26</t>
+          <t>Última actualización: 18:38:58</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 45</t>
+          <t>Total filas: 47</t>
         </is>
       </c>
     </row>
@@ -10620,7 +11195,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>18:38:58</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -10634,7 +11209,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -10670,23 +11245,73 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
+          <t>18:38:58</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>19:39</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>61</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
           <t>18:04:26</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B51" t="inlineStr">
         <is>
           <t>19:40</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="C51" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D50" t="n">
+      <c r="D51" t="n">
         <v>96</v>
       </c>
-      <c r="E50" t="inlineStr">
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>18:38:58</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>105</v>
+      </c>
+      <c r="E52" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10703,7 +11328,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10721,14 +11346,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:04:26</t>
+          <t>Última actualización: 18:38:58</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 51</t>
+          <t>Total filas: 54</t>
         </is>
       </c>
     </row>
@@ -11962,12 +12587,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>18:38:58</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>18:51</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -11976,7 +12601,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -11992,16 +12617,16 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -12012,23 +12637,98 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
+          <t>18:38:58</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>19:03</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>25</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
           <t>18:04:26</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>60</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>18:04:26</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
         <is>
           <t>19:54</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="C58" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D56" t="n">
+      <c r="D58" t="n">
         <v>110</v>
       </c>
-      <c r="E56" t="inlineStr">
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>18:38:58</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>19:58</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>80</v>
+      </c>
+      <c r="E59" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 753
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E389"/>
+  <dimension ref="A1:E393"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:38:58</t>
+          <t>Última actualización: 18:55:55</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 384</t>
+          <t>Total filas: 388</t>
         </is>
       </c>
     </row>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1738,7 +1738,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2853,7 +2853,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2863,11 +2863,11 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2878,7 +2878,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2888,11 +2888,11 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -3538,7 +3538,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D128" t="n">
@@ -3563,7 +3563,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D129" t="n">
@@ -3688,7 +3688,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -3713,7 +3713,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D135" t="n">
@@ -3828,7 +3828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3838,11 +3838,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>94</v>
+        <v>2</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,7 +3853,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3863,11 +3863,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4613,7 +4613,7 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D171" t="n">
@@ -4628,7 +4628,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -4638,11 +4638,11 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4653,7 +4653,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -4663,11 +4663,11 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4788,7 +4788,7 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D178" t="n">
@@ -4813,7 +4813,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D179" t="n">
@@ -4838,7 +4838,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -4888,7 +4888,7 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D182" t="n">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -5628,7 +5628,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
@@ -5638,11 +5638,11 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D212" t="n">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -5653,7 +5653,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5663,11 +5663,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -5863,7 +5863,7 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D221" t="n">
@@ -6063,7 +6063,7 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D229" t="n">
@@ -6088,7 +6088,7 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D230" t="n">
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,7 +6378,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6388,11 +6388,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6913,7 +6913,7 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D263" t="n">
@@ -6938,7 +6938,7 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D264" t="n">
@@ -7403,7 +7403,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -7413,11 +7413,11 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7428,7 +7428,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
@@ -7438,11 +7438,11 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7538,7 +7538,7 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D288" t="n">
@@ -7588,7 +7588,7 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D290" t="n">
@@ -7613,7 +7613,7 @@
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D291" t="n">
@@ -7638,7 +7638,7 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D292" t="n">
@@ -7663,7 +7663,7 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D293" t="n">
@@ -7978,7 +7978,7 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
@@ -7988,11 +7988,11 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -8003,7 +8003,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -8013,11 +8013,11 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8028,7 +8028,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>15:57:46</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -8038,11 +8038,11 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>31</v>
+        <v>97</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8063,11 +8063,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>97</v>
+        <v>31</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8288,7 +8288,7 @@
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D318" t="n">
@@ -8313,7 +8313,7 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D319" t="n">
@@ -8378,7 +8378,7 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
@@ -8388,11 +8388,11 @@
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D322" t="n">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -8403,7 +8403,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -8413,11 +8413,11 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8503,7 +8503,7 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
@@ -8513,11 +8513,11 @@
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -8528,7 +8528,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -8538,11 +8538,11 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8763,7 +8763,7 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D337" t="n">
@@ -8788,7 +8788,7 @@
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D338" t="n">
@@ -9203,7 +9203,7 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">
@@ -9217,7 +9217,7 @@
         </is>
       </c>
       <c r="D355" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -9253,7 +9253,7 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B357" t="inlineStr">
@@ -9267,7 +9267,7 @@
         </is>
       </c>
       <c r="D357" t="n">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="E357" t="inlineStr">
         <is>
@@ -9303,7 +9303,7 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B359" t="inlineStr">
@@ -9317,7 +9317,7 @@
         </is>
       </c>
       <c r="D359" t="n">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
@@ -9328,7 +9328,7 @@
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B360" t="inlineStr">
@@ -9342,7 +9342,7 @@
         </is>
       </c>
       <c r="D360" t="n">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E360" t="inlineStr">
         <is>
@@ -9378,7 +9378,7 @@
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B362" t="inlineStr">
@@ -9392,7 +9392,7 @@
         </is>
       </c>
       <c r="D362" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="E362" t="inlineStr">
         <is>
@@ -9428,7 +9428,7 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
@@ -9442,7 +9442,7 @@
         </is>
       </c>
       <c r="D364" t="n">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
@@ -9478,7 +9478,7 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
@@ -9492,7 +9492,7 @@
         </is>
       </c>
       <c r="D366" t="n">
-        <v>92</v>
+        <v>21</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -9503,7 +9503,7 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
@@ -9517,7 +9517,7 @@
         </is>
       </c>
       <c r="D367" t="n">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -9553,7 +9553,7 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B369" t="inlineStr">
@@ -9563,11 +9563,11 @@
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D369" t="n">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="E369" t="inlineStr">
         <is>
@@ -9578,7 +9578,7 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B370" t="inlineStr">
@@ -9588,11 +9588,11 @@
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D370" t="n">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="E370" t="inlineStr">
         <is>
@@ -9603,7 +9603,7 @@
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B371" t="inlineStr">
@@ -9617,7 +9617,7 @@
         </is>
       </c>
       <c r="D371" t="n">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="E371" t="inlineStr">
         <is>
@@ -9653,7 +9653,7 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B373" t="inlineStr">
@@ -9667,7 +9667,7 @@
         </is>
       </c>
       <c r="D373" t="n">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="E373" t="inlineStr">
         <is>
@@ -9678,7 +9678,7 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
@@ -9692,7 +9692,7 @@
         </is>
       </c>
       <c r="D374" t="n">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="E374" t="inlineStr">
         <is>
@@ -9728,21 +9728,21 @@
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="C376" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D376" t="n">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="E376" t="inlineStr">
         <is>
@@ -9753,12 +9753,12 @@
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:39</t>
         </is>
       </c>
       <c r="C377" t="inlineStr">
@@ -9767,7 +9767,7 @@
         </is>
       </c>
       <c r="D377" t="n">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="E377" t="inlineStr">
         <is>
@@ -9778,21 +9778,21 @@
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>19:49</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D378" t="n">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="E378" t="inlineStr">
         <is>
@@ -9803,21 +9803,21 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D379" t="n">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="E379" t="inlineStr">
         <is>
@@ -9828,21 +9828,21 @@
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:49</t>
         </is>
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D380" t="n">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="E380" t="inlineStr">
         <is>
@@ -9878,12 +9878,12 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>18:38:58</t>
         </is>
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C382" t="inlineStr">
@@ -9892,7 +9892,7 @@
         </is>
       </c>
       <c r="D382" t="n">
-        <v>107</v>
+        <v>72</v>
       </c>
       <c r="E382" t="inlineStr">
         <is>
@@ -9903,21 +9903,21 @@
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>19:58</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D383" t="n">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -9928,21 +9928,21 @@
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D384" t="n">
-        <v>115</v>
+        <v>56</v>
       </c>
       <c r="E384" t="inlineStr">
         <is>
@@ -9958,16 +9958,16 @@
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:58</t>
         </is>
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D385" t="n">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="E385" t="inlineStr">
         <is>
@@ -9978,21 +9978,21 @@
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>20:20</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="C386" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D386" t="n">
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="E386" t="inlineStr">
         <is>
@@ -10003,21 +10003,21 @@
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C387" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D387" t="n">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="E387" t="inlineStr">
         <is>
@@ -10028,21 +10028,21 @@
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C388" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D388" t="n">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="E388" t="inlineStr">
         <is>
@@ -10053,23 +10053,123 @@
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
+          <t>18:55:55</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>20:20</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D389" t="n">
+        <v>85</v>
+      </c>
+      <c r="E389" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
           <t>18:38:58</t>
         </is>
       </c>
-      <c r="B389" t="inlineStr">
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D390" t="n">
+        <v>103</v>
+      </c>
+      <c r="E390" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>18:55:55</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D391" t="n">
+        <v>88</v>
+      </c>
+      <c r="E391" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>18:55:55</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
         <is>
           <t>20:30</t>
         </is>
       </c>
-      <c r="C389" t="inlineStr">
+      <c r="C392" t="inlineStr">
         <is>
           <t>225_GOMEZ</t>
         </is>
       </c>
-      <c r="D389" t="n">
-        <v>112</v>
-      </c>
-      <c r="E389" t="inlineStr">
+      <c r="D392" t="n">
+        <v>95</v>
+      </c>
+      <c r="E392" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>18:55:55</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>20:46</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D393" t="n">
+        <v>111</v>
+      </c>
+      <c r="E393" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10104,7 +10204,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:38:58</t>
+          <t>Última actualización: 18:55:55</t>
         </is>
       </c>
     </row>
@@ -11195,7 +11295,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -11209,7 +11309,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -11245,7 +11345,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -11259,7 +11359,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -11295,7 +11395,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -11309,7 +11409,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -11328,7 +11428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11346,14 +11446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:38:58</t>
+          <t>Última actualización: 18:55:55</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 54</t>
+          <t>Total filas: 56</t>
         </is>
       </c>
     </row>
@@ -12637,7 +12737,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -12651,7 +12751,7 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -12687,12 +12787,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>19:53</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -12701,7 +12801,7 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>110</v>
+        <v>58</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -12712,25 +12812,75 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
+          <t>18:04:26</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>19:54</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>110</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
           <t>18:38:58</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr">
+      <c r="B60" t="inlineStr">
         <is>
           <t>19:58</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr">
+      <c r="C60" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D59" t="n">
+      <c r="D60" t="n">
         <v>80</v>
       </c>
-      <c r="E59" t="inlineStr">
+      <c r="E60" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>18:55:55</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>20:38</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>103</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 754
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E393"/>
+  <dimension ref="A1:E403"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:55:55</t>
+          <t>Última actualización: 19:16:50</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 388</t>
+          <t>Total filas: 398</t>
         </is>
       </c>
     </row>
@@ -928,7 +928,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>03:42:43</t>
+          <t>04:17:03</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -938,11 +938,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -953,7 +953,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>04:17:03</t>
+          <t>03:42:43</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -963,11 +963,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2513,7 +2513,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2538,7 +2538,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2853,7 +2853,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2863,11 +2863,11 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2878,7 +2878,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2888,11 +2888,11 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -3688,7 +3688,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -3713,7 +3713,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D135" t="n">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D138" t="n">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -4613,7 +4613,7 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D171" t="n">
@@ -4663,7 +4663,7 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D173" t="n">
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4778,7 +4778,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4788,11 +4788,11 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4813,7 +4813,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D179" t="n">
@@ -4838,7 +4838,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -4863,7 +4863,7 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D181" t="n">
@@ -5238,7 +5238,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D196" t="n">
@@ -5263,7 +5263,7 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D197" t="n">
@@ -5503,7 +5503,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -5513,11 +5513,11 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5628,7 +5628,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
@@ -5638,11 +5638,11 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D212" t="n">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -5653,7 +5653,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5663,11 +5663,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -5863,7 +5863,7 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D221" t="n">
@@ -6063,7 +6063,7 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D229" t="n">
@@ -6088,7 +6088,7 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D230" t="n">
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,7 +6378,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6388,11 +6388,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -7263,7 +7263,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D277" t="n">
@@ -7288,7 +7288,7 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D278" t="n">
@@ -7353,7 +7353,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -7363,11 +7363,11 @@
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7378,7 +7378,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
@@ -7388,11 +7388,11 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -7403,7 +7403,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -7413,11 +7413,11 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7428,7 +7428,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
@@ -7438,11 +7438,11 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7538,7 +7538,7 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D288" t="n">
@@ -7563,7 +7563,7 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D289" t="n">
@@ -7588,7 +7588,7 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D290" t="n">
@@ -7613,7 +7613,7 @@
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D291" t="n">
@@ -7638,7 +7638,7 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D292" t="n">
@@ -7663,7 +7663,7 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D293" t="n">
@@ -7978,7 +7978,7 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
@@ -7988,11 +7988,11 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -8003,7 +8003,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -8013,11 +8013,11 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8028,7 +8028,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -8038,11 +8038,11 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>97</v>
+        <v>31</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8063,11 +8063,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8078,7 +8078,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>15:57:46</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8088,11 +8088,11 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>47</v>
+        <v>97</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8238,7 +8238,7 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D316" t="n">
@@ -8263,7 +8263,7 @@
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D317" t="n">
@@ -8288,7 +8288,7 @@
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D318" t="n">
@@ -8313,7 +8313,7 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D319" t="n">
@@ -8378,7 +8378,7 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
@@ -8388,11 +8388,11 @@
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D322" t="n">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -8403,7 +8403,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -8413,11 +8413,11 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -9313,7 +9313,7 @@
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D359" t="n">
@@ -9338,7 +9338,7 @@
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D360" t="n">
@@ -9403,7 +9403,7 @@
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B363" t="inlineStr">
@@ -9413,11 +9413,11 @@
       </c>
       <c r="C363" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D363" t="n">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="E363" t="inlineStr">
         <is>
@@ -9428,7 +9428,7 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
@@ -9438,11 +9438,11 @@
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D364" t="n">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
@@ -9478,7 +9478,7 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
@@ -9488,11 +9488,11 @@
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D366" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -9513,7 +9513,7 @@
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D367" t="n">
@@ -9563,7 +9563,7 @@
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D369" t="n">
@@ -9588,7 +9588,7 @@
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D370" t="n">
@@ -9603,7 +9603,7 @@
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B371" t="inlineStr">
@@ -9613,11 +9613,11 @@
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D371" t="n">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="E371" t="inlineStr">
         <is>
@@ -9628,7 +9628,7 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B372" t="inlineStr">
@@ -9642,7 +9642,7 @@
         </is>
       </c>
       <c r="D372" t="n">
-        <v>77</v>
+        <v>5</v>
       </c>
       <c r="E372" t="inlineStr">
         <is>
@@ -9653,7 +9653,7 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B373" t="inlineStr">
@@ -9667,7 +9667,7 @@
         </is>
       </c>
       <c r="D373" t="n">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="E373" t="inlineStr">
         <is>
@@ -9678,7 +9678,7 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
@@ -9692,7 +9692,7 @@
         </is>
       </c>
       <c r="D374" t="n">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="E374" t="inlineStr">
         <is>
@@ -9753,21 +9753,21 @@
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>19:35</t>
         </is>
       </c>
       <c r="C377" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D377" t="n">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="E377" t="inlineStr">
         <is>
@@ -9778,12 +9778,12 @@
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:39</t>
         </is>
       </c>
       <c r="C378" t="inlineStr">
@@ -9792,7 +9792,7 @@
         </is>
       </c>
       <c r="D378" t="n">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="E378" t="inlineStr">
         <is>
@@ -9803,7 +9803,7 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
@@ -9817,7 +9817,7 @@
         </is>
       </c>
       <c r="D379" t="n">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="E379" t="inlineStr">
         <is>
@@ -9828,21 +9828,21 @@
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>19:49</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D380" t="n">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="E380" t="inlineStr">
         <is>
@@ -9858,16 +9858,16 @@
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D381" t="n">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="E381" t="inlineStr">
         <is>
@@ -9878,21 +9878,21 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:49</t>
         </is>
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D382" t="n">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="E382" t="inlineStr">
         <is>
@@ -9903,7 +9903,7 @@
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>18:38:58</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
@@ -9913,11 +9913,11 @@
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D383" t="n">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -9928,21 +9928,21 @@
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D384" t="n">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="E384" t="inlineStr">
         <is>
@@ -9953,21 +9953,21 @@
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>19:58</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D385" t="n">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="E385" t="inlineStr">
         <is>
@@ -9978,21 +9978,21 @@
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C386" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D386" t="n">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="E386" t="inlineStr">
         <is>
@@ -10003,21 +10003,21 @@
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>18:38:58</t>
         </is>
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>19:58</t>
         </is>
       </c>
       <c r="C387" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D387" t="n">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E387" t="inlineStr">
         <is>
@@ -10028,21 +10028,21 @@
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="C388" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D388" t="n">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="E388" t="inlineStr">
         <is>
@@ -10053,21 +10053,21 @@
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>20:20</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C389" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D389" t="n">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="E389" t="inlineStr">
         <is>
@@ -10078,21 +10078,21 @@
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C390" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D390" t="n">
-        <v>103</v>
+        <v>54</v>
       </c>
       <c r="E390" t="inlineStr">
         <is>
@@ -10103,21 +10103,21 @@
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C391" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D391" t="n">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="E391" t="inlineStr">
         <is>
@@ -10128,21 +10128,21 @@
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D392" t="n">
-        <v>95</v>
+        <v>56</v>
       </c>
       <c r="E392" t="inlineStr">
         <is>
@@ -10153,23 +10153,273 @@
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B393" t="inlineStr">
         <is>
+          <t>20:20</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D393" t="n">
+        <v>64</v>
+      </c>
+      <c r="E393" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>18:38:58</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D394" t="n">
+        <v>103</v>
+      </c>
+      <c r="E394" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>19:16:50</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D395" t="n">
+        <v>66</v>
+      </c>
+      <c r="E395" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>19:16:50</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D396" t="n">
+        <v>67</v>
+      </c>
+      <c r="E396" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>19:16:50</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D397" t="n">
+        <v>74</v>
+      </c>
+      <c r="E397" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>19:16:50</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
           <t>20:46</t>
         </is>
       </c>
-      <c r="C393" t="inlineStr">
+      <c r="C398" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D393" t="n">
+      <c r="D398" t="n">
+        <v>90</v>
+      </c>
+      <c r="E398" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>19:16:50</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D399" t="n">
+        <v>96</v>
+      </c>
+      <c r="E399" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>19:16:50</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>20:55</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D400" t="n">
+        <v>99</v>
+      </c>
+      <c r="E400" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>19:16:50</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>20:56</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D401" t="n">
+        <v>100</v>
+      </c>
+      <c r="E401" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>19:16:50</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>21:04</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D402" t="n">
+        <v>108</v>
+      </c>
+      <c r="E402" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>19:16:50</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D403" t="n">
         <v>111</v>
       </c>
-      <c r="E393" t="inlineStr">
+      <c r="E403" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10186,7 +10436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10204,14 +10454,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:55:55</t>
+          <t>Última actualización: 19:16:50</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 47</t>
+          <t>Total filas: 48</t>
         </is>
       </c>
     </row>
@@ -11345,7 +11595,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -11359,7 +11609,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -11395,7 +11645,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -11409,9 +11659,34 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="E52" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>19:16:50</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>111</v>
+      </c>
+      <c r="E53" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -11428,7 +11703,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11446,14 +11721,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:55:55</t>
+          <t>Última actualización: 19:16:50</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 56</t>
+          <t>Total filas: 57</t>
         </is>
       </c>
     </row>
@@ -12812,7 +13087,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -12826,7 +13101,7 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>110</v>
+        <v>38</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -12879,6 +13154,31 @@
         <v>103</v>
       </c>
       <c r="E61" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>19:16:50</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>20:39</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>83</v>
+      </c>
+      <c r="E62" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 755
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E403"/>
+  <dimension ref="A1:E415"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:16:50</t>
+          <t>Última actualización: 19:46:58</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 398</t>
+          <t>Total filas: 410</t>
         </is>
       </c>
     </row>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1738,7 +1738,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -2203,7 +2203,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2228,7 +2228,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2238,11 +2238,11 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2513,7 +2513,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2538,7 +2538,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2853,7 +2853,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2863,11 +2863,11 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3538,7 +3538,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D128" t="n">
@@ -3563,7 +3563,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D129" t="n">
@@ -3688,7 +3688,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -3713,7 +3713,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D135" t="n">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D138" t="n">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -4553,7 +4553,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -4563,11 +4563,11 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4578,7 +4578,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>11:45:10</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -4588,11 +4588,11 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4603,7 +4603,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -4613,11 +4613,11 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4628,7 +4628,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -4638,11 +4638,11 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4778,7 +4778,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4788,11 +4788,11 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4803,7 +4803,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -4813,11 +4813,11 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4838,7 +4838,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -4888,7 +4888,7 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D182" t="n">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -5503,7 +5503,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -5513,11 +5513,11 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5578,7 +5578,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -5588,11 +5588,11 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5603,7 +5603,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -5613,11 +5613,11 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -5628,7 +5628,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
@@ -5638,11 +5638,11 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D212" t="n">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -5653,7 +5653,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5663,11 +5663,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -5863,7 +5863,7 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D221" t="n">
@@ -6913,7 +6913,7 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D263" t="n">
@@ -6938,7 +6938,7 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D264" t="n">
@@ -7263,7 +7263,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D277" t="n">
@@ -7288,7 +7288,7 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D278" t="n">
@@ -7538,7 +7538,7 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D288" t="n">
@@ -7563,7 +7563,7 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D289" t="n">
@@ -7588,7 +7588,7 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D290" t="n">
@@ -7813,7 +7813,7 @@
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D299" t="n">
@@ -7838,7 +7838,7 @@
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D300" t="n">
@@ -8028,7 +8028,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -8038,11 +8038,11 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8063,11 +8063,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8238,7 +8238,7 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D316" t="n">
@@ -8263,7 +8263,7 @@
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D317" t="n">
@@ -8288,7 +8288,7 @@
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D318" t="n">
@@ -8313,7 +8313,7 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D319" t="n">
@@ -8503,7 +8503,7 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
@@ -8513,11 +8513,11 @@
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -8528,7 +8528,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -8538,11 +8538,11 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8603,7 +8603,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
@@ -8613,11 +8613,11 @@
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8628,7 +8628,7 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
@@ -8638,11 +8638,11 @@
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -8763,7 +8763,7 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D337" t="n">
@@ -8788,7 +8788,7 @@
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D338" t="n">
@@ -9563,7 +9563,7 @@
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D369" t="n">
@@ -9578,7 +9578,7 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B370" t="inlineStr">
@@ -9588,11 +9588,11 @@
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D370" t="n">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="E370" t="inlineStr">
         <is>
@@ -9603,7 +9603,7 @@
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B371" t="inlineStr">
@@ -9613,11 +9613,11 @@
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D371" t="n">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="E371" t="inlineStr">
         <is>
@@ -9678,7 +9678,7 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
@@ -9688,11 +9688,11 @@
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D374" t="n">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="E374" t="inlineStr">
         <is>
@@ -9703,7 +9703,7 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B375" t="inlineStr">
@@ -9713,11 +9713,11 @@
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D375" t="n">
-        <v>86</v>
+        <v>14</v>
       </c>
       <c r="E375" t="inlineStr">
         <is>
@@ -9803,7 +9803,7 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
@@ -9813,11 +9813,11 @@
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D379" t="n">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="E379" t="inlineStr">
         <is>
@@ -9838,7 +9838,7 @@
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D380" t="n">
@@ -9853,7 +9853,7 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
@@ -9863,11 +9863,11 @@
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D381" t="n">
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="E381" t="inlineStr">
         <is>
@@ -9878,21 +9878,21 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>19:49</t>
+          <t>19:46</t>
         </is>
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D382" t="n">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="E382" t="inlineStr">
         <is>
@@ -9903,21 +9903,21 @@
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:49</t>
         </is>
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D383" t="n">
-        <v>72</v>
+        <v>3</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -9928,7 +9928,7 @@
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B384" t="inlineStr">
@@ -9938,11 +9938,11 @@
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D384" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="E384" t="inlineStr">
         <is>
@@ -9953,7 +9953,7 @@
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B385" t="inlineStr">
@@ -9967,7 +9967,7 @@
         </is>
       </c>
       <c r="D385" t="n">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="E385" t="inlineStr">
         <is>
@@ -9983,16 +9983,16 @@
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C386" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D386" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E386" t="inlineStr">
         <is>
@@ -10003,21 +10003,21 @@
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>19:58</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C387" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D387" t="n">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="E387" t="inlineStr">
         <is>
@@ -10028,12 +10028,12 @@
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:58</t>
         </is>
       </c>
       <c r="C388" t="inlineStr">
@@ -10042,7 +10042,7 @@
         </is>
       </c>
       <c r="D388" t="n">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="E388" t="inlineStr">
         <is>
@@ -10058,16 +10058,16 @@
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="C389" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D389" t="n">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E389" t="inlineStr">
         <is>
@@ -10078,21 +10078,21 @@
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="C390" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D390" t="n">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="E390" t="inlineStr">
         <is>
@@ -10103,21 +10103,21 @@
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="C391" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D391" t="n">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="E391" t="inlineStr">
         <is>
@@ -10128,21 +10128,21 @@
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>20:08</t>
         </is>
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D392" t="n">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="E392" t="inlineStr">
         <is>
@@ -10158,16 +10158,16 @@
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>20:20</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D393" t="n">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E393" t="inlineStr">
         <is>
@@ -10178,21 +10178,21 @@
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C394" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D394" t="n">
-        <v>103</v>
+        <v>24</v>
       </c>
       <c r="E394" t="inlineStr">
         <is>
@@ -10203,21 +10203,21 @@
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C395" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D395" t="n">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="E395" t="inlineStr">
         <is>
@@ -10233,16 +10233,16 @@
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D396" t="n">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="E396" t="inlineStr">
         <is>
@@ -10253,21 +10253,21 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D397" t="n">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="E397" t="inlineStr">
         <is>
@@ -10278,21 +10278,21 @@
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>20:46</t>
+          <t>20:15</t>
         </is>
       </c>
       <c r="C398" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D398" t="n">
-        <v>90</v>
+        <v>29</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -10303,21 +10303,21 @@
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>20:20</t>
         </is>
       </c>
       <c r="C399" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D399" t="n">
-        <v>96</v>
+        <v>34</v>
       </c>
       <c r="E399" t="inlineStr">
         <is>
@@ -10328,21 +10328,21 @@
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>20:55</t>
+          <t>20:21</t>
         </is>
       </c>
       <c r="C400" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D400" t="n">
-        <v>99</v>
+        <v>35</v>
       </c>
       <c r="E400" t="inlineStr">
         <is>
@@ -10358,16 +10358,16 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="C401" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D401" t="n">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="E401" t="inlineStr">
         <is>
@@ -10378,21 +10378,21 @@
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>20:23</t>
         </is>
       </c>
       <c r="C402" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D402" t="n">
-        <v>108</v>
+        <v>37</v>
       </c>
       <c r="E402" t="inlineStr">
         <is>
@@ -10403,23 +10403,323 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
+          <t>19:46:58</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D403" t="n">
+        <v>44</v>
+      </c>
+      <c r="E403" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>19:46:58</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>20:43</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D404" t="n">
+        <v>57</v>
+      </c>
+      <c r="E404" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
           <t>19:16:50</t>
         </is>
       </c>
-      <c r="B403" t="inlineStr">
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>20:46</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D405" t="n">
+        <v>90</v>
+      </c>
+      <c r="E405" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>19:46:58</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>20:51</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D406" t="n">
+        <v>65</v>
+      </c>
+      <c r="E406" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>19:16:50</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D407" t="n">
+        <v>96</v>
+      </c>
+      <c r="E407" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>19:46:58</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>20:55</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D408" t="n">
+        <v>69</v>
+      </c>
+      <c r="E408" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>19:46:58</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>20:56</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D409" t="n">
+        <v>70</v>
+      </c>
+      <c r="E409" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>19:46:58</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>21:03</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D410" t="n">
+        <v>77</v>
+      </c>
+      <c r="E410" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>19:16:50</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>21:04</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D411" t="n">
+        <v>108</v>
+      </c>
+      <c r="E411" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>19:46:58</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
         <is>
           <t>21:07</t>
         </is>
       </c>
-      <c r="C403" t="inlineStr">
+      <c r="C412" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D403" t="n">
+      <c r="D412" t="n">
+        <v>81</v>
+      </c>
+      <c r="E412" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>19:46:58</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D413" t="n">
+        <v>94</v>
+      </c>
+      <c r="E413" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>19:46:58</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>21:37</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D414" t="n">
         <v>111</v>
       </c>
-      <c r="E403" t="inlineStr">
+      <c r="E414" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>19:46:58</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>21:37</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D415" t="n">
+        <v>111</v>
+      </c>
+      <c r="E415" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10454,7 +10754,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:16:50</t>
+          <t>Última actualización: 19:46:58</t>
         </is>
       </c>
     </row>
@@ -11645,7 +11945,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -11659,7 +11959,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -11670,7 +11970,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -11684,7 +11984,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -11703,7 +12003,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11721,14 +12021,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:16:50</t>
+          <t>Última actualización: 19:46:58</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 57</t>
+          <t>Total filas: 59</t>
         </is>
       </c>
     </row>
@@ -13112,12 +13412,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>18:38:58</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>19:58</t>
+          <t>19:56</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -13126,7 +13426,7 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -13137,50 +13437,100 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>18:38:58</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>20:38</t>
+          <t>19:58</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
+          <t>19:46:58</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>20:38</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>52</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
           <t>19:16:50</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr">
+      <c r="B63" t="inlineStr">
         <is>
           <t>20:39</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
+      <c r="C63" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D62" t="n">
+      <c r="D63" t="n">
         <v>83</v>
       </c>
-      <c r="E62" t="inlineStr">
+      <c r="E63" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>19:46:58</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>21:28</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>102</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 756
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E415"/>
+  <dimension ref="A1:E431"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:46:58</t>
+          <t>Última actualización: 20:01:28</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 410</t>
+          <t>Total filas: 426</t>
         </is>
       </c>
     </row>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2513,7 +2513,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2538,7 +2538,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -2788,7 +2788,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D98" t="n">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -2828,7 +2828,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2838,11 +2838,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2853,7 +2853,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2863,11 +2863,11 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2878,7 +2878,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2888,11 +2888,11 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -3688,7 +3688,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -3713,7 +3713,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D135" t="n">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D138" t="n">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -5578,7 +5578,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -5588,11 +5588,11 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5603,7 +5603,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -5613,11 +5613,11 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -6063,7 +6063,7 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D229" t="n">
@@ -6088,7 +6088,7 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D230" t="n">
@@ -6753,7 +6753,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -6763,11 +6763,11 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6778,7 +6778,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -6788,11 +6788,11 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -7353,7 +7353,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -7363,11 +7363,11 @@
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7378,7 +7378,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
@@ -7388,11 +7388,11 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -7538,7 +7538,7 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D288" t="n">
@@ -7563,7 +7563,7 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D289" t="n">
@@ -7588,7 +7588,7 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D290" t="n">
@@ -7613,7 +7613,7 @@
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D291" t="n">
@@ -7638,7 +7638,7 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D292" t="n">
@@ -7663,7 +7663,7 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D293" t="n">
@@ -7978,7 +7978,7 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
@@ -7988,11 +7988,11 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -8003,7 +8003,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -8013,11 +8013,11 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>15:57:46</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8063,11 +8063,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>31</v>
+        <v>97</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8078,7 +8078,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8088,11 +8088,11 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>97</v>
+        <v>31</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8378,7 +8378,7 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
@@ -8388,11 +8388,11 @@
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D322" t="n">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -8403,7 +8403,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -8413,11 +8413,11 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8763,7 +8763,7 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D337" t="n">
@@ -8788,7 +8788,7 @@
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D338" t="n">
@@ -9403,7 +9403,7 @@
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B363" t="inlineStr">
@@ -9413,11 +9413,11 @@
       </c>
       <c r="C363" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D363" t="n">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="E363" t="inlineStr">
         <is>
@@ -9428,7 +9428,7 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
@@ -9438,11 +9438,11 @@
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D364" t="n">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
@@ -9553,7 +9553,7 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B369" t="inlineStr">
@@ -9563,11 +9563,11 @@
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D369" t="n">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="E369" t="inlineStr">
         <is>
@@ -9578,7 +9578,7 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B370" t="inlineStr">
@@ -9588,11 +9588,11 @@
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D370" t="n">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="E370" t="inlineStr">
         <is>
@@ -9613,7 +9613,7 @@
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D371" t="n">
@@ -9678,7 +9678,7 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
@@ -9688,11 +9688,11 @@
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D374" t="n">
-        <v>86</v>
+        <v>14</v>
       </c>
       <c r="E374" t="inlineStr">
         <is>
@@ -9703,7 +9703,7 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B375" t="inlineStr">
@@ -9713,11 +9713,11 @@
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D375" t="n">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="E375" t="inlineStr">
         <is>
@@ -10128,21 +10128,21 @@
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>20:08</t>
+          <t>20:01</t>
         </is>
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D392" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="E392" t="inlineStr">
         <is>
@@ -10153,21 +10153,21 @@
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>20:01</t>
         </is>
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D393" t="n">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="E393" t="inlineStr">
         <is>
@@ -10183,16 +10183,16 @@
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:08</t>
         </is>
       </c>
       <c r="C394" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D394" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E394" t="inlineStr">
         <is>
@@ -10203,21 +10203,21 @@
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C395" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D395" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E395" t="inlineStr">
         <is>
@@ -10228,21 +10228,21 @@
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D396" t="n">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="E396" t="inlineStr">
         <is>
@@ -10253,21 +10253,21 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D397" t="n">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="E397" t="inlineStr">
         <is>
@@ -10278,21 +10278,21 @@
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>20:15</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="C398" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D398" t="n">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -10303,21 +10303,21 @@
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>20:20</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C399" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D399" t="n">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="E399" t="inlineStr">
         <is>
@@ -10333,16 +10333,16 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="C400" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D400" t="n">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E400" t="inlineStr">
         <is>
@@ -10353,21 +10353,21 @@
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:15</t>
         </is>
       </c>
       <c r="C401" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D401" t="n">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="E401" t="inlineStr">
         <is>
@@ -10383,16 +10383,16 @@
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>20:20</t>
         </is>
       </c>
       <c r="C402" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D402" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E402" t="inlineStr">
         <is>
@@ -10403,21 +10403,21 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>20:21</t>
         </is>
       </c>
       <c r="C403" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D403" t="n">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -10433,7 +10433,7 @@
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>20:43</t>
+          <t>20:21</t>
         </is>
       </c>
       <c r="C404" t="inlineStr">
@@ -10442,7 +10442,7 @@
         </is>
       </c>
       <c r="D404" t="n">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="E404" t="inlineStr">
         <is>
@@ -10453,21 +10453,21 @@
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>20:46</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="C405" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D405" t="n">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="E405" t="inlineStr">
         <is>
@@ -10478,21 +10478,21 @@
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>20:51</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="C406" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D406" t="n">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="E406" t="inlineStr">
         <is>
@@ -10503,21 +10503,21 @@
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>20:23</t>
         </is>
       </c>
       <c r="C407" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D407" t="n">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="E407" t="inlineStr">
         <is>
@@ -10533,16 +10533,16 @@
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>20:55</t>
+          <t>20:30</t>
         </is>
       </c>
       <c r="C408" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D408" t="n">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="E408" t="inlineStr">
         <is>
@@ -10553,21 +10553,21 @@
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:31</t>
         </is>
       </c>
       <c r="C409" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D409" t="n">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="E409" t="inlineStr">
         <is>
@@ -10583,16 +10583,16 @@
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>21:03</t>
+          <t>20:43</t>
         </is>
       </c>
       <c r="C410" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D410" t="n">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="E410" t="inlineStr">
         <is>
@@ -10603,21 +10603,21 @@
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="C411" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D411" t="n">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="E411" t="inlineStr">
         <is>
@@ -10628,21 +10628,21 @@
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B412" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="C412" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D412" t="n">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="E412" t="inlineStr">
         <is>
@@ -10653,21 +10653,21 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B413" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>20:46</t>
         </is>
       </c>
       <c r="C413" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D413" t="n">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -10683,16 +10683,16 @@
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>20:51</t>
         </is>
       </c>
       <c r="C414" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D414" t="n">
-        <v>111</v>
+        <v>65</v>
       </c>
       <c r="E414" t="inlineStr">
         <is>
@@ -10703,23 +10703,423 @@
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
+          <t>20:01:28</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D415" t="n">
+        <v>51</v>
+      </c>
+      <c r="E415" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>20:01:28</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D416" t="n">
+        <v>51</v>
+      </c>
+      <c r="E416" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
           <t>19:46:58</t>
         </is>
       </c>
-      <c r="B415" t="inlineStr">
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>20:55</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D417" t="n">
+        <v>69</v>
+      </c>
+      <c r="E417" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>19:46:58</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>20:56</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D418" t="n">
+        <v>70</v>
+      </c>
+      <c r="E418" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>20:01:28</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>20:57</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D419" t="n">
+        <v>56</v>
+      </c>
+      <c r="E419" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>19:46:58</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>21:03</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D420" t="n">
+        <v>77</v>
+      </c>
+      <c r="E420" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>20:01:28</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>21:04</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D421" t="n">
+        <v>63</v>
+      </c>
+      <c r="E421" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>19:46:58</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D422" t="n">
+        <v>81</v>
+      </c>
+      <c r="E422" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>20:01:28</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>21:08</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D423" t="n">
+        <v>67</v>
+      </c>
+      <c r="E423" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>19:46:58</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D424" t="n">
+        <v>94</v>
+      </c>
+      <c r="E424" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>20:01:28</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D425" t="n">
+        <v>80</v>
+      </c>
+      <c r="E425" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>20:01:28</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>21:23</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D426" t="n">
+        <v>82</v>
+      </c>
+      <c r="E426" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>19:46:58</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
         <is>
           <t>21:37</t>
         </is>
       </c>
-      <c r="C415" t="inlineStr">
+      <c r="C427" t="inlineStr">
         <is>
           <t>17_ROMERO</t>
         </is>
       </c>
-      <c r="D415" t="n">
+      <c r="D427" t="n">
         <v>111</v>
       </c>
-      <c r="E415" t="inlineStr">
+      <c r="E427" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>19:46:58</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>21:37</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D428" t="n">
+        <v>111</v>
+      </c>
+      <c r="E428" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>20:01:28</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D429" t="n">
+        <v>97</v>
+      </c>
+      <c r="E429" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>20:01:28</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D430" t="n">
+        <v>97</v>
+      </c>
+      <c r="E430" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>20:01:28</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D431" t="n">
+        <v>106</v>
+      </c>
+      <c r="E431" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10736,7 +11136,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10754,14 +11154,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:46:58</t>
+          <t>Última actualización: 20:01:28</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 48</t>
+          <t>Total filas: 50</t>
         </is>
       </c>
     </row>
@@ -11945,7 +12345,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -11959,7 +12359,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -11987,6 +12387,56 @@
         <v>81</v>
       </c>
       <c r="E53" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>20:01:28</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>21:08</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>67</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>20:01:28</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>106</v>
+      </c>
+      <c r="E55" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -12003,7 +12453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12021,14 +12471,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:46:58</t>
+          <t>Última actualización: 20:01:28</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 59</t>
+          <t>Total filas: 60</t>
         </is>
       </c>
     </row>
@@ -13487,7 +13937,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -13501,7 +13951,7 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -13529,6 +13979,31 @@
         <v>102</v>
       </c>
       <c r="E64" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>20:01:28</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>88</v>
+      </c>
+      <c r="E65" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 757
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E431"/>
+  <dimension ref="A1:E441"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:01:28</t>
+          <t>Última actualización: 20:35:32</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 426</t>
+          <t>Total filas: 436</t>
         </is>
       </c>
     </row>
@@ -2513,7 +2513,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2538,7 +2538,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -2788,7 +2788,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D98" t="n">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -2878,7 +2878,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>08:52:26</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2888,11 +2888,11 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:52:26</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2913,11 +2913,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -3828,7 +3828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3838,11 +3838,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,7 +3853,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3863,11 +3863,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>94</v>
+        <v>2</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4638,7 +4638,7 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D172" t="n">
@@ -4663,7 +4663,7 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D173" t="n">
@@ -4778,7 +4778,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4788,11 +4788,11 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4803,7 +4803,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -4813,11 +4813,11 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -5238,7 +5238,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D196" t="n">
@@ -5263,7 +5263,7 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D197" t="n">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5938,11 +5938,11 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5953,7 +5953,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -5963,11 +5963,11 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>112</v>
+        <v>53</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,7 +6378,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6388,11 +6388,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6753,7 +6753,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -6763,11 +6763,11 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6778,7 +6778,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -6788,11 +6788,11 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -6913,7 +6913,7 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D263" t="n">
@@ -6938,7 +6938,7 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D264" t="n">
@@ -7263,7 +7263,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D277" t="n">
@@ -7288,7 +7288,7 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D278" t="n">
@@ -7563,7 +7563,7 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D289" t="n">
@@ -7588,7 +7588,7 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D290" t="n">
@@ -7613,7 +7613,7 @@
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D291" t="n">
@@ -7638,7 +7638,7 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D292" t="n">
@@ -7978,7 +7978,7 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
@@ -7988,11 +7988,11 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -8003,7 +8003,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -8013,11 +8013,11 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8028,7 +8028,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -8038,11 +8038,11 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8078,7 +8078,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8088,11 +8088,11 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8288,7 +8288,7 @@
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D318" t="n">
@@ -8313,7 +8313,7 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D319" t="n">
@@ -8503,7 +8503,7 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
@@ -8513,11 +8513,11 @@
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -8528,7 +8528,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -8538,11 +8538,11 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8603,7 +8603,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
@@ -8613,11 +8613,11 @@
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8628,7 +8628,7 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
@@ -8638,11 +8638,11 @@
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -9038,7 +9038,7 @@
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D348" t="n">
@@ -9063,7 +9063,7 @@
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D349" t="n">
@@ -9313,7 +9313,7 @@
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D359" t="n">
@@ -9338,7 +9338,7 @@
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D360" t="n">
@@ -9553,7 +9553,7 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B369" t="inlineStr">
@@ -9563,11 +9563,11 @@
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D369" t="n">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="E369" t="inlineStr">
         <is>
@@ -9578,7 +9578,7 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B370" t="inlineStr">
@@ -9588,11 +9588,11 @@
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D370" t="n">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="E370" t="inlineStr">
         <is>
@@ -9613,7 +9613,7 @@
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D371" t="n">
@@ -9803,7 +9803,7 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
@@ -9813,11 +9813,11 @@
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D379" t="n">
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="E379" t="inlineStr">
         <is>
@@ -9853,7 +9853,7 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
@@ -9863,11 +9863,11 @@
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D381" t="n">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="E381" t="inlineStr">
         <is>
@@ -9938,7 +9938,7 @@
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D384" t="n">
@@ -9953,7 +9953,7 @@
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B385" t="inlineStr">
@@ -9963,11 +9963,11 @@
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D385" t="n">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="E385" t="inlineStr">
         <is>
@@ -9978,7 +9978,7 @@
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B386" t="inlineStr">
@@ -9988,11 +9988,11 @@
       </c>
       <c r="C386" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D386" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="E386" t="inlineStr">
         <is>
@@ -10138,7 +10138,7 @@
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D392" t="n">
@@ -10163,7 +10163,7 @@
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D393" t="n">
@@ -10228,7 +10228,7 @@
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B396" t="inlineStr">
@@ -10238,11 +10238,11 @@
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D396" t="n">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E396" t="inlineStr">
         <is>
@@ -10253,7 +10253,7 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
@@ -10263,11 +10263,11 @@
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D397" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E397" t="inlineStr">
         <is>
@@ -10403,7 +10403,7 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B403" t="inlineStr">
@@ -10413,11 +10413,11 @@
       </c>
       <c r="C403" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D403" t="n">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -10428,7 +10428,7 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
@@ -10438,11 +10438,11 @@
       </c>
       <c r="C404" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D404" t="n">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="E404" t="inlineStr">
         <is>
@@ -10463,7 +10463,7 @@
       </c>
       <c r="C405" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D405" t="n">
@@ -10488,7 +10488,7 @@
       </c>
       <c r="C406" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D406" t="n">
@@ -10578,21 +10578,21 @@
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:35:32</t>
         </is>
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>20:43</t>
+          <t>20:35</t>
         </is>
       </c>
       <c r="C410" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D410" t="n">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="E410" t="inlineStr">
         <is>
@@ -10603,21 +10603,21 @@
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>20:43</t>
         </is>
       </c>
       <c r="C411" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D411" t="n">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="E411" t="inlineStr">
         <is>
@@ -10628,7 +10628,7 @@
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>20:35:32</t>
         </is>
       </c>
       <c r="B412" t="inlineStr">
@@ -10642,7 +10642,7 @@
         </is>
       </c>
       <c r="D412" t="n">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="E412" t="inlineStr">
         <is>
@@ -10653,21 +10653,21 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B413" t="inlineStr">
         <is>
-          <t>20:46</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="C413" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D413" t="n">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -10678,21 +10678,21 @@
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>20:51</t>
+          <t>20:46</t>
         </is>
       </c>
       <c r="C414" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D414" t="n">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="E414" t="inlineStr">
         <is>
@@ -10703,21 +10703,21 @@
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>20:35:32</t>
         </is>
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>20:46</t>
         </is>
       </c>
       <c r="C415" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D415" t="n">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="E415" t="inlineStr">
         <is>
@@ -10728,12 +10728,12 @@
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B416" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>20:51</t>
         </is>
       </c>
       <c r="C416" t="inlineStr">
@@ -10742,7 +10742,7 @@
         </is>
       </c>
       <c r="D416" t="n">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="E416" t="inlineStr">
         <is>
@@ -10753,21 +10753,21 @@
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:35:32</t>
         </is>
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>20:55</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="C417" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D417" t="n">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="E417" t="inlineStr">
         <is>
@@ -10778,21 +10778,21 @@
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:35:32</t>
         </is>
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="C418" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D418" t="n">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="E418" t="inlineStr">
         <is>
@@ -10803,21 +10803,21 @@
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>20:55</t>
         </is>
       </c>
       <c r="C419" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D419" t="n">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="E419" t="inlineStr">
         <is>
@@ -10828,21 +10828,21 @@
     <row r="420">
       <c r="A420" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:35:32</t>
         </is>
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>21:03</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C420" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D420" t="n">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="E420" t="inlineStr">
         <is>
@@ -10858,16 +10858,16 @@
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C421" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D421" t="n">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E421" t="inlineStr">
         <is>
@@ -10883,16 +10883,16 @@
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>21:03</t>
         </is>
       </c>
       <c r="C422" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D422" t="n">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E422" t="inlineStr">
         <is>
@@ -10903,21 +10903,21 @@
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>20:35:32</t>
         </is>
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="C423" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D423" t="n">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="E423" t="inlineStr">
         <is>
@@ -10928,21 +10928,21 @@
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:35:32</t>
         </is>
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="C424" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D424" t="n">
-        <v>94</v>
+        <v>32</v>
       </c>
       <c r="E424" t="inlineStr">
         <is>
@@ -10958,16 +10958,16 @@
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="C425" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D425" t="n">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="E425" t="inlineStr">
         <is>
@@ -10978,21 +10978,21 @@
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>20:35:32</t>
         </is>
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="C426" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D426" t="n">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="E426" t="inlineStr">
         <is>
@@ -11003,21 +11003,21 @@
     <row r="427">
       <c r="A427" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="C427" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D427" t="n">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="E427" t="inlineStr">
         <is>
@@ -11028,21 +11028,21 @@
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:35:32</t>
         </is>
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="C428" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D428" t="n">
-        <v>111</v>
+        <v>47</v>
       </c>
       <c r="E428" t="inlineStr">
         <is>
@@ -11053,21 +11053,21 @@
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>20:35:32</t>
         </is>
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="C429" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D429" t="n">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="E429" t="inlineStr">
         <is>
@@ -11083,16 +11083,16 @@
       </c>
       <c r="B430" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="C430" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D430" t="n">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="E430" t="inlineStr">
         <is>
@@ -11103,23 +11103,273 @@
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
+          <t>20:35:32</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>21:34</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D431" t="n">
+        <v>59</v>
+      </c>
+      <c r="E431" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>19:46:58</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>21:37</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D432" t="n">
+        <v>111</v>
+      </c>
+      <c r="E432" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>20:35:32</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>21:37</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D433" t="n">
+        <v>62</v>
+      </c>
+      <c r="E433" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>20:35:32</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D434" t="n">
+        <v>63</v>
+      </c>
+      <c r="E434" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
           <t>20:01:28</t>
         </is>
       </c>
-      <c r="B431" t="inlineStr">
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D435" t="n">
+        <v>97</v>
+      </c>
+      <c r="E435" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>20:35:32</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
         <is>
           <t>21:47</t>
         </is>
       </c>
-      <c r="C431" t="inlineStr">
+      <c r="C436" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D431" t="n">
-        <v>106</v>
-      </c>
-      <c r="E431" t="inlineStr">
+      <c r="D436" t="n">
+        <v>72</v>
+      </c>
+      <c r="E436" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>20:35:32</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>21:52</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D437" t="n">
+        <v>77</v>
+      </c>
+      <c r="E437" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>20:35:32</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>22:07</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D438" t="n">
+        <v>92</v>
+      </c>
+      <c r="E438" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>20:35:32</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>22:08</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D439" t="n">
+        <v>93</v>
+      </c>
+      <c r="E439" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>20:35:32</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>22:18</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D440" t="n">
+        <v>103</v>
+      </c>
+      <c r="E440" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>20:35:32</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>22:27</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D441" t="n">
+        <v>112</v>
+      </c>
+      <c r="E441" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -11154,7 +11404,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:01:28</t>
+          <t>Última actualización: 20:35:32</t>
         </is>
       </c>
     </row>
@@ -12370,7 +12620,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:35:32</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -12384,7 +12634,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -12420,7 +12670,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>20:35:32</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -12434,7 +12684,7 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -12453,7 +12703,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12471,14 +12721,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:01:28</t>
+          <t>Última actualización: 20:35:32</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 60</t>
+          <t>Total filas: 62</t>
         </is>
       </c>
     </row>
@@ -13937,7 +14187,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>20:35:32</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -13951,7 +14201,7 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -13987,7 +14237,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>20:35:32</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -14001,11 +14251,61 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>20:35:32</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>22:05</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>90</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>20:35:32</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>22:20</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>105</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 758
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E441"/>
+  <dimension ref="A1:E454"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:35:32</t>
+          <t>Última actualización: 20:52:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 436</t>
+          <t>Total filas: 449</t>
         </is>
       </c>
     </row>
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1738,7 +1738,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2788,7 +2788,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D98" t="n">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -3828,7 +3828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3838,11 +3838,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>94</v>
+        <v>2</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3853,7 +3853,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3863,11 +3863,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4603,7 +4603,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -4613,11 +4613,11 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4653,7 +4653,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -4663,11 +4663,11 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4778,7 +4778,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4788,11 +4788,11 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4813,7 +4813,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D179" t="n">
@@ -4838,7 +4838,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D180" t="n">
@@ -4888,7 +4888,7 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D182" t="n">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -5503,7 +5503,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -5513,11 +5513,11 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5528,7 +5528,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -5538,11 +5538,11 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5578,7 +5578,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -5588,11 +5588,11 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5603,7 +5603,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -5613,11 +5613,11 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -5628,7 +5628,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>12:44:48</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
@@ -5638,11 +5638,11 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D212" t="n">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -5653,7 +5653,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:44:48</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5663,11 +5663,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -5863,7 +5863,7 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D221" t="n">
@@ -5928,7 +5928,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>13:03:48</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -5938,11 +5938,11 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>112</v>
+        <v>53</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5953,7 +5953,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>13:03:48</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -5963,11 +5963,11 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,7 +6378,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6388,11 +6388,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -7353,7 +7353,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -7363,11 +7363,11 @@
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7378,7 +7378,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
@@ -7388,11 +7388,11 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -7403,7 +7403,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -7413,11 +7413,11 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7428,7 +7428,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
@@ -7438,11 +7438,11 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7538,7 +7538,7 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D288" t="n">
@@ -7563,7 +7563,7 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D289" t="n">
@@ -7613,7 +7613,7 @@
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D291" t="n">
@@ -7638,7 +7638,7 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D292" t="n">
@@ -7663,7 +7663,7 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D293" t="n">
@@ -7813,7 +7813,7 @@
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D299" t="n">
@@ -7838,7 +7838,7 @@
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D300" t="n">
@@ -7978,7 +7978,7 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
@@ -7988,11 +7988,11 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -8003,7 +8003,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -8013,11 +8013,11 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8028,7 +8028,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -8038,11 +8038,11 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8053,7 +8053,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8063,11 +8063,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>97</v>
+        <v>31</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8078,7 +8078,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>15:57:46</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8088,11 +8088,11 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>47</v>
+        <v>97</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8378,7 +8378,7 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
@@ -8388,11 +8388,11 @@
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D322" t="n">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -8403,7 +8403,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -8413,11 +8413,11 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8603,7 +8603,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
@@ -8613,11 +8613,11 @@
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8628,7 +8628,7 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
@@ -8638,11 +8638,11 @@
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -9563,7 +9563,7 @@
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D369" t="n">
@@ -9578,7 +9578,7 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B370" t="inlineStr">
@@ -9588,11 +9588,11 @@
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D370" t="n">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="E370" t="inlineStr">
         <is>
@@ -9603,7 +9603,7 @@
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B371" t="inlineStr">
@@ -9613,11 +9613,11 @@
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D371" t="n">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="E371" t="inlineStr">
         <is>
@@ -9803,7 +9803,7 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
@@ -9813,11 +9813,11 @@
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D379" t="n">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="E379" t="inlineStr">
         <is>
@@ -9838,7 +9838,7 @@
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D380" t="n">
@@ -9853,7 +9853,7 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
@@ -9863,11 +9863,11 @@
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D381" t="n">
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="E381" t="inlineStr">
         <is>
@@ -9928,7 +9928,7 @@
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B384" t="inlineStr">
@@ -9938,11 +9938,11 @@
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D384" t="n">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="E384" t="inlineStr">
         <is>
@@ -9953,7 +9953,7 @@
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B385" t="inlineStr">
@@ -9963,11 +9963,11 @@
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D385" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="E385" t="inlineStr">
         <is>
@@ -9988,7 +9988,7 @@
       </c>
       <c r="C386" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D386" t="n">
@@ -10138,7 +10138,7 @@
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D392" t="n">
@@ -10163,7 +10163,7 @@
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D393" t="n">
@@ -10228,7 +10228,7 @@
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B396" t="inlineStr">
@@ -10238,11 +10238,11 @@
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D396" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E396" t="inlineStr">
         <is>
@@ -10253,7 +10253,7 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
@@ -10263,11 +10263,11 @@
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D397" t="n">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E397" t="inlineStr">
         <is>
@@ -10403,7 +10403,7 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B403" t="inlineStr">
@@ -10413,11 +10413,11 @@
       </c>
       <c r="C403" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D403" t="n">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -10428,7 +10428,7 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
@@ -10438,11 +10438,11 @@
       </c>
       <c r="C404" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D404" t="n">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E404" t="inlineStr">
         <is>
@@ -10628,7 +10628,7 @@
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>20:35:32</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B412" t="inlineStr">
@@ -10638,11 +10638,11 @@
       </c>
       <c r="C412" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D412" t="n">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="E412" t="inlineStr">
         <is>
@@ -10653,7 +10653,7 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>20:35:32</t>
         </is>
       </c>
       <c r="B413" t="inlineStr">
@@ -10663,11 +10663,11 @@
       </c>
       <c r="C413" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D413" t="n">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -10753,7 +10753,7 @@
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>20:35:32</t>
+          <t>20:52:15</t>
         </is>
       </c>
       <c r="B417" t="inlineStr">
@@ -10763,11 +10763,11 @@
       </c>
       <c r="C417" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D417" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E417" t="inlineStr">
         <is>
@@ -10778,7 +10778,7 @@
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>20:35:32</t>
+          <t>20:52:15</t>
         </is>
       </c>
       <c r="B418" t="inlineStr">
@@ -10792,7 +10792,7 @@
         </is>
       </c>
       <c r="D418" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E418" t="inlineStr">
         <is>
@@ -10803,21 +10803,21 @@
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:52:15</t>
         </is>
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>20:55</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="C419" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D419" t="n">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="E419" t="inlineStr">
         <is>
@@ -10828,21 +10828,21 @@
     <row r="420">
       <c r="A420" t="inlineStr">
         <is>
-          <t>20:35:32</t>
+          <t>20:52:15</t>
         </is>
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:53</t>
         </is>
       </c>
       <c r="C420" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D420" t="n">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="E420" t="inlineStr">
         <is>
@@ -10853,21 +10853,21 @@
     <row r="421">
       <c r="A421" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>20:52:15</t>
         </is>
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>20:53</t>
         </is>
       </c>
       <c r="C421" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D421" t="n">
-        <v>56</v>
+        <v>1</v>
       </c>
       <c r="E421" t="inlineStr">
         <is>
@@ -10883,16 +10883,16 @@
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>21:03</t>
+          <t>20:55</t>
         </is>
       </c>
       <c r="C422" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D422" t="n">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E422" t="inlineStr">
         <is>
@@ -10903,21 +10903,21 @@
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t>20:35:32</t>
+          <t>20:52:15</t>
         </is>
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C423" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D423" t="n">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="E423" t="inlineStr">
         <is>
@@ -10933,16 +10933,16 @@
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C424" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D424" t="n">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E424" t="inlineStr">
         <is>
@@ -10953,21 +10953,21 @@
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>20:52:15</t>
         </is>
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C425" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D425" t="n">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="E425" t="inlineStr">
         <is>
@@ -10978,21 +10978,21 @@
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t>20:35:32</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:03</t>
         </is>
       </c>
       <c r="C426" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D426" t="n">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="E426" t="inlineStr">
         <is>
@@ -11003,21 +11003,21 @@
     <row r="427">
       <c r="A427" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>20:52:15</t>
         </is>
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="C427" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D427" t="n">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="E427" t="inlineStr">
         <is>
@@ -11033,16 +11033,16 @@
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>21:22</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="C428" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D428" t="n">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="E428" t="inlineStr">
         <is>
@@ -11053,21 +11053,21 @@
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>20:35:32</t>
+          <t>20:52:15</t>
         </is>
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>21:22</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="C429" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D429" t="n">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="E429" t="inlineStr">
         <is>
@@ -11078,21 +11078,21 @@
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>20:35:32</t>
         </is>
       </c>
       <c r="B430" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="C430" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D430" t="n">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="E430" t="inlineStr">
         <is>
@@ -11103,21 +11103,21 @@
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>20:35:32</t>
+          <t>20:52:15</t>
         </is>
       </c>
       <c r="B431" t="inlineStr">
         <is>
-          <t>21:34</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="C431" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D431" t="n">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="E431" t="inlineStr">
         <is>
@@ -11128,21 +11128,21 @@
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:35:32</t>
         </is>
       </c>
       <c r="B432" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="C432" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D432" t="n">
-        <v>111</v>
+        <v>47</v>
       </c>
       <c r="E432" t="inlineStr">
         <is>
@@ -11158,16 +11158,16 @@
       </c>
       <c r="B433" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="C433" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D433" t="n">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="E433" t="inlineStr">
         <is>
@@ -11178,21 +11178,21 @@
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>20:35:32</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="C434" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D434" t="n">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="E434" t="inlineStr">
         <is>
@@ -11203,21 +11203,21 @@
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>20:52:15</t>
         </is>
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:32</t>
         </is>
       </c>
       <c r="C435" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D435" t="n">
-        <v>97</v>
+        <v>40</v>
       </c>
       <c r="E435" t="inlineStr">
         <is>
@@ -11233,16 +11233,16 @@
       </c>
       <c r="B436" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>21:34</t>
         </is>
       </c>
       <c r="C436" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D436" t="n">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="E436" t="inlineStr">
         <is>
@@ -11253,21 +11253,21 @@
     <row r="437">
       <c r="A437" t="inlineStr">
         <is>
-          <t>20:35:32</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B437" t="inlineStr">
         <is>
-          <t>21:52</t>
+          <t>21:37</t>
         </is>
       </c>
       <c r="C437" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D437" t="n">
-        <v>77</v>
+        <v>111</v>
       </c>
       <c r="E437" t="inlineStr">
         <is>
@@ -11283,7 +11283,7 @@
       </c>
       <c r="B438" t="inlineStr">
         <is>
-          <t>22:07</t>
+          <t>21:37</t>
         </is>
       </c>
       <c r="C438" t="inlineStr">
@@ -11292,7 +11292,7 @@
         </is>
       </c>
       <c r="D438" t="n">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="E438" t="inlineStr">
         <is>
@@ -11303,21 +11303,21 @@
     <row r="439">
       <c r="A439" t="inlineStr">
         <is>
-          <t>20:35:32</t>
+          <t>20:52:15</t>
         </is>
       </c>
       <c r="B439" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>21:38</t>
         </is>
       </c>
       <c r="C439" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D439" t="n">
-        <v>93</v>
+        <v>46</v>
       </c>
       <c r="E439" t="inlineStr">
         <is>
@@ -11328,21 +11328,21 @@
     <row r="440">
       <c r="A440" t="inlineStr">
         <is>
-          <t>20:35:32</t>
+          <t>20:52:15</t>
         </is>
       </c>
       <c r="B440" t="inlineStr">
         <is>
-          <t>22:18</t>
+          <t>21:38</t>
         </is>
       </c>
       <c r="C440" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D440" t="n">
-        <v>103</v>
+        <v>46</v>
       </c>
       <c r="E440" t="inlineStr">
         <is>
@@ -11353,23 +11353,348 @@
     <row r="441">
       <c r="A441" t="inlineStr">
         <is>
+          <t>20:52:15</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D441" t="n">
+        <v>55</v>
+      </c>
+      <c r="E441" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
           <t>20:35:32</t>
         </is>
       </c>
-      <c r="B441" t="inlineStr">
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>21:52</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D442" t="n">
+        <v>77</v>
+      </c>
+      <c r="E442" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>20:35:32</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>22:07</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D443" t="n">
+        <v>92</v>
+      </c>
+      <c r="E443" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>20:35:32</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>22:08</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D444" t="n">
+        <v>93</v>
+      </c>
+      <c r="E444" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>20:52:15</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>22:08</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D445" t="n">
+        <v>76</v>
+      </c>
+      <c r="E445" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>20:35:32</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>22:18</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D446" t="n">
+        <v>103</v>
+      </c>
+      <c r="E446" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>20:52:15</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>22:18</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D447" t="n">
+        <v>86</v>
+      </c>
+      <c r="E447" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>20:52:15</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>22:21</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D448" t="n">
+        <v>89</v>
+      </c>
+      <c r="E448" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>20:52:15</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>22:21</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D449" t="n">
+        <v>89</v>
+      </c>
+      <c r="E449" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>20:35:32</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
         <is>
           <t>22:27</t>
         </is>
       </c>
-      <c r="C441" t="inlineStr">
+      <c r="C450" t="inlineStr">
         <is>
           <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
-      <c r="D441" t="n">
+      <c r="D450" t="n">
         <v>112</v>
       </c>
-      <c r="E441" t="inlineStr">
+      <c r="E450" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>20:52:15</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>22:28</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D451" t="n">
+        <v>96</v>
+      </c>
+      <c r="E451" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>20:52:15</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>22:28</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D452" t="n">
+        <v>96</v>
+      </c>
+      <c r="E452" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>20:52:15</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>22:39</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D453" t="n">
+        <v>107</v>
+      </c>
+      <c r="E453" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>20:52:15</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>22:48</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D454" t="n">
+        <v>116</v>
+      </c>
+      <c r="E454" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -11386,7 +11711,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11404,14 +11729,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:35:32</t>
+          <t>Última actualización: 20:52:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 50</t>
+          <t>Total filas: 51</t>
         </is>
       </c>
     </row>
@@ -12645,7 +12970,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>20:52:15</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -12659,7 +12984,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -12670,7 +12995,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>20:35:32</t>
+          <t>20:52:15</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -12684,9 +13009,34 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="E55" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>20:52:15</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>22:39</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>107</v>
+      </c>
+      <c r="E56" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -12703,7 +13053,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12721,14 +13071,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:35:32</t>
+          <t>Última actualización: 20:52:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 62</t>
+          <t>Total filas: 63</t>
         </is>
       </c>
     </row>
@@ -14237,7 +14587,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>20:35:32</t>
+          <t>20:52:15</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -14251,7 +14601,7 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -14262,7 +14612,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>20:35:32</t>
+          <t>20:52:15</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -14276,7 +14626,7 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -14304,6 +14654,31 @@
         <v>105</v>
       </c>
       <c r="E67" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>20:52:15</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>22:21</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>89</v>
+      </c>
+      <c r="E68" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 759
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-21.xlsx
+++ b/data/horarios-141-2026-01-21.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E454"/>
+  <dimension ref="A1:E464"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,14 +437,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:52:15</t>
+          <t>Última actualización: 22:01:34</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 449</t>
+          <t>Total filas: 459</t>
         </is>
       </c>
     </row>
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1738,7 +1738,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -2453,7 +2453,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>07:50:23</t>
+          <t>07:17:57</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>07:17:57</t>
+          <t>07:50:23</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2488,11 +2488,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2788,7 +2788,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D98" t="n">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -3128,7 +3128,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>09:28:24</t>
+          <t>08:39:38</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3138,11 +3138,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>08:39:38</t>
+          <t>09:28:24</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -4553,7 +4553,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>11:45:10</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -4563,11 +4563,11 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4578,7 +4578,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>11:45:10</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -4588,11 +4588,11 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4603,7 +4603,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>12:04:07</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -4613,11 +4613,11 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4653,7 +4653,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>12:04:07</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -4663,11 +4663,11 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>11:00:36</t>
+          <t>10:25:56</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4778,7 +4778,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>10:25:56</t>
+          <t>11:00:36</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4788,11 +4788,11 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4813,7 +4813,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D179" t="n">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -5838,7 +5838,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -5863,7 +5863,7 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D221" t="n">
@@ -6353,7 +6353,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>14:13:45</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6363,11 +6363,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6378,7 +6378,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>14:13:45</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6388,11 +6388,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6913,7 +6913,7 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D263" t="n">
@@ -6938,7 +6938,7 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D264" t="n">
@@ -7353,7 +7353,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>15:06:15</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -7363,11 +7363,11 @@
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7378,7 +7378,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>15:06:15</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
@@ -7388,11 +7388,11 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -7403,7 +7403,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -7413,11 +7413,11 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7428,7 +7428,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
@@ -7438,11 +7438,11 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7538,7 +7538,7 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D288" t="n">
@@ -7563,7 +7563,7 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D289" t="n">
@@ -7613,7 +7613,7 @@
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D291" t="n">
@@ -7638,7 +7638,7 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D292" t="n">
@@ -7663,7 +7663,7 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D293" t="n">
@@ -7978,7 +7978,7 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>16:24:39</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
@@ -7988,11 +7988,11 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -8003,7 +8003,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>16:24:39</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -8013,11 +8013,11 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8028,7 +8028,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>16:47:35</t>
+          <t>15:57:46</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -8038,11 +8038,11 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>47</v>
+        <v>97</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8078,7 +8078,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>15:57:46</t>
+          <t>16:47:35</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8088,11 +8088,11 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8238,7 +8238,7 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D316" t="n">
@@ -8263,7 +8263,7 @@
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D317" t="n">
@@ -8288,7 +8288,7 @@
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D318" t="n">
@@ -8313,7 +8313,7 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D319" t="n">
@@ -8378,7 +8378,7 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
@@ -8388,11 +8388,11 @@
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D322" t="n">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -8403,7 +8403,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -8413,11 +8413,11 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8503,7 +8503,7 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
@@ -8513,11 +8513,11 @@
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -8528,7 +8528,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -8538,11 +8538,11 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8603,7 +8603,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>17:44:08</t>
+          <t>17:03:02</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
@@ -8613,11 +8613,11 @@
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8628,7 +8628,7 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>17:03:02</t>
+          <t>17:44:08</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
@@ -8638,11 +8638,11 @@
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -8763,7 +8763,7 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D337" t="n">
@@ -8788,7 +8788,7 @@
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D338" t="n">
@@ -9478,7 +9478,7 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
@@ -9488,11 +9488,11 @@
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D366" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -9503,7 +9503,7 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
@@ -9513,11 +9513,11 @@
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D367" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -9563,7 +9563,7 @@
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D369" t="n">
@@ -9578,7 +9578,7 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>18:55:55</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B370" t="inlineStr">
@@ -9588,11 +9588,11 @@
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D370" t="n">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="E370" t="inlineStr">
         <is>
@@ -9603,7 +9603,7 @@
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>18:55:55</t>
         </is>
       </c>
       <c r="B371" t="inlineStr">
@@ -9613,11 +9613,11 @@
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D371" t="n">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="E371" t="inlineStr">
         <is>
@@ -9678,7 +9678,7 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
@@ -9688,11 +9688,11 @@
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D374" t="n">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="E374" t="inlineStr">
         <is>
@@ -9703,7 +9703,7 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B375" t="inlineStr">
@@ -9713,11 +9713,11 @@
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D375" t="n">
-        <v>86</v>
+        <v>14</v>
       </c>
       <c r="E375" t="inlineStr">
         <is>
@@ -9803,7 +9803,7 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>18:04:26</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
@@ -9813,11 +9813,11 @@
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D379" t="n">
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="E379" t="inlineStr">
         <is>
@@ -9828,7 +9828,7 @@
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>18:04:26</t>
         </is>
       </c>
       <c r="B380" t="inlineStr">
@@ -9838,11 +9838,11 @@
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D380" t="n">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="E380" t="inlineStr">
         <is>
@@ -9863,7 +9863,7 @@
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D381" t="n">
@@ -9928,7 +9928,7 @@
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>19:16:50</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B384" t="inlineStr">
@@ -9938,11 +9938,11 @@
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D384" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="E384" t="inlineStr">
         <is>
@@ -9963,7 +9963,7 @@
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D385" t="n">
@@ -9978,7 +9978,7 @@
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>19:16:50</t>
         </is>
       </c>
       <c r="B386" t="inlineStr">
@@ -9988,11 +9988,11 @@
       </c>
       <c r="C386" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D386" t="n">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="E386" t="inlineStr">
         <is>
@@ -10088,7 +10088,7 @@
       </c>
       <c r="C390" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D390" t="n">
@@ -10113,7 +10113,7 @@
       </c>
       <c r="C391" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D391" t="n">
@@ -10138,7 +10138,7 @@
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D392" t="n">
@@ -10163,7 +10163,7 @@
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D393" t="n">
@@ -10228,7 +10228,7 @@
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B396" t="inlineStr">
@@ -10238,11 +10238,11 @@
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D396" t="n">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E396" t="inlineStr">
         <is>
@@ -10253,7 +10253,7 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
@@ -10263,11 +10263,11 @@
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D397" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E397" t="inlineStr">
         <is>
@@ -10403,7 +10403,7 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>19:46:58</t>
         </is>
       </c>
       <c r="B403" t="inlineStr">
@@ -10413,11 +10413,11 @@
       </c>
       <c r="C403" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D403" t="n">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -10428,7 +10428,7 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>19:46:58</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
@@ -10438,11 +10438,11 @@
       </c>
       <c r="C404" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D404" t="n">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="E404" t="inlineStr">
         <is>
@@ -10463,7 +10463,7 @@
       </c>
       <c r="C405" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D405" t="n">
@@ -10488,7 +10488,7 @@
       </c>
       <c r="C406" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D406" t="n">
@@ -10628,7 +10628,7 @@
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>20:01:28</t>
+          <t>20:35:32</t>
         </is>
       </c>
       <c r="B412" t="inlineStr">
@@ -10638,11 +10638,11 @@
       </c>
       <c r="C412" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D412" t="n">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="E412" t="inlineStr">
         <is>
@@ -10653,7 +10653,7 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>20:35:32</t>
+          <t>20:01:28</t>
         </is>
       </c>
       <c r="B413" t="inlineStr">
@@ -10663,11 +10663,11 @@
       </c>
       <c r="C413" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D413" t="n">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -10788,7 +10788,7 @@
       </c>
       <c r="C418" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D418" t="n">
@@ -10813,7 +10813,7 @@
       </c>
       <c r="C419" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D419" t="n">
@@ -10903,7 +10903,7 @@
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t>20:52:15</t>
+          <t>20:35:32</t>
         </is>
       </c>
       <c r="B423" t="inlineStr">
@@ -10913,11 +10913,11 @@
       </c>
       <c r="C423" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D423" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E423" t="inlineStr">
         <is>
@@ -10928,7 +10928,7 @@
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t>20:35:32</t>
+          <t>20:52:15</t>
         </is>
       </c>
       <c r="B424" t="inlineStr">
@@ -10938,11 +10938,11 @@
       </c>
       <c r="C424" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D424" t="n">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="E424" t="inlineStr">
         <is>
@@ -11138,7 +11138,7 @@
       </c>
       <c r="C432" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D432" t="n">
@@ -11163,7 +11163,7 @@
       </c>
       <c r="C433" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D433" t="n">
@@ -11313,7 +11313,7 @@
       </c>
       <c r="C439" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D439" t="n">
@@ -11338,7 +11338,7 @@
       </c>
       <c r="C440" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D440" t="n">
@@ -11403,7 +11403,7 @@
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>20:35:32</t>
+          <t>22:01:34</t>
         </is>
       </c>
       <c r="B443" t="inlineStr">
@@ -11417,7 +11417,7 @@
         </is>
       </c>
       <c r="D443" t="n">
-        <v>92</v>
+        <v>6</v>
       </c>
       <c r="E443" t="inlineStr">
         <is>
@@ -11428,7 +11428,7 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>20:35:32</t>
+          <t>22:01:34</t>
         </is>
       </c>
       <c r="B444" t="inlineStr">
@@ -11442,7 +11442,7 @@
         </is>
       </c>
       <c r="D444" t="n">
-        <v>93</v>
+        <v>7</v>
       </c>
       <c r="E444" t="inlineStr">
         <is>
@@ -11478,7 +11478,7 @@
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>20:35:32</t>
+          <t>20:52:15</t>
         </is>
       </c>
       <c r="B446" t="inlineStr">
@@ -11488,11 +11488,11 @@
       </c>
       <c r="C446" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D446" t="n">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="E446" t="inlineStr">
         <is>
@@ -11503,7 +11503,7 @@
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>20:52:15</t>
+          <t>20:35:32</t>
         </is>
       </c>
       <c r="B447" t="inlineStr">
@@ -11513,11 +11513,11 @@
       </c>
       <c r="C447" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D447" t="n">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="E447" t="inlineStr">
         <is>
@@ -11528,21 +11528,21 @@
     <row r="448">
       <c r="A448" t="inlineStr">
         <is>
-          <t>20:52:15</t>
+          <t>22:01:34</t>
         </is>
       </c>
       <c r="B448" t="inlineStr">
         <is>
-          <t>22:21</t>
+          <t>22:20</t>
         </is>
       </c>
       <c r="C448" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D448" t="n">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="E448" t="inlineStr">
         <is>
@@ -11563,7 +11563,7 @@
       </c>
       <c r="C449" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D449" t="n">
@@ -11578,21 +11578,21 @@
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>20:35:32</t>
+          <t>20:52:15</t>
         </is>
       </c>
       <c r="B450" t="inlineStr">
         <is>
-          <t>22:27</t>
+          <t>22:21</t>
         </is>
       </c>
       <c r="C450" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D450" t="n">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="E450" t="inlineStr">
         <is>
@@ -11603,21 +11603,21 @@
     <row r="451">
       <c r="A451" t="inlineStr">
         <is>
-          <t>20:52:15</t>
+          <t>22:01:34</t>
         </is>
       </c>
       <c r="B451" t="inlineStr">
         <is>
-          <t>22:28</t>
+          <t>22:24</t>
         </is>
       </c>
       <c r="C451" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D451" t="n">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="E451" t="inlineStr">
         <is>
@@ -11628,21 +11628,21 @@
     <row r="452">
       <c r="A452" t="inlineStr">
         <is>
-          <t>20:52:15</t>
+          <t>22:01:34</t>
         </is>
       </c>
       <c r="B452" t="inlineStr">
         <is>
-          <t>22:28</t>
+          <t>22:26</t>
         </is>
       </c>
       <c r="C452" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D452" t="n">
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="E452" t="inlineStr">
         <is>
@@ -11653,21 +11653,21 @@
     <row r="453">
       <c r="A453" t="inlineStr">
         <is>
-          <t>20:52:15</t>
+          <t>22:01:34</t>
         </is>
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>22:39</t>
+          <t>22:27</t>
         </is>
       </c>
       <c r="C453" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D453" t="n">
-        <v>107</v>
+        <v>26</v>
       </c>
       <c r="E453" t="inlineStr">
         <is>
@@ -11678,23 +11678,273 @@
     <row r="454">
       <c r="A454" t="inlineStr">
         <is>
+          <t>22:01:34</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>22:27</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D454" t="n">
+        <v>26</v>
+      </c>
+      <c r="E454" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
           <t>20:52:15</t>
         </is>
       </c>
-      <c r="B454" t="inlineStr">
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>22:28</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D455" t="n">
+        <v>96</v>
+      </c>
+      <c r="E455" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>20:52:15</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>22:28</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D456" t="n">
+        <v>96</v>
+      </c>
+      <c r="E456" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>22:01:34</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>22:36</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D457" t="n">
+        <v>35</v>
+      </c>
+      <c r="E457" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>22:01:34</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>22:39</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D458" t="n">
+        <v>38</v>
+      </c>
+      <c r="E458" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>22:01:34</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
         <is>
           <t>22:48</t>
         </is>
       </c>
-      <c r="C454" t="inlineStr">
+      <c r="C459" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D454" t="n">
-        <v>116</v>
-      </c>
-      <c r="E454" t="inlineStr">
+      <c r="D459" t="n">
+        <v>47</v>
+      </c>
+      <c r="E459" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>22:01:34</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>23:07</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D460" t="n">
+        <v>66</v>
+      </c>
+      <c r="E460" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>22:01:34</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>23:08</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D461" t="n">
+        <v>67</v>
+      </c>
+      <c r="E461" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>22:01:34</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>23:16</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D462" t="n">
+        <v>75</v>
+      </c>
+      <c r="E462" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>22:01:34</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>23:46</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D463" t="n">
+        <v>105</v>
+      </c>
+      <c r="E463" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>22:01:34</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>23:58</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D464" t="n">
+        <v>117</v>
+      </c>
+      <c r="E464" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -11711,7 +11961,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11729,14 +11979,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:52:15</t>
+          <t>Última actualización: 22:01:34</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 51</t>
+          <t>Total filas: 52</t>
         </is>
       </c>
     </row>
@@ -13020,7 +13270,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>20:52:15</t>
+          <t>22:01:34</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -13034,9 +13284,34 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>107</v>
+        <v>38</v>
       </c>
       <c r="E56" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>22:01:34</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>23:46</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>105</v>
+      </c>
+      <c r="E57" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -13053,7 +13328,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13071,14 +13346,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:52:15</t>
+          <t>Última actualización: 22:01:34</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 63</t>
+          <t>Total filas: 65</t>
         </is>
       </c>
     </row>
@@ -14612,7 +14887,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>20:52:15</t>
+          <t>22:01:34</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -14626,7 +14901,7 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>73</v>
+        <v>4</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -14679,6 +14954,56 @@
         <v>89</v>
       </c>
       <c r="E68" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>22:01:34</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>22:28</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>27</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>22:01:34</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>23:08</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>67</v>
+      </c>
+      <c r="E70" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>